<commit_message>
Update formula for royalties in quarterly model
Do this because it was referrencing the wrong row.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Quarterly_Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Quarterly_Premier_Pricing_Model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890" activeTab="2"/>
+    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="2" r:id="rId1"/>
@@ -2220,7 +2220,7 @@
   </sheetPr>
   <dimension ref="B1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -4090,11 +4090,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4246,11 +4246,11 @@
         <v>0</v>
       </c>
       <c r="P3" s="65">
-        <f>$F3*Outputs_Internal!M$51/12</f>
+        <f>$F3*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q3" s="65">
-        <f>$F3*Outputs_Internal!N$51/12</f>
+        <f>$F3*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S3" s="65"/>
@@ -4305,11 +4305,11 @@
         <v>0</v>
       </c>
       <c r="P4" s="65">
-        <f>$F4*Outputs_Internal!M$51/12</f>
+        <f>$F4*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q4" s="65">
-        <f>$F4*Outputs_Internal!N$51/12</f>
+        <f>$F4*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
     </row>
@@ -4359,11 +4359,11 @@
         <v>0</v>
       </c>
       <c r="P5" s="65">
-        <f>$F5*Outputs_Internal!M$51/12</f>
+        <f>$F5*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q5" s="65">
-        <f>$F5*Outputs_Internal!N$51/12</f>
+        <f>$F5*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S5" s="65">
@@ -4433,11 +4433,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P6" s="65">
-        <f>$F6*Outputs_Internal!M$51/12</f>
+        <f>$F6*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q6" s="65">
-        <f>$F6*Outputs_Internal!N$51/12</f>
+        <f>$F6*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S6" s="65">
@@ -4507,11 +4507,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P7" s="65">
-        <f>$F7*Outputs_Internal!M$51/12</f>
+        <f>$F7*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q7" s="65">
-        <f>$F7*Outputs_Internal!N$51/12</f>
+        <f>$F7*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S7" s="65">
@@ -4581,11 +4581,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P8" s="65">
-        <f>$F8*Outputs_Internal!M$51/12</f>
+        <f>$F8*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q8" s="65">
-        <f>$F8*Outputs_Internal!N$51/12</f>
+        <f>$F8*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S8" s="65">
@@ -4655,11 +4655,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P9" s="65">
-        <f>$F9*Outputs_Internal!M$51/12</f>
+        <f>$F9*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q9" s="65">
-        <f>$F9*Outputs_Internal!N$51/12</f>
+        <f>$F9*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S9" s="65">
@@ -4729,11 +4729,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P10" s="65">
-        <f>$F10*Outputs_Internal!M$51/12</f>
+        <f>$F10*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q10" s="65">
-        <f>$F10*Outputs_Internal!N$51/12</f>
+        <f>$F10*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S10" s="65">
@@ -4803,11 +4803,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P11" s="65">
-        <f>$F11*Outputs_Internal!M$51/12</f>
+        <f>$F11*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q11" s="65">
-        <f>$F11*Outputs_Internal!N$51/12</f>
+        <f>$F11*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S11" s="65">
@@ -4877,11 +4877,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P12" s="65">
-        <f>$F12*Outputs_Internal!M$51/12</f>
+        <f>$F12*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q12" s="65">
-        <f>$F12*Outputs_Internal!N$51/12</f>
+        <f>$F12*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S12" s="65">
@@ -4951,11 +4951,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P13" s="65">
-        <f>$F13*Outputs_Internal!M$51/12</f>
+        <f>$F13*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q13" s="65">
-        <f>$F13*Outputs_Internal!N$51/12</f>
+        <f>$F13*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S13" s="65">
@@ -5025,11 +5025,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P14" s="65">
-        <f>$F14*Outputs_Internal!M$51/12</f>
+        <f>$F14*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q14" s="65">
-        <f>$F14*Outputs_Internal!N$51/12</f>
+        <f>$F14*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S14" s="65">
@@ -5099,11 +5099,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P15" s="65">
-        <f>$F15*Outputs_Internal!M$51/12</f>
+        <f>$F15*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q15" s="65">
-        <f>$F15*Outputs_Internal!N$51/12</f>
+        <f>$F15*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S15" s="65">
@@ -5173,11 +5173,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P16" s="65">
-        <f>$F16*Outputs_Internal!M$51/12</f>
+        <f>$F16*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q16" s="65">
-        <f>$F16*Outputs_Internal!N$51/12</f>
+        <f>$F16*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S16" s="65">
@@ -5247,11 +5247,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P17" s="65">
-        <f>$F17*Outputs_Internal!M$51/12</f>
+        <f>$F17*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q17" s="65">
-        <f>$F17*Outputs_Internal!N$51/12</f>
+        <f>$F17*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S17" s="65">
@@ -5321,11 +5321,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P18" s="65">
-        <f>$F18*Outputs_Internal!M$51/12</f>
+        <f>$F18*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q18" s="65">
-        <f>$F18*Outputs_Internal!N$51/12</f>
+        <f>$F18*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S18" s="65">
@@ -5395,11 +5395,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P19" s="65">
-        <f>$F19*Outputs_Internal!M$51/12</f>
+        <f>$F19*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q19" s="65">
-        <f>$F19*Outputs_Internal!N$51/12</f>
+        <f>$F19*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S19" s="65">
@@ -5469,11 +5469,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P20" s="65">
-        <f>$F20*Outputs_Internal!M$51/12</f>
+        <f>$F20*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q20" s="65">
-        <f>$F20*Outputs_Internal!N$51/12</f>
+        <f>$F20*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S20" s="65">
@@ -5543,11 +5543,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P21" s="65">
-        <f>$F21*Outputs_Internal!M$51/12</f>
+        <f>$F21*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q21" s="65">
-        <f>$F21*Outputs_Internal!N$51/12</f>
+        <f>$F21*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S21" s="65">
@@ -5617,11 +5617,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P22" s="65">
-        <f>$F22*Outputs_Internal!M$51/12</f>
+        <f>$F22*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q22" s="65">
-        <f>$F22*Outputs_Internal!N$51/12</f>
+        <f>$F22*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S22" s="65">
@@ -5691,11 +5691,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P23" s="65">
-        <f>$F23*Outputs_Internal!M$51/12</f>
+        <f>$F23*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q23" s="65">
-        <f>$F23*Outputs_Internal!N$51/12</f>
+        <f>$F23*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S23" s="65">
@@ -5765,11 +5765,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P24" s="65">
-        <f>$F24*Outputs_Internal!M$51/12</f>
+        <f>$F24*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q24" s="65">
-        <f>$F24*Outputs_Internal!N$51/12</f>
+        <f>$F24*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S24" s="65">
@@ -5839,11 +5839,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P25" s="65">
-        <f>$F25*Outputs_Internal!M$51/12</f>
+        <f>$F25*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q25" s="65">
-        <f>$F25*Outputs_Internal!N$51/12</f>
+        <f>$F25*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S25" s="65">
@@ -5913,11 +5913,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P26" s="65">
-        <f>$F26*Outputs_Internal!M$51/12</f>
+        <f>$F26*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q26" s="65">
-        <f>$F26*Outputs_Internal!N$51/12</f>
+        <f>$F26*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S26" s="65">
@@ -5987,11 +5987,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P27" s="65">
-        <f>$F27*Outputs_Internal!M$51/12</f>
+        <f>$F27*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q27" s="65">
-        <f>$F27*Outputs_Internal!N$51/12</f>
+        <f>$F27*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S27" s="65">
@@ -6061,11 +6061,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P28" s="65">
-        <f>$F28*Outputs_Internal!M$51/12</f>
+        <f>$F28*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q28" s="65">
-        <f>$F28*Outputs_Internal!N$51/12</f>
+        <f>$F28*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S28" s="65">
@@ -6135,11 +6135,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P29" s="65">
-        <f>$F29*Outputs_Internal!M$51/12</f>
+        <f>$F29*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q29" s="65">
-        <f>$F29*Outputs_Internal!N$51/12</f>
+        <f>$F29*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S29" s="65">
@@ -6209,11 +6209,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P30" s="65">
-        <f>$F30*Outputs_Internal!M$51/12</f>
+        <f>$F30*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q30" s="65">
-        <f>$F30*Outputs_Internal!N$51/12</f>
+        <f>$F30*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S30" s="65">
@@ -6283,11 +6283,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P31" s="65">
-        <f>$F31*Outputs_Internal!M$51/12</f>
+        <f>$F31*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q31" s="65">
-        <f>$F31*Outputs_Internal!N$51/12</f>
+        <f>$F31*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S31" s="65">
@@ -6357,11 +6357,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P32" s="65">
-        <f>$F32*Outputs_Internal!M$51/12</f>
+        <f>$F32*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q32" s="65">
-        <f>$F32*Outputs_Internal!N$51/12</f>
+        <f>$F32*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S32" s="65">
@@ -6431,11 +6431,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P33" s="65">
-        <f>$F33*Outputs_Internal!M$51/12</f>
+        <f>$F33*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q33" s="65">
-        <f>$F33*Outputs_Internal!N$51/12</f>
+        <f>$F33*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S33" s="65">
@@ -6505,11 +6505,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P34" s="65">
-        <f>$F34*Outputs_Internal!M$51/12</f>
+        <f>$F34*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q34" s="65">
-        <f>$F34*Outputs_Internal!N$51/12</f>
+        <f>$F34*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S34" s="65">
@@ -6579,11 +6579,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P35" s="65">
-        <f>$F35*Outputs_Internal!M$51/12</f>
+        <f>$F35*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q35" s="65">
-        <f>$F35*Outputs_Internal!N$51/12</f>
+        <f>$F35*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S35" s="65">
@@ -6653,11 +6653,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P36" s="65">
-        <f>$F36*Outputs_Internal!M$51/12</f>
+        <f>$F36*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q36" s="65">
-        <f>$F36*Outputs_Internal!N$51/12</f>
+        <f>$F36*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S36" s="65">
@@ -6727,11 +6727,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P37" s="65">
-        <f>$F37*Outputs_Internal!M$51/12</f>
+        <f>$F37*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q37" s="65">
-        <f>$F37*Outputs_Internal!N$51/12</f>
+        <f>$F37*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S37" s="65">
@@ -6801,11 +6801,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P38" s="65">
-        <f>$F38*Outputs_Internal!M$51/12</f>
+        <f>$F38*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q38" s="65">
-        <f>$F38*Outputs_Internal!N$51/12</f>
+        <f>$F38*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S38" s="65">
@@ -6875,11 +6875,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P39" s="65">
-        <f>$F39*Outputs_Internal!M$51/12</f>
+        <f>$F39*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q39" s="65">
-        <f>$F39*Outputs_Internal!N$51/12</f>
+        <f>$F39*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S39" s="65">
@@ -6949,11 +6949,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P40" s="65">
-        <f>$F40*Outputs_Internal!M$51/12</f>
+        <f>$F40*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q40" s="65">
-        <f>$F40*Outputs_Internal!N$51/12</f>
+        <f>$F40*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S40" s="65">
@@ -7023,11 +7023,11 @@
         <v>697.70833333333337</v>
       </c>
       <c r="P41" s="65">
-        <f>$F41*Outputs_Internal!M$51/12</f>
+        <f>$F41*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q41" s="65">
-        <f>$F41*Outputs_Internal!N$51/12</f>
+        <f>$F41*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S41" s="65">
@@ -7097,11 +7097,11 @@
         <v>0</v>
       </c>
       <c r="P42" s="65">
-        <f>$F42*Outputs_Internal!M$51/12</f>
+        <f>$F42*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q42" s="65">
-        <f>$F42*Outputs_Internal!N$51/12</f>
+        <f>$F42*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S42" s="65">
@@ -7171,11 +7171,11 @@
         <v>0</v>
       </c>
       <c r="P43" s="65">
-        <f>$F43*Outputs_Internal!M$51/12</f>
+        <f>$F43*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q43" s="65">
-        <f>$F43*Outputs_Internal!N$51/12</f>
+        <f>$F43*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S43" s="65">
@@ -7245,11 +7245,11 @@
         <v>0</v>
       </c>
       <c r="P44" s="65">
-        <f>$F44*Outputs_Internal!M$51/12</f>
+        <f>$F44*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q44" s="65">
-        <f>$F44*Outputs_Internal!N$51/12</f>
+        <f>$F44*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S44" s="65">
@@ -7319,11 +7319,11 @@
         <v>0</v>
       </c>
       <c r="P45" s="65">
-        <f>$F45*Outputs_Internal!M$51/12</f>
+        <f>$F45*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q45" s="65">
-        <f>$F45*Outputs_Internal!N$51/12</f>
+        <f>$F45*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S45" s="65">
@@ -7393,11 +7393,11 @@
         <v>0</v>
       </c>
       <c r="P46" s="65">
-        <f>$F46*Outputs_Internal!M$51/12</f>
+        <f>$F46*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q46" s="65">
-        <f>$F46*Outputs_Internal!N$51/12</f>
+        <f>$F46*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S46" s="65">
@@ -7467,11 +7467,11 @@
         <v>0</v>
       </c>
       <c r="P47" s="65">
-        <f>$F47*Outputs_Internal!M$51/12</f>
+        <f>$F47*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q47" s="65">
-        <f>$F47*Outputs_Internal!N$51/12</f>
+        <f>$F47*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S47" s="65">
@@ -7541,11 +7541,11 @@
         <v>0</v>
       </c>
       <c r="P48" s="65">
-        <f>$F48*Outputs_Internal!M$51/12</f>
+        <f>$F48*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q48" s="65">
-        <f>$F48*Outputs_Internal!N$51/12</f>
+        <f>$F48*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S48" s="65">
@@ -7615,11 +7615,11 @@
         <v>0</v>
       </c>
       <c r="P49" s="65">
-        <f>$F49*Outputs_Internal!M$51/12</f>
+        <f>$F49*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q49" s="65">
-        <f>$F49*Outputs_Internal!N$51/12</f>
+        <f>$F49*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S49" s="65">
@@ -7689,11 +7689,11 @@
         <v>0</v>
       </c>
       <c r="P50" s="65">
-        <f>$F50*Outputs_Internal!M$51/12</f>
+        <f>$F50*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q50" s="65">
-        <f>$F50*Outputs_Internal!N$51/12</f>
+        <f>$F50*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S50" s="65">
@@ -7763,11 +7763,11 @@
         <v>0</v>
       </c>
       <c r="P51" s="65">
-        <f>$F51*Outputs_Internal!M$51/12</f>
+        <f>$F51*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q51" s="65">
-        <f>$F51*Outputs_Internal!N$51/12</f>
+        <f>$F51*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S51" s="65">
@@ -7837,11 +7837,11 @@
         <v>0</v>
       </c>
       <c r="P52" s="65">
-        <f>$F52*Outputs_Internal!M$51/12</f>
+        <f>$F52*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q52" s="65">
-        <f>$F52*Outputs_Internal!N$51/12</f>
+        <f>$F52*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S52" s="65">
@@ -7911,11 +7911,11 @@
         <v>0</v>
       </c>
       <c r="P53" s="65">
-        <f>$F53*Outputs_Internal!M$51/12</f>
+        <f>$F53*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q53" s="65">
-        <f>$F53*Outputs_Internal!N$51/12</f>
+        <f>$F53*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S53" s="65">
@@ -7985,11 +7985,11 @@
         <v>0</v>
       </c>
       <c r="P54" s="65">
-        <f>$F54*Outputs_Internal!M$51/12</f>
+        <f>$F54*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q54" s="65">
-        <f>$F54*Outputs_Internal!N$51/12</f>
+        <f>$F54*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S54" s="65">
@@ -8059,11 +8059,11 @@
         <v>0</v>
       </c>
       <c r="P55" s="65">
-        <f>$F55*Outputs_Internal!M$51/12</f>
+        <f>$F55*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q55" s="65">
-        <f>$F55*Outputs_Internal!N$51/12</f>
+        <f>$F55*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S55" s="65">
@@ -8133,11 +8133,11 @@
         <v>0</v>
       </c>
       <c r="P56" s="65">
-        <f>$F56*Outputs_Internal!M$51/12</f>
+        <f>$F56*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q56" s="65">
-        <f>$F56*Outputs_Internal!N$51/12</f>
+        <f>$F56*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S56" s="65">
@@ -8207,11 +8207,11 @@
         <v>0</v>
       </c>
       <c r="P57" s="65">
-        <f>$F57*Outputs_Internal!M$51/12</f>
+        <f>$F57*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q57" s="65">
-        <f>$F57*Outputs_Internal!N$51/12</f>
+        <f>$F57*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S57" s="65">
@@ -8281,11 +8281,11 @@
         <v>0</v>
       </c>
       <c r="P58" s="65">
-        <f>$F58*Outputs_Internal!M$51/12</f>
+        <f>$F58*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q58" s="65">
-        <f>$F58*Outputs_Internal!N$51/12</f>
+        <f>$F58*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S58" s="65">
@@ -8355,11 +8355,11 @@
         <v>0</v>
       </c>
       <c r="P59" s="65">
-        <f>$F59*Outputs_Internal!M$51/12</f>
+        <f>$F59*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q59" s="65">
-        <f>$F59*Outputs_Internal!N$51/12</f>
+        <f>$F59*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S59" s="65">
@@ -8429,11 +8429,11 @@
         <v>0</v>
       </c>
       <c r="P60" s="65">
-        <f>$F60*Outputs_Internal!M$51/12</f>
+        <f>$F60*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q60" s="65">
-        <f>$F60*Outputs_Internal!N$51/12</f>
+        <f>$F60*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S60" s="65">
@@ -8503,11 +8503,11 @@
         <v>0</v>
       </c>
       <c r="P61" s="65">
-        <f>$F61*Outputs_Internal!M$51/12</f>
+        <f>$F61*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q61" s="65">
-        <f>$F61*Outputs_Internal!N$51/12</f>
+        <f>$F61*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S61" s="65">
@@ -8577,11 +8577,11 @@
         <v>0</v>
       </c>
       <c r="P62" s="65">
-        <f>$F62*Outputs_Internal!M$51/12</f>
+        <f>$F62*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q62" s="65">
-        <f>$F62*Outputs_Internal!N$51/12</f>
+        <f>$F62*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S62" s="65">
@@ -8651,11 +8651,11 @@
         <v>0</v>
       </c>
       <c r="P63" s="65">
-        <f>$F63*Outputs_Internal!M$51/12</f>
+        <f>$F63*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q63" s="65">
-        <f>$F63*Outputs_Internal!N$51/12</f>
+        <f>$F63*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S63" s="65">
@@ -8725,11 +8725,11 @@
         <v>0</v>
       </c>
       <c r="P64" s="65">
-        <f>$F64*Outputs_Internal!M$51/12</f>
+        <f>$F64*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q64" s="65">
-        <f>$F64*Outputs_Internal!N$51/12</f>
+        <f>$F64*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S64" s="65">
@@ -8799,11 +8799,11 @@
         <v>0</v>
       </c>
       <c r="P65" s="65">
-        <f>$F65*Outputs_Internal!M$51/12</f>
+        <f>$F65*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q65" s="65">
-        <f>$F65*Outputs_Internal!N$51/12</f>
+        <f>$F65*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S65" s="65">
@@ -8873,11 +8873,11 @@
         <v>0</v>
       </c>
       <c r="P66" s="65">
-        <f>$F66*Outputs_Internal!M$51/12</f>
+        <f>$F66*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q66" s="65">
-        <f>$F66*Outputs_Internal!N$51/12</f>
+        <f>$F66*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S66" s="65">
@@ -8947,11 +8947,11 @@
         <v>0</v>
       </c>
       <c r="P67" s="65">
-        <f>$F67*Outputs_Internal!M$51/12</f>
+        <f>$F67*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q67" s="65">
-        <f>$F67*Outputs_Internal!N$51/12</f>
+        <f>$F67*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S67" s="65">
@@ -9021,11 +9021,11 @@
         <v>0</v>
       </c>
       <c r="P68" s="65">
-        <f>$F68*Outputs_Internal!M$51/12</f>
+        <f>$F68*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q68" s="65">
-        <f>$F68*Outputs_Internal!N$51/12</f>
+        <f>$F68*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S68" s="65">
@@ -9095,11 +9095,11 @@
         <v>0</v>
       </c>
       <c r="P69" s="65">
-        <f>$F69*Outputs_Internal!M$51/12</f>
+        <f>$F69*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q69" s="65">
-        <f>$F69*Outputs_Internal!N$51/12</f>
+        <f>$F69*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S69" s="65">
@@ -9169,11 +9169,11 @@
         <v>0</v>
       </c>
       <c r="P70" s="65">
-        <f>$F70*Outputs_Internal!M$51/12</f>
+        <f>$F70*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q70" s="65">
-        <f>$F70*Outputs_Internal!N$51/12</f>
+        <f>$F70*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S70" s="65">
@@ -9243,11 +9243,11 @@
         <v>0</v>
       </c>
       <c r="P71" s="65">
-        <f>$F71*Outputs_Internal!M$51/12</f>
+        <f>$F71*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q71" s="65">
-        <f>$F71*Outputs_Internal!N$51/12</f>
+        <f>$F71*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S71" s="65">
@@ -9317,11 +9317,11 @@
         <v>0</v>
       </c>
       <c r="P72" s="65">
-        <f>$F72*Outputs_Internal!M$51/12</f>
+        <f>$F72*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q72" s="65">
-        <f>$F72*Outputs_Internal!N$51/12</f>
+        <f>$F72*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S72" s="65">
@@ -9391,11 +9391,11 @@
         <v>0</v>
       </c>
       <c r="P73" s="65">
-        <f>$F73*Outputs_Internal!M$51/12</f>
+        <f>$F73*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q73" s="65">
-        <f>$F73*Outputs_Internal!N$51/12</f>
+        <f>$F73*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S73" s="65">
@@ -9465,11 +9465,11 @@
         <v>0</v>
       </c>
       <c r="P74" s="65">
-        <f>$F74*Outputs_Internal!M$51/12</f>
+        <f>$F74*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q74" s="65">
-        <f>$F74*Outputs_Internal!N$51/12</f>
+        <f>$F74*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S74" s="65">
@@ -9539,11 +9539,11 @@
         <v>0</v>
       </c>
       <c r="P75" s="65">
-        <f>$F75*Outputs_Internal!M$51/12</f>
+        <f>$F75*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q75" s="65">
-        <f>$F75*Outputs_Internal!N$51/12</f>
+        <f>$F75*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S75" s="65">
@@ -9613,11 +9613,11 @@
         <v>0</v>
       </c>
       <c r="P76" s="65">
-        <f>$F76*Outputs_Internal!M$51/12</f>
+        <f>$F76*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q76" s="65">
-        <f>$F76*Outputs_Internal!N$51/12</f>
+        <f>$F76*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S76" s="65">
@@ -9687,11 +9687,11 @@
         <v>0</v>
       </c>
       <c r="P77" s="65">
-        <f>$F77*Outputs_Internal!M$51/12</f>
+        <f>$F77*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q77" s="65">
-        <f>$F77*Outputs_Internal!N$51/12</f>
+        <f>$F77*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S77" s="65">
@@ -9761,11 +9761,11 @@
         <v>0</v>
       </c>
       <c r="P78" s="65">
-        <f>$F78*Outputs_Internal!M$51/12</f>
+        <f>$F78*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q78" s="65">
-        <f>$F78*Outputs_Internal!N$51/12</f>
+        <f>$F78*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S78" s="65">
@@ -9835,11 +9835,11 @@
         <v>0</v>
       </c>
       <c r="P79" s="65">
-        <f>$F79*Outputs_Internal!M$51/12</f>
+        <f>$F79*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q79" s="65">
-        <f>$F79*Outputs_Internal!N$51/12</f>
+        <f>$F79*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S79" s="65">
@@ -9909,11 +9909,11 @@
         <v>0</v>
       </c>
       <c r="P80" s="65">
-        <f>$F80*Outputs_Internal!M$51/12</f>
+        <f>$F80*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q80" s="65">
-        <f>$F80*Outputs_Internal!N$51/12</f>
+        <f>$F80*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S80" s="65">
@@ -9983,11 +9983,11 @@
         <v>0</v>
       </c>
       <c r="P81" s="65">
-        <f>$F81*Outputs_Internal!M$51/12</f>
+        <f>$F81*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q81" s="65">
-        <f>$F81*Outputs_Internal!N$51/12</f>
+        <f>$F81*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S81" s="65">
@@ -10057,11 +10057,11 @@
         <v>0</v>
       </c>
       <c r="P82" s="65">
-        <f>$F82*Outputs_Internal!M$51/12</f>
+        <f>$F82*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q82" s="65">
-        <f>$F82*Outputs_Internal!N$51/12</f>
+        <f>$F82*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S82" s="65">
@@ -10131,11 +10131,11 @@
         <v>0</v>
       </c>
       <c r="P83" s="65">
-        <f>$F83*Outputs_Internal!M$51/12</f>
+        <f>$F83*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q83" s="65">
-        <f>$F83*Outputs_Internal!N$51/12</f>
+        <f>$F83*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S83" s="65">
@@ -10205,11 +10205,11 @@
         <v>0</v>
       </c>
       <c r="P84" s="65">
-        <f>$F84*Outputs_Internal!M$51/12</f>
+        <f>$F84*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q84" s="65">
-        <f>$F84*Outputs_Internal!N$51/12</f>
+        <f>$F84*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S84" s="65">
@@ -10279,11 +10279,11 @@
         <v>0</v>
       </c>
       <c r="P85" s="65">
-        <f>$F85*Outputs_Internal!M$51/12</f>
+        <f>$F85*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q85" s="65">
-        <f>$F85*Outputs_Internal!N$51/12</f>
+        <f>$F85*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S85" s="65">
@@ -10353,11 +10353,11 @@
         <v>0</v>
       </c>
       <c r="P86" s="65">
-        <f>$F86*Outputs_Internal!M$51/12</f>
+        <f>$F86*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q86" s="65">
-        <f>$F86*Outputs_Internal!N$51/12</f>
+        <f>$F86*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S86" s="65">
@@ -10427,11 +10427,11 @@
         <v>0</v>
       </c>
       <c r="P87" s="65">
-        <f>$F87*Outputs_Internal!M$51/12</f>
+        <f>$F87*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q87" s="65">
-        <f>$F87*Outputs_Internal!N$51/12</f>
+        <f>$F87*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S87" s="65">
@@ -10501,11 +10501,11 @@
         <v>0</v>
       </c>
       <c r="P88" s="65">
-        <f>$F88*Outputs_Internal!M$51/12</f>
+        <f>$F88*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q88" s="65">
-        <f>$F88*Outputs_Internal!N$51/12</f>
+        <f>$F88*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S88" s="65">
@@ -10575,11 +10575,11 @@
         <v>0</v>
       </c>
       <c r="P89" s="65">
-        <f>$F89*Outputs_Internal!M$51/12</f>
+        <f>$F89*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q89" s="65">
-        <f>$F89*Outputs_Internal!N$51/12</f>
+        <f>$F89*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S89" s="65">
@@ -10649,11 +10649,11 @@
         <v>0</v>
       </c>
       <c r="P90" s="65">
-        <f>$F90*Outputs_Internal!M$51/12</f>
+        <f>$F90*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q90" s="65">
-        <f>$F90*Outputs_Internal!N$51/12</f>
+        <f>$F90*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S90" s="65">
@@ -10723,11 +10723,11 @@
         <v>0</v>
       </c>
       <c r="P91" s="65">
-        <f>$F91*Outputs_Internal!M$51/12</f>
+        <f>$F91*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q91" s="65">
-        <f>$F91*Outputs_Internal!N$51/12</f>
+        <f>$F91*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S91" s="65">
@@ -10797,11 +10797,11 @@
         <v>0</v>
       </c>
       <c r="P92" s="65">
-        <f>$F92*Outputs_Internal!M$51/12</f>
+        <f>$F92*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q92" s="65">
-        <f>$F92*Outputs_Internal!N$51/12</f>
+        <f>$F92*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S92" s="65">
@@ -10871,11 +10871,11 @@
         <v>0</v>
       </c>
       <c r="P93" s="65">
-        <f>$F93*Outputs_Internal!M$51/12</f>
+        <f>$F93*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q93" s="65">
-        <f>$F93*Outputs_Internal!N$51/12</f>
+        <f>$F93*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S93" s="65">
@@ -10945,11 +10945,11 @@
         <v>0</v>
       </c>
       <c r="P94" s="65">
-        <f>$F94*Outputs_Internal!M$51/12</f>
+        <f>$F94*Outputs_Internal!M$52/12</f>
         <v>0</v>
       </c>
       <c r="Q94" s="65">
-        <f>$F94*Outputs_Internal!N$51/12</f>
+        <f>$F94*Outputs_Internal!N$52/12</f>
         <v>0</v>
       </c>
       <c r="S94" s="65">

</xml_diff>

<commit_message>
Update the collaborative discount calc
Do this to reflect how NY has been handling it
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Quarterly_Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Quarterly_Premier_Pricing_Model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890" activeTab="3"/>
+    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="2" r:id="rId1"/>
@@ -4090,11 +4090,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q24" sqref="Q24"/>
+      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11002,11 +11002,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12883,7 +12883,7 @@
         <v>104</v>
       </c>
       <c r="D92" s="2">
-        <f>IF(Inputs!$D5="Y", Prices!$I$17, 0)*D94*-1</f>
+        <f>IF(Inputs!$D5="Y", Prices!$I$17, 0)*SUM(Prices!C6, Prices!C20)*-1</f>
         <v>-3525</v>
       </c>
       <c r="E92" s="2">

</xml_diff>

<commit_message>
Update it for all columns
Do this so the formula is the same for all datafeeds
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Quarterly_Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Quarterly_Premier_Pricing_Model.xlsx
@@ -11006,7 +11006,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D92" sqref="D92"/>
+      <selection pane="bottomRight" activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12883,23 +12883,23 @@
         <v>104</v>
       </c>
       <c r="D92" s="2">
-        <f>IF(Inputs!$D5="Y", Prices!$I$17, 0)*SUM(Prices!C6, Prices!C20)*-1</f>
+        <f>IF(Inputs!D5="Y", Prices!$I$17, 0)*SUM(Prices!$C$6, Prices!$C$20)*-1</f>
         <v>-3525</v>
       </c>
       <c r="E92" s="2">
-        <f>IF(Inputs!$D5="Y", Prices!$I$17, 0)*SUM(SUM(E73:E76), E94, -1*SUM(E85:E86))*-1</f>
+        <f>IF(Inputs!E5="Y", Prices!$I$17, 0)*SUM(Prices!$C$6, Prices!$C$20)*-1</f>
         <v>0</v>
       </c>
       <c r="F92" s="2">
-        <f>IF(Inputs!$D5="Y", Prices!$I$17, 0)*SUM(SUM(F73:F76), F94, -1*SUM(F85:F86))*-1</f>
+        <f>IF(Inputs!F5="Y", Prices!$I$17, 0)*SUM(Prices!$C$6, Prices!$C$20)*-1</f>
         <v>0</v>
       </c>
       <c r="G92" s="2">
-        <f>IF(Inputs!$D5="Y", Prices!$I$17, 0)*SUM(SUM(G73:G76), G94, -1*SUM(G85:G86))*-1</f>
+        <f>IF(Inputs!G5="Y", Prices!$I$17, 0)*SUM(Prices!$C$6, Prices!$C$20)*-1</f>
         <v>0</v>
       </c>
       <c r="H92" s="2">
-        <f>IF(Inputs!$D5="Y", Prices!$I$17, 0)*SUM(SUM(H73:H76), H94, -1*SUM(H85:H86))*-1</f>
+        <f>IF(Inputs!H5="Y", Prices!$I$17, 0)*SUM(Prices!$C$6, Prices!$C$20)*-1</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add collaborative discount in for monthly
Do this because it is how NY has been billing Premier.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Quarterly_Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Quarterly_Premier_Pricing_Model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890" activeTab="4"/>
+    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="2" r:id="rId1"/>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>CCLF</t>
-  </si>
-  <si>
-    <t>Collaborative Member</t>
   </si>
   <si>
     <t>Non-CMS Files</t>
@@ -357,6 +354,9 @@
   </si>
   <si>
     <t>Other Royalties</t>
+  </si>
+  <si>
+    <t>Collaborative Member Prior to 2017-07-01</t>
   </si>
 </sst>
 </file>
@@ -1025,11 +1025,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,7 +1044,7 @@
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" s="58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="74">
         <v>43009</v>
@@ -1052,7 +1052,7 @@
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="70" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="75">
         <v>36</v>
@@ -1062,19 +1062,19 @@
       <c r="B3" s="71"/>
       <c r="C3" s="76"/>
       <c r="D3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>24</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1094,7 +1094,7 @@
     </row>
     <row r="5" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="72" t="s">
-        <v>7</v>
+        <v>107</v>
       </c>
       <c r="D5" s="56" t="s">
         <v>4</v>
@@ -1104,15 +1104,15 @@
       <c r="G5" s="56"/>
       <c r="H5" s="56"/>
       <c r="L5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="72" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="56"/>
       <c r="F6" s="56"/>
@@ -1133,10 +1133,10 @@
     </row>
     <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="56"/>
       <c r="F8" s="56"/>
@@ -1145,10 +1145,10 @@
     </row>
     <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="56"/>
       <c r="F9" s="56"/>
@@ -1157,10 +1157,10 @@
     </row>
     <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="72" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="56"/>
       <c r="F10" s="56"/>
@@ -1169,10 +1169,10 @@
     </row>
     <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="72" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="56"/>
       <c r="F11" s="56"/>
@@ -1181,10 +1181,10 @@
     </row>
     <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="72" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="56"/>
       <c r="F12" s="56"/>
@@ -1193,10 +1193,10 @@
     </row>
     <row r="13" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="72" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" s="56"/>
       <c r="F13" s="56"/>
@@ -1205,10 +1205,10 @@
     </row>
     <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="72" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D14" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="56"/>
       <c r="F14" s="56"/>
@@ -1217,10 +1217,10 @@
     </row>
     <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="56"/>
       <c r="F15" s="56"/>
@@ -1229,10 +1229,10 @@
     </row>
     <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" s="56"/>
       <c r="F16" s="56"/>
@@ -1241,10 +1241,10 @@
     </row>
     <row r="17" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="72" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17" s="56"/>
       <c r="F17" s="56"/>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="18" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="56" t="s">
         <v>4</v>
@@ -1265,10 +1265,10 @@
     </row>
     <row r="19" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="72" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19" s="56"/>
       <c r="F19" s="56"/>
@@ -1277,10 +1277,10 @@
     </row>
     <row r="20" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="72" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20" s="56"/>
       <c r="F20" s="56"/>
@@ -1289,11 +1289,11 @@
     </row>
     <row r="21" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="73" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="69"/>
       <c r="D21" s="57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E21" s="57"/>
       <c r="F21" s="57"/>
@@ -1322,7 +1322,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,19 +1340,19 @@
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
@@ -1485,7 +1485,7 @@
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C9" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="18">
         <f>SUM(Calcs!D37, Calcs!D50)</f>
@@ -1521,7 +1521,7 @@
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C10" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="18">
         <f>SUM(Calcs!D38, Calcs!D51)</f>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C11" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="18">
         <f>SUM(Calcs!D39, Calcs!D52)</f>
@@ -1592,7 +1592,7 @@
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C12" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="18">
         <f>SUM(Calcs!D40, Calcs!D53)</f>
@@ -1627,7 +1627,7 @@
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C13" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="18">
         <f>SUM(Calcs!D41, Calcs!D54)</f>
@@ -1662,7 +1662,7 @@
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C14" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D14" s="18">
         <f>SUM(Calcs!D42, Calcs!D55)</f>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C15" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="20">
         <f>SUM(Calcs!D43, Calcs!D56)</f>
@@ -1732,7 +1732,7 @@
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C16" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="20">
         <f>SUM(Calcs!D44, Calcs!D57)</f>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C17" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" s="20">
         <f>SUM(Calcs!D45, Calcs!D58)</f>
@@ -1802,12 +1802,12 @@
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="1">
         <f>SUM(Calcs!D61, Calcs!D67)</f>
@@ -1842,7 +1842,7 @@
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="1">
         <f>SUM(Calcs!D62, Calcs!D68)</f>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" s="1">
         <f>SUM(Calcs!D63, Calcs!D69)</f>
@@ -1912,7 +1912,7 @@
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23" s="1">
         <f>SUM(Calcs!D64, Calcs!D70)</f>
@@ -1947,12 +1947,12 @@
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D26" s="1">
         <f>SUM(Calcs!D85:D86)</f>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D27" s="1">
         <f>Calcs!D90</f>
@@ -2022,7 +2022,7 @@
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D28" s="1">
         <f>Calcs!D92</f>
@@ -2057,7 +2057,7 @@
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" s="7">
         <f>SUM(D7:D17, D20:D23, D26:D28)</f>
@@ -2103,7 +2103,7 @@
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -2129,7 +2129,7 @@
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D35" s="7">
         <f>(D30/12*Inputs!$C$2+D4)*$C$33</f>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.25">
@@ -2221,10 +2221,10 @@
   <dimension ref="B1:N63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F26" sqref="F26:I26"/>
+      <selection pane="bottomRight" activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2245,7 +2245,7 @@
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F1" s="51" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G1" s="51"/>
       <c r="H1" s="51"/>
@@ -2253,32 +2253,32 @@
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D2" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>63</v>
-      </c>
       <c r="H2" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="L2" s="9" t="s">
-        <v>63</v>
-      </c>
       <c r="M2" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
@@ -2288,7 +2288,7 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" s="1">
         <f>SUMIF(Inputs!$D$4:$H$4, "Y", Outputs_External!D4:'Outputs_External'!H4)</f>
@@ -2325,7 +2325,7 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" s="1">
         <f>SUMIF(Inputs!$D$4:$H$4, "N", Outputs_External!D4:'Outputs_External'!H4)</f>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
@@ -2461,7 +2461,7 @@
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C10" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="18">
         <f>SUM(Calcs!D11:H11)</f>
@@ -2500,7 +2500,7 @@
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C11" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="18">
         <f>SUM(Calcs!D12:H12)</f>
@@ -2538,7 +2538,7 @@
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C12" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="18">
         <f>SUM(Calcs!D13:H13)</f>
@@ -2576,7 +2576,7 @@
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C13" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="18">
         <f>SUM(Calcs!D14:H14)</f>
@@ -2614,7 +2614,7 @@
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C14" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="18">
         <f>SUM(Calcs!D15:H15)</f>
@@ -2651,7 +2651,7 @@
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C15" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15" s="18">
         <f>SUM(Calcs!D16:H16)</f>
@@ -2689,7 +2689,7 @@
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C16" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" s="20">
         <f>SUM(Calcs!D17:H17)</f>
@@ -2727,7 +2727,7 @@
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C17" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="20">
         <f>SUM(Calcs!D18:H18)</f>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C18" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="20">
         <f>SUM(Calcs!D19:H19)</f>
@@ -2813,7 +2813,7 @@
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G20" s="49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H20" s="10">
         <v>0.1</v>
@@ -2836,7 +2836,7 @@
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -2933,7 +2933,7 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C25" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="18">
         <f>SUM(Calcs!D24:H24)</f>
@@ -2975,7 +2975,7 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C26" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D26" s="18">
         <f>SUM(Calcs!D25:H25)</f>
@@ -3017,7 +3017,7 @@
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C27" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D27" s="18">
         <f>SUM(Calcs!D26:H26)</f>
@@ -3058,7 +3058,7 @@
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C28" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D28" s="18">
         <f>SUM(Calcs!D27:H27)</f>
@@ -3099,7 +3099,7 @@
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C29" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D29" s="18">
         <f>SUM(Calcs!D28:H28)</f>
@@ -3140,7 +3140,7 @@
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C30" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D30" s="18">
         <f>SUM(Calcs!D29:H29)</f>
@@ -3181,7 +3181,7 @@
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C31" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D31" s="20">
         <f>SUM(Calcs!D30:H30)</f>
@@ -3222,7 +3222,7 @@
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C32" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D32" s="20">
         <f>SUM(Calcs!D31:H31)</f>
@@ -3263,7 +3263,7 @@
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C33" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33" s="29">
         <f>SUM(Calcs!D32:H32)</f>
@@ -3314,7 +3314,7 @@
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -3327,7 +3327,7 @@
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C36" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D36" s="18">
         <f>SUM(Calcs!D73:H73)</f>
@@ -3365,7 +3365,7 @@
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C37" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" s="18">
         <f>SUM(Calcs!D74:H74)</f>
@@ -3403,7 +3403,7 @@
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C38" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D38" s="20">
         <f>SUM(Calcs!D75:H75)</f>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C39" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D39" s="20">
         <f>SUM(Calcs!D76:H76)</f>
@@ -3485,7 +3485,7 @@
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
@@ -3498,7 +3498,7 @@
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C42" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D42" s="29">
         <f>SUM(Calcs!D79:H79)</f>
@@ -3538,7 +3538,7 @@
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C43" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D43" s="18">
         <f>SUM(Calcs!D80:H80)</f>
@@ -3578,7 +3578,7 @@
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C44" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D44" s="20">
         <f>SUM(Calcs!D81:H81)</f>
@@ -3618,7 +3618,7 @@
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C45" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D45" s="20">
         <f>SUM(Calcs!D82:H82)</f>
@@ -3663,7 +3663,7 @@
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
@@ -3671,7 +3671,7 @@
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D48" s="1">
         <f>SUM(Outputs_External!D26:'Outputs_External'!H26)</f>
@@ -3712,7 +3712,7 @@
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D49" s="1">
         <f>SUM(Outputs_External!D27:'Outputs_External'!H27)</f>
@@ -3753,7 +3753,7 @@
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D50" s="1">
         <f>SUM(Outputs_External!D28:H28)</f>
@@ -3799,7 +3799,7 @@
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B52" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D52" s="1">
         <f>SUM(Outputs_External!D30:'Outputs_External'!H30)</f>
@@ -3824,7 +3824,7 @@
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C53" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D53" s="23">
         <f>SUM(K52:N52)</f>
@@ -3841,7 +3841,7 @@
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D55" s="1">
         <f>SUM(Outputs_Timeline!S:S)</f>
@@ -3890,7 +3890,7 @@
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B59" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C59" s="21"/>
       <c r="D59" s="21"/>
@@ -3907,7 +3907,7 @@
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B60" s="27"/>
       <c r="C60" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D60" s="23">
         <f>SUM(Calcs!D61:H61)+SUM(Calcs!D67:H67)</f>
@@ -3951,7 +3951,7 @@
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B61" s="27"/>
       <c r="C61" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D61" s="23">
         <f>SUM(Calcs!D62:H62)+SUM(Calcs!D68:H68)</f>
@@ -3995,7 +3995,7 @@
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B62" s="27"/>
       <c r="C62" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D62" s="23">
         <f>SUM(Calcs!D63:H63)+SUM(Calcs!D69:H69)</f>
@@ -4039,7 +4039,7 @@
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B63" s="27"/>
       <c r="C63" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D63" s="23">
         <f>SUM(Calcs!D64:H64)+SUM(Calcs!D70:H70)</f>
@@ -4123,20 +4123,20 @@
         <v>36</v>
       </c>
       <c r="H1" s="63" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I1" s="63"/>
       <c r="J1" s="63"/>
       <c r="K1" s="63"/>
       <c r="M1" s="63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N1" s="63"/>
       <c r="O1" s="63"/>
       <c r="P1" s="63"/>
       <c r="Q1" s="63"/>
       <c r="S1" s="63" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="T1" s="63"/>
       <c r="U1" s="63"/>
@@ -4145,60 +4145,60 @@
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" s="61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C2" s="61"/>
       <c r="D2" s="61" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E2" s="61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F2" s="61" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G2" s="61"/>
       <c r="H2" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="J2" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="64" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2" s="64" t="s">
-        <v>89</v>
-      </c>
       <c r="M2" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="N2" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="N2" s="64" t="s">
-        <v>88</v>
-      </c>
       <c r="O2" s="64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P2" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="Q2" s="64" t="s">
-        <v>107</v>
-      </c>
       <c r="S2" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="T2" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="T2" s="64" t="s">
-        <v>88</v>
-      </c>
       <c r="U2" s="64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V2" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="W2" s="64" t="s">
         <v>106</v>
-      </c>
-      <c r="W2" s="64" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
@@ -11002,7 +11002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -11020,34 +11020,34 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
       <c r="K2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="M2" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="N2" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="O2" s="21" t="s">
         <v>51</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
@@ -11089,7 +11089,7 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="5">
         <f>IF(Inputs!D4="N",MAX(Inputs!D7-25000,0),0)</f>
@@ -11121,7 +11121,7 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -11176,7 +11176,7 @@
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D9="Y",Inputs!D$19="Y"), Prices!$C10, 0)</f>
@@ -11201,7 +11201,7 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D10="Y",Inputs!D$19="Y"), Prices!$C11, 0)</f>
@@ -11226,7 +11226,7 @@
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C13" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D11="Y",Inputs!D$19="Y"), Prices!$C12, 0)</f>
@@ -11251,7 +11251,7 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C14" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D12="Y",Inputs!D$19="Y"), Prices!$C13, 0)</f>
@@ -11276,7 +11276,7 @@
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C15" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D13="Y",Inputs!D$19="Y"), Prices!$C14, 0)</f>
@@ -11301,7 +11301,7 @@
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C16" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D16" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D14="Y",Inputs!D$19="Y"), Prices!$C15, 0)</f>
@@ -11326,7 +11326,7 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C17" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" s="20">
         <f xml:space="preserve"> IF(OR(Inputs!D15="Y",Inputs!D$20="Y"), Prices!$C16, 0)</f>
@@ -11351,7 +11351,7 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C18" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="20">
         <f xml:space="preserve"> IF(OR(Inputs!D16="Y",Inputs!D$20="Y"), Prices!$C17, 0)</f>
@@ -11376,7 +11376,7 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C19" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="20">
         <f xml:space="preserve"> IF(OR(Inputs!D17="Y",Inputs!D$20="Y"), Prices!$C18, 0)</f>
@@ -11401,7 +11401,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -11451,7 +11451,7 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C24" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(OR(Inputs!D9="Y",Inputs!D$19="Y"),PRODUCT(D$6, Prices!$D10),0))</f>
@@ -11476,7 +11476,7 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C25" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(OR(Inputs!D10="Y",Inputs!D$19="Y"),PRODUCT(D$6, Prices!$D11),0))</f>
@@ -11501,7 +11501,7 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C26" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D26" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(OR(Inputs!D11="Y",Inputs!D$19="Y"),PRODUCT(D$6, Prices!$D12),0))</f>
@@ -11526,7 +11526,7 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C27" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(OR(Inputs!D12="Y",Inputs!D$19="Y"),PRODUCT(D$6, Prices!$D13),0))</f>
@@ -11551,7 +11551,7 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C28" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D28" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(OR(Inputs!D13="Y",Inputs!D$19="Y"),PRODUCT(D$6, Prices!$D14),0))</f>
@@ -11576,7 +11576,7 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C29" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D29" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(OR(Inputs!D14="Y",Inputs!D$19="Y"),PRODUCT(D$6, Prices!$D15),0))</f>
@@ -11601,7 +11601,7 @@
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C30" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D30" s="20">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(OR(Inputs!D15="Y",Inputs!D$20="Y"),PRODUCT(D$6, Prices!$D16),0))</f>
@@ -11626,7 +11626,7 @@
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C31" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D31" s="20">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(OR(Inputs!D16="Y",Inputs!D$20="Y"),PRODUCT(D$6, Prices!$D17),0))</f>
@@ -11651,7 +11651,7 @@
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C32" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32" s="29">
         <v>0</v>
@@ -11678,7 +11678,7 @@
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -11733,7 +11733,7 @@
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C37" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D37" s="18">
         <f>IF(AND(Inputs!D9="Y",Inputs!D$19="N"),Prices!$C10,0)</f>
@@ -11758,7 +11758,7 @@
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D38" s="18">
         <f>IF(AND(Inputs!D10="Y",Inputs!D$19="N"),Prices!$C11,0)</f>
@@ -11783,7 +11783,7 @@
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C39" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D39" s="18">
         <f>IF(AND(Inputs!D11="Y",Inputs!D$19="N"),Prices!$C12,0)</f>
@@ -11808,7 +11808,7 @@
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C40" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D40" s="18">
         <f>IF(AND(Inputs!D12="Y",Inputs!D$19="N"),Prices!$C13,0)</f>
@@ -11833,7 +11833,7 @@
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C41" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D41" s="18">
         <f>IF(AND(Inputs!D13="Y",Inputs!D$19="N"),Prices!$C14,0)</f>
@@ -11858,7 +11858,7 @@
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C42" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D42" s="18">
         <f>IF(AND(Inputs!D14="Y",Inputs!D$19="N"),Prices!$C15,0)</f>
@@ -11883,7 +11883,7 @@
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C43" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D43" s="20">
         <f>IF(AND(Inputs!D15="Y",Inputs!D$20="N"),Prices!$C16,0)</f>
@@ -11908,7 +11908,7 @@
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C44" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D44" s="20">
         <f>IF(AND(Inputs!D16="Y",Inputs!D$20="N"),Prices!$C17,0)</f>
@@ -11933,7 +11933,7 @@
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C45" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D45" s="20">
         <f>IF(AND(Inputs!D17="Y",Inputs!D$20="N"),Prices!$C18,0)</f>
@@ -11958,7 +11958,7 @@
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
@@ -12008,7 +12008,7 @@
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C50" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D50" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(AND(Inputs!D9="Y",Inputs!D$19="N"),PRODUCT(D$6, Prices!$D10),0))</f>
@@ -12033,7 +12033,7 @@
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C51" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D51" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(AND(Inputs!D10="Y",Inputs!D$19="N"),PRODUCT(D$6, Prices!$D11),0))</f>
@@ -12058,7 +12058,7 @@
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C52" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D52" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(AND(Inputs!D11="Y",Inputs!D$19="N"),PRODUCT(D$6, Prices!$D12),0))</f>
@@ -12083,7 +12083,7 @@
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C53" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D53" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(AND(Inputs!D12="Y",Inputs!D$19="N"),PRODUCT(D$6, Prices!$D13),0))</f>
@@ -12108,7 +12108,7 @@
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C54" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D54" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(AND(Inputs!D13="Y",Inputs!D$19="N"),PRODUCT(D$6, Prices!$D14),0))</f>
@@ -12133,7 +12133,7 @@
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C55" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D55" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(AND(Inputs!D14="Y",Inputs!D$19="N"),PRODUCT(D$6, Prices!$D15),0))</f>
@@ -12158,7 +12158,7 @@
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C56" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D56" s="20">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(AND(Inputs!D15="Y",Inputs!D$20="N"),PRODUCT(D$6, Prices!$D16),0))</f>
@@ -12183,7 +12183,7 @@
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C57" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D57" s="20">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(AND(Inputs!D16="Y",Inputs!D$20="N"),PRODUCT(D$6, Prices!$D17),0))</f>
@@ -12208,7 +12208,7 @@
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C58" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D58" s="29">
         <v>0</v>
@@ -12228,12 +12228,12 @@
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B60" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C61" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D61" s="18">
         <f>IF(Inputs!D$19 = "Y", 0, IF(Inputs!D18="Y", Prices!$C20, 0))</f>
@@ -12278,7 +12278,7 @@
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C62" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D62" s="18">
         <f>IF(Inputs!D19="Y", Prices!$C21, 0)</f>
@@ -12323,7 +12323,7 @@
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C63" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D63" s="20">
         <f>IF(Inputs!D20="Y", Prices!$C22, 0)</f>
@@ -12368,7 +12368,7 @@
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C64" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D64" s="20">
         <f>IF(Inputs!D21="Y", Prices!$C23, 0)</f>
@@ -12413,12 +12413,12 @@
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C67" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D67" s="29">
         <v>0</v>
@@ -12458,7 +12458,7 @@
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C68" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D68" s="18">
         <f>IF(Inputs!D$4="Y", 0, IF(D$6 = "", 0, IF(Inputs!D19 = "Y", D$6*Prices!$D21, 0)))</f>
@@ -12483,7 +12483,7 @@
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C69" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D69" s="20">
         <f>IF(Inputs!D$4="Y", 0, IF(D$6 = "", 0, IF(Inputs!D20 = "Y", D$6*Prices!$D22, 0)))</f>
@@ -12508,7 +12508,7 @@
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C70" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D70" s="20">
         <f>IF(Inputs!D$4="Y", 0, IF(D$6 = "", 0, IF(Inputs!D21 = "Y", D$6*Prices!$D23, 0)))</f>
@@ -12540,12 +12540,12 @@
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B72" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C73" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D73" s="18">
         <f>D61</f>
@@ -12570,7 +12570,7 @@
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C74" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D74" s="18">
         <f>IF(D62=0,0,D62-SUM(D11:D16))</f>
@@ -12595,7 +12595,7 @@
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C75" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D75" s="20">
         <f>IF(D63=0,0,D63-SUM(D17:D19))</f>
@@ -12620,7 +12620,7 @@
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C76" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D76" s="20">
         <f t="shared" ref="D76:H76" si="12">D64</f>
@@ -12645,12 +12645,12 @@
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B78" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C79" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D79" s="29">
         <v>0</v>
@@ -12690,7 +12690,7 @@
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C80" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D80" s="18">
         <f>IF(D68=0,0,D68-SUM(D24:D29))</f>
@@ -12715,7 +12715,7 @@
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C81" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D81" s="20">
         <f>IF(D69=0,0,D69-SUM(D30:D31))</f>
@@ -12740,7 +12740,7 @@
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C82" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D82" s="20">
         <f t="shared" ref="D82:H82" si="19">D70</f>
@@ -12765,12 +12765,12 @@
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D85" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$61:D$64, MATCH(2, K$61:K$64, 0)), INDEX(D$66:D$70, MATCH(2, K$61:K$64, 0)))*Prices!$I$5*-1, 0)</f>
@@ -12795,7 +12795,7 @@
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D86" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$61:D$64, MATCH(3, K$61:K$64, 0)), INDEX(D$66:D$70, MATCH(3, K$61:K$64, 0)))*Prices!$I$5*-1, 0)</f>
@@ -12820,7 +12820,7 @@
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B88" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D88" s="7">
         <f>SUM(D35:D45, D48:D58, D61:D64, D67:D70, D85:D86)</f>
@@ -12848,7 +12848,7 @@
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D90" s="1">
         <f>IF(D100=1, 0, IF(D100=2, $E$103, IF(D100=3, $E$104, IF(D100=4, $E$105, IF(D100=5, $E$106, "")))))</f>
@@ -12880,7 +12880,7 @@
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D92" s="2">
         <f>IF(Inputs!D5="Y", Prices!$I$17, 0)*SUM(Prices!$C$6, Prices!$C$20)*-1</f>
@@ -12905,7 +12905,7 @@
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D94" s="7">
         <f>SUM(D88, D90)</f>
@@ -12931,7 +12931,7 @@
     <row r="97" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B97" s="27"/>
       <c r="C97" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D97" s="21">
         <f>IFERROR(_xlfn.RANK.EQ(D88,$D$88:$H$88),5)</f>
@@ -13024,13 +13024,13 @@
     <row r="102" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B102" s="27"/>
       <c r="C102" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="103" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B103" s="27"/>
       <c r="D103" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E103" s="23">
         <f>INDEX($D$88:$H$88, 1, MATCH(2, $D$100:$H$100, 0))*Prices!$I$10*-1</f>
@@ -13040,7 +13040,7 @@
     <row r="104" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B104" s="27"/>
       <c r="D104" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E104" s="23">
         <f>INDEX($D$88:$H$88, 1, MATCH(3, $D$100:$H$100, 0))*Prices!$I$11*-1</f>
@@ -13050,7 +13050,7 @@
     <row r="105" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B105" s="27"/>
       <c r="D105" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E105" s="23">
         <f>INDEX($D$88:$H$88, 1, MATCH(4, $D$100:$H$100, 0))*Prices!$I$11*-1</f>
@@ -13060,7 +13060,7 @@
     <row r="106" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B106" s="27"/>
       <c r="D106" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E106" s="23">
         <f>INDEX($D$88:$H$88, 1, MATCH(5, $D$100:$H$100, 0))*Prices!$I$11*-1</f>
@@ -13099,12 +13099,12 @@
         <v>6</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1">
         <v>5000</v>
@@ -13114,12 +13114,12 @@
       </c>
       <c r="E3" s="1"/>
       <c r="H3" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1">
         <v>5000</v>
@@ -13129,7 +13129,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="H4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I4" s="3">
         <v>0</v>
@@ -13137,10 +13137,10 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" s="3">
         <v>0.3</v>
@@ -13148,7 +13148,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="43">
         <v>15000</v>
@@ -13160,7 +13160,7 @@
         <v>0.27</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I6" s="3">
         <v>0.45</v>
@@ -13168,7 +13168,7 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="43">
         <v>6750</v>
@@ -13184,18 +13184,18 @@
       <c r="C8" s="44"/>
       <c r="D8" s="40"/>
       <c r="H8" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C9" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9" s="3">
         <v>0</v>
@@ -13203,7 +13203,7 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="45">
         <v>1000</v>
@@ -13212,7 +13212,7 @@
         <v>0.04</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I10" s="3">
         <v>0.45</v>
@@ -13220,7 +13220,7 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="45">
         <v>4000</v>
@@ -13229,7 +13229,7 @@
         <v>0.05</v>
       </c>
       <c r="H11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I11" s="3">
         <v>0.5</v>
@@ -13237,7 +13237,7 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="45">
         <v>2000</v>
@@ -13248,7 +13248,7 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="45">
         <v>2000</v>
@@ -13260,7 +13260,7 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="45">
         <v>6000</v>
@@ -13269,7 +13269,7 @@
         <v>0.05</v>
       </c>
       <c r="H14" s="60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I14" s="59">
         <v>1.2500000000000001E-2</v>
@@ -13277,7 +13277,7 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C15" s="45">
         <v>4000</v>
@@ -13286,7 +13286,7 @@
         <v>0.05</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I15" s="55">
         <v>43466</v>
@@ -13294,7 +13294,7 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="46">
         <v>10000</v>
@@ -13307,7 +13307,7 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="46">
         <v>5000</v>
@@ -13316,7 +13316,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I17" s="3">
         <v>0.15</v>
@@ -13324,7 +13324,7 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="46">
         <v>5000</v>
@@ -13333,7 +13333,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I18" s="55">
         <v>44197</v>
@@ -13345,7 +13345,7 @@
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="45">
         <v>8500</v>
@@ -13356,7 +13356,7 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="45">
         <v>33000</v>
@@ -13367,7 +13367,7 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="46">
         <v>35000</v>
@@ -13378,7 +13378,7 @@
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="46">
         <v>28000</v>

</xml_diff>

<commit_message>
Tweak pricing for PCP Dashboard
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Quarterly_Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Quarterly_Premier_Pricing_Model.xlsx
@@ -1176,7 +1176,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,7 +1291,7 @@
         <v>116</v>
       </c>
       <c r="D8" s="55" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="E8" s="55" t="s">
         <v>39</v>
@@ -1305,7 +1305,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="55" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="E9" s="55" t="s">
         <v>39</v>
@@ -1319,7 +1319,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="55" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="E10" s="55" t="s">
         <v>39</v>
@@ -1445,7 +1445,7 @@
         <v>15</v>
       </c>
       <c r="D19" s="55" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="E19" s="55" t="s">
         <v>39</v>
@@ -1476,7 +1476,7 @@
         <v>3</v>
       </c>
       <c r="E21" s="55" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="F21" s="55"/>
       <c r="G21" s="55"/>
@@ -1490,7 +1490,7 @@
         <v>3</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="F22" s="55"/>
       <c r="G22" s="55"/>
@@ -1502,10 +1502,10 @@
       </c>
       <c r="C23" s="93"/>
       <c r="D23" s="94" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="E23" s="94" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="F23" s="94"/>
       <c r="G23" s="94"/>
@@ -2024,7 +2024,7 @@
       </c>
       <c r="D20" s="1">
         <f>SUM(Calcs!D63, Calcs!D72)</f>
-        <v>33000</v>
+        <v>0</v>
       </c>
       <c r="E20" s="1">
         <f>SUM(Calcs!E63, Calcs!E72)</f>
@@ -2098,7 +2098,7 @@
       </c>
       <c r="E22" s="1">
         <f>SUM(Calcs!E65, Calcs!E74)</f>
-        <v>44380</v>
+        <v>0</v>
       </c>
       <c r="F22" s="1">
         <f>SUM(Calcs!F65, Calcs!F74)</f>
@@ -2129,11 +2129,11 @@
       </c>
       <c r="D23" s="1">
         <f>SUM(Calcs!D66, Calcs!D75)</f>
-        <v>28000</v>
+        <v>23520</v>
       </c>
       <c r="E23" s="1">
         <f>SUM(Calcs!E66, Calcs!E75)</f>
-        <v>44380</v>
+        <v>0</v>
       </c>
       <c r="F23" s="1">
         <f>SUM(Calcs!F66, Calcs!F75)</f>
@@ -2164,11 +2164,11 @@
       </c>
       <c r="D24" s="1">
         <f>SUM(Calcs!D67, Calcs!D76)</f>
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="E24" s="1">
         <f>SUM(Calcs!E67, Calcs!E76)</f>
-        <v>32740</v>
+        <v>0</v>
       </c>
       <c r="F24" s="1">
         <f>SUM(Calcs!F67, Calcs!F76)</f>
@@ -2199,7 +2199,7 @@
       </c>
       <c r="D25" s="1">
         <f>SUM(Calcs!D68, Calcs!D77)</f>
-        <v>6750</v>
+        <v>0</v>
       </c>
       <c r="E25" s="1">
         <f>SUM(Calcs!E68, Calcs!E77)</f>
@@ -2239,11 +2239,11 @@
       </c>
       <c r="D28" s="1">
         <f>SUM(Calcs!D98:D102)</f>
-        <v>-33037.5</v>
+        <v>-7056</v>
       </c>
       <c r="E28" s="1">
         <f>SUM(Calcs!E98:E102)</f>
-        <v>-28047</v>
+        <v>0</v>
       </c>
       <c r="F28" s="1">
         <f>SUM(Calcs!F98:F102)</f>
@@ -2274,11 +2274,11 @@
       </c>
       <c r="D29" s="1">
         <f>Calcs!D106</f>
-        <v>-43970.625</v>
+        <v>0</v>
       </c>
       <c r="E29" s="1">
         <f>Calcs!E106</f>
-        <v>0</v>
+        <v>-24556.5</v>
       </c>
       <c r="F29" s="1">
         <f>Calcs!F106</f>
@@ -2340,11 +2340,11 @@
       </c>
       <c r="D32" s="7">
         <f>SUM(D7:D16, D19:D25, D28:D30)</f>
-        <v>53741.875</v>
+        <v>59464</v>
       </c>
       <c r="E32" s="7">
         <f>SUM(E7:E16, E19:E25, E28:E29)</f>
-        <v>148023</v>
+        <v>30013.5</v>
       </c>
       <c r="F32" s="7">
         <f>SUM(F7:F16, F19:F25, F28:F29)</f>
@@ -2412,11 +2412,11 @@
       </c>
       <c r="D37" s="7">
         <f>(D32/12*Inputs!$C$2+D4)*$C$35</f>
-        <v>171225.625</v>
+        <v>188392</v>
       </c>
       <c r="E37" s="7">
         <f>(E32/12*Inputs!$C$2+E4)*$C$35</f>
-        <v>476819</v>
+        <v>122790.5</v>
       </c>
       <c r="F37" s="7">
         <f>(F32/12*Inputs!$C$2+F4)*$C$35</f>
@@ -2461,13 +2461,13 @@
     <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C41" s="7">
         <f>SUM(Outputs_Timeline!S:S)</f>
-        <v>648044.625</v>
+        <v>311182.5</v>
       </c>
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C42" s="52">
         <f>SUM(D37:H37)</f>
-        <v>648044.625</v>
+        <v>311182.5</v>
       </c>
       <c r="D42" s="1"/>
       <c r="G42" s="1"/>
@@ -2710,7 +2710,7 @@
       </c>
       <c r="D9" s="18">
         <f>SUM(Calcs!D15:H15)</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="32">
@@ -2728,11 +2728,11 @@
       </c>
       <c r="K9" s="18">
         <f t="shared" ref="K9:K17" si="3">F9*$D9</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="L9" s="18">
         <f t="shared" ref="L9:L16" si="4">G9*$D9</f>
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="M9" s="18">
         <f t="shared" si="2"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D10" s="18">
         <f>SUM(Calcs!D16:H16)</f>
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="74">
@@ -2766,11 +2766,11 @@
       </c>
       <c r="K10" s="18">
         <f t="shared" si="3"/>
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="L10" s="18">
         <f t="shared" si="4"/>
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="M10" s="18">
         <f t="shared" si="2"/>
@@ -2778,7 +2778,7 @@
       </c>
       <c r="N10" s="18">
         <f t="shared" si="2"/>
-        <v>400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
@@ -2787,7 +2787,7 @@
       </c>
       <c r="D11" s="18">
         <f>SUM(Calcs!D17:H17)</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="F11" s="32">
         <v>0.9</v>
@@ -2804,11 +2804,11 @@
       </c>
       <c r="K11" s="18">
         <f t="shared" si="3"/>
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="L11" s="18">
         <f t="shared" si="4"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="M11" s="18">
         <f t="shared" si="2"/>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="D12" s="18">
         <f>SUM(Calcs!D18:H18)</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="F12" s="32">
         <v>0.1</v>
@@ -2842,11 +2842,11 @@
       </c>
       <c r="K12" s="18">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="L12" s="18">
         <f t="shared" si="4"/>
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="M12" s="18">
         <f t="shared" si="2"/>
@@ -2863,7 +2863,7 @@
       </c>
       <c r="D13" s="18">
         <f>SUM(Calcs!D19:H19)</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="F13" s="32">
         <v>0.1</v>
@@ -2879,15 +2879,15 @@
       </c>
       <c r="K13" s="18">
         <f t="shared" si="3"/>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="L13" s="18">
         <f t="shared" si="4"/>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="M13" s="18">
         <f t="shared" si="2"/>
-        <v>4800</v>
+        <v>0</v>
       </c>
       <c r="N13" s="18">
         <f>I13*$D13</f>
@@ -2900,7 +2900,7 @@
       </c>
       <c r="D14" s="18">
         <f>SUM(Calcs!D20:H20)</f>
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="F14" s="74">
         <v>0.6</v>
@@ -2917,11 +2917,11 @@
       </c>
       <c r="K14" s="18">
         <f t="shared" si="3"/>
-        <v>2400</v>
+        <v>0</v>
       </c>
       <c r="L14" s="18">
         <f t="shared" si="4"/>
-        <v>1600</v>
+        <v>0</v>
       </c>
       <c r="M14" s="18">
         <f t="shared" si="2"/>
@@ -3566,7 +3566,7 @@
       </c>
       <c r="D35" s="18">
         <f>SUM(Calcs!D81:H81)</f>
-        <v>14000</v>
+        <v>0</v>
       </c>
       <c r="F35" s="32">
         <v>0.9</v>
@@ -3583,11 +3583,11 @@
       </c>
       <c r="K35" s="18">
         <f t="shared" si="12"/>
-        <v>12600</v>
+        <v>0</v>
       </c>
       <c r="L35" s="18">
         <f t="shared" si="12"/>
-        <v>1400</v>
+        <v>0</v>
       </c>
       <c r="M35" s="18">
         <f t="shared" si="12"/>
@@ -3642,7 +3642,7 @@
       </c>
       <c r="D37" s="20">
         <f>SUM(Calcs!D83:H83)</f>
-        <v>56000</v>
+        <v>28000</v>
       </c>
       <c r="F37" s="33">
         <v>0.1</v>
@@ -3659,11 +3659,11 @@
       </c>
       <c r="K37" s="20">
         <f t="shared" ref="K37" si="15">F37*$D37</f>
-        <v>5600</v>
+        <v>2800</v>
       </c>
       <c r="L37" s="20">
         <f t="shared" ref="L37" si="16">G37*$D37</f>
-        <v>50400</v>
+        <v>25200</v>
       </c>
       <c r="M37" s="20">
         <f t="shared" ref="M37" si="17">H37*$D37</f>
@@ -3680,7 +3680,7 @@
       </c>
       <c r="D38" s="20">
         <f>SUM(Calcs!D84:H84)</f>
-        <v>56000</v>
+        <v>23520</v>
       </c>
       <c r="F38" s="33">
         <v>0.1</v>
@@ -3697,11 +3697,11 @@
       </c>
       <c r="K38" s="20">
         <f t="shared" ref="K38:K39" si="20">F38*$D38</f>
-        <v>5600</v>
+        <v>2352</v>
       </c>
       <c r="L38" s="20">
         <f t="shared" ref="L38:L39" si="21">G38*$D38</f>
-        <v>50400</v>
+        <v>21168</v>
       </c>
       <c r="M38" s="20">
         <f t="shared" ref="M38:M39" si="22">H38*$D38</f>
@@ -3718,7 +3718,7 @@
       </c>
       <c r="D39" s="20">
         <f>SUM(Calcs!D85:H85)</f>
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="F39" s="33">
         <v>0.1</v>
@@ -3735,11 +3735,11 @@
       </c>
       <c r="K39" s="20">
         <f t="shared" si="20"/>
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="L39" s="20">
         <f t="shared" si="21"/>
-        <v>36000</v>
+        <v>0</v>
       </c>
       <c r="M39" s="20">
         <f t="shared" si="22"/>
@@ -3756,7 +3756,7 @@
       </c>
       <c r="D40" s="84">
         <f>SUM(Calcs!D86:H86)</f>
-        <v>6750</v>
+        <v>0</v>
       </c>
       <c r="F40" s="85">
         <v>0.2</v>
@@ -3773,11 +3773,11 @@
       </c>
       <c r="K40" s="84">
         <f t="shared" si="12"/>
-        <v>1350</v>
+        <v>0</v>
       </c>
       <c r="L40" s="84">
         <f t="shared" si="12"/>
-        <v>5400</v>
+        <v>0</v>
       </c>
       <c r="M40" s="84">
         <f t="shared" si="12"/>
@@ -3931,7 +3931,7 @@
       </c>
       <c r="D46" s="20">
         <f>SUM(Calcs!D92:H92)</f>
-        <v>16380</v>
+        <v>0</v>
       </c>
       <c r="F46" s="31">
         <f>IFERROR((1-G46)*F37/SUM(F37,H37),0)</f>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="L46" s="20">
         <f t="shared" si="24"/>
-        <v>16380</v>
+        <v>0</v>
       </c>
       <c r="M46" s="20">
         <f t="shared" si="25"/>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="D47" s="20">
         <f>SUM(Calcs!D93:H93)</f>
-        <v>16380</v>
+        <v>0</v>
       </c>
       <c r="F47" s="31">
         <f t="shared" ref="F47:F48" si="27">IFERROR((1-G47)*F38/SUM(F38,H38),0)</f>
@@ -3994,7 +3994,7 @@
       </c>
       <c r="L47" s="20">
         <f t="shared" ref="L47:L48" si="31">G47*$D47</f>
-        <v>16380</v>
+        <v>0</v>
       </c>
       <c r="M47" s="20">
         <f t="shared" ref="M47:M48" si="32">H47*$D47</f>
@@ -4011,7 +4011,7 @@
       </c>
       <c r="D48" s="20">
         <f>SUM(Calcs!D94:H94)</f>
-        <v>12740.000000000002</v>
+        <v>0</v>
       </c>
       <c r="F48" s="31">
         <f t="shared" si="27"/>
@@ -4034,7 +4034,7 @@
       </c>
       <c r="L48" s="20">
         <f t="shared" si="31"/>
-        <v>12740.000000000002</v>
+        <v>0</v>
       </c>
       <c r="M48" s="20">
         <f t="shared" si="32"/>
@@ -4104,39 +4104,39 @@
       </c>
       <c r="D52" s="1">
         <f>SUM(Outputs_External!D28:'Outputs_External'!H28)</f>
-        <v>-61084.5</v>
+        <v>-7056</v>
       </c>
       <c r="F52" s="8">
         <f>IFERROR(SUM(K64:K70)/SUM($K$64:$N$70), 0)</f>
-        <v>0.15194942044257112</v>
+        <v>0.1</v>
       </c>
       <c r="G52" s="8">
         <f t="shared" ref="G52:I52" si="41">IFERROR(SUM(L64:L70)/SUM($K$64:$N$70), 0)</f>
-        <v>0.8261327713382508</v>
+        <v>0.9</v>
       </c>
       <c r="H52" s="8">
         <f t="shared" si="41"/>
-        <v>2.0231822971548998E-2</v>
+        <v>0</v>
       </c>
       <c r="I52" s="8">
         <f t="shared" si="41"/>
-        <v>1.6859852476290833E-3</v>
+        <v>0</v>
       </c>
       <c r="K52" s="12">
         <f>F52*$D$52</f>
-        <v>-9281.754373024236</v>
+        <v>-705.6</v>
       </c>
       <c r="L52" s="12">
         <f>G52*$D$52</f>
-        <v>-50463.907270811382</v>
+        <v>-6350.4000000000005</v>
       </c>
       <c r="M52" s="12">
         <f>H52*$D$52</f>
-        <v>-1235.8507903055847</v>
+        <v>0</v>
       </c>
       <c r="N52" s="12">
         <f>I52*$D$52</f>
-        <v>-102.98756585879875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
@@ -4145,39 +4145,39 @@
       </c>
       <c r="D53" s="1">
         <f>SUM(Outputs_External!D29:'Outputs_External'!H29)</f>
-        <v>-43970.625</v>
+        <v>-24556.5</v>
       </c>
       <c r="F53" s="3">
         <f>IFERROR(SUM(K8:K52)/SUM($K8:$N52), 0)</f>
-        <v>0.21217628558745383</v>
+        <v>0.26147815563779225</v>
       </c>
       <c r="G53" s="3">
         <f>IFERROR(SUM(L8:L52)/SUM($K8:$N52), 0)</f>
-        <v>0.77211104105507178</v>
+        <v>0.7385218443622078</v>
       </c>
       <c r="H53" s="3">
         <f>IFERROR(SUM(M8:M52)/SUM($K8:$N52), 0)</f>
-        <v>1.4504006176130086E-2</v>
+        <v>0</v>
       </c>
       <c r="I53" s="3">
         <f>1-F53-G53-H53</f>
-        <v>1.2086671813443077E-3</v>
+        <v>-1.1102230246251565E-16</v>
       </c>
       <c r="K53" s="12">
         <f>F53*$D$53</f>
-        <v>-9329.5238874588376</v>
+        <v>-6420.9883289194458</v>
       </c>
       <c r="L53" s="12">
         <f>G53*$D$53</f>
-        <v>-33950.205044592163</v>
+        <v>-18135.511671080556</v>
       </c>
       <c r="M53" s="12">
         <f>H53*$D$53</f>
-        <v>-637.75021656829995</v>
+        <v>0</v>
       </c>
       <c r="N53" s="12">
         <f>I53*$D$53</f>
-        <v>-53.14585138069755</v>
+        <v>2.7263191704207657E-12</v>
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.25">
@@ -4229,23 +4229,23 @@
       </c>
       <c r="D56" s="1">
         <f>SUM(Outputs_External!D32:'Outputs_External'!H32)</f>
-        <v>201764.875</v>
+        <v>89477.5</v>
       </c>
       <c r="K56" s="12">
         <f>SUM(K52:K54, K34:K40, K8:K17,K22:K31,K43:K49)</f>
-        <v>42809.721739516928</v>
+        <v>23396.411671080554</v>
       </c>
       <c r="L56" s="12">
         <f t="shared" ref="L56:N56" si="43">SUM(L52:L54, L34:L40, L8:L17,L22:L31,L43:L49)</f>
-        <v>155784.88768459647</v>
+        <v>66081.088328919446</v>
       </c>
       <c r="M56" s="12">
         <f t="shared" si="43"/>
-        <v>2926.3989931261153</v>
+        <v>0</v>
       </c>
       <c r="N56" s="12">
         <f t="shared" si="43"/>
-        <v>243.86658276050372</v>
+        <v>2.7263191704207657E-12</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
@@ -4254,7 +4254,7 @@
       </c>
       <c r="D57" s="23">
         <f>SUM(K56:N56)</f>
-        <v>201764.87500000003</v>
+        <v>89477.5</v>
       </c>
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
@@ -4271,42 +4271,42 @@
       </c>
       <c r="D59" s="1">
         <f>SUM(Outputs_Timeline!S:S)</f>
-        <v>648044.625</v>
+        <v>311182.5</v>
       </c>
       <c r="K59" s="12">
         <f>SUM(Outputs_Timeline!T:T)</f>
-        <v>136704.1652185508</v>
+        <v>78464.23501324169</v>
       </c>
       <c r="L59" s="12">
         <f>SUM(Outputs_Timeline!U:U)</f>
-        <v>501829.66305378941</v>
+        <v>232718.26498675838</v>
       </c>
       <c r="M59" s="12">
         <f>SUM(Outputs_Timeline!V:V)</f>
-        <v>8779.1969793783483</v>
+        <v>0</v>
       </c>
       <c r="N59" s="12">
         <f>SUM(Outputs_Timeline!W:W)</f>
-        <v>731.5997482815111</v>
+        <v>8.178957511262297E-12</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D60" s="1"/>
       <c r="K60" s="53">
         <f>IFERROR(K59/$D$59, 0)</f>
-        <v>0.21094869079201267</v>
+        <v>0.25214861058459809</v>
       </c>
       <c r="L60" s="53">
         <f>IFERROR(L59/$D$59, 0)</f>
-        <v>0.77437516444764809</v>
+        <v>0.74785138941540219</v>
       </c>
       <c r="M60" s="53">
         <f>IFERROR(M59/$D$59, 0)</f>
-        <v>1.3547210548005622E-2</v>
+        <v>0</v>
       </c>
       <c r="N60" s="53">
         <f>IFERROR(N59/$D$59, 0)</f>
-        <v>1.1289342123337743E-3</v>
+        <v>2.6283475167344877E-17</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
@@ -4381,41 +4381,41 @@
       </c>
       <c r="D65" s="23">
         <f>SUM(Calcs!D63:H63)+SUM(Calcs!D72:H72)</f>
-        <v>33000</v>
+        <v>0</v>
       </c>
       <c r="E65" s="21"/>
       <c r="F65" s="24">
         <f>IFERROR(SUM(K$35,K$9:K$14,K$44,K$23:K$28)/SUM($K$35:$N$35,$K$9:$N$14,$K$44:$N$44,$K$23:$N$28),0)</f>
-        <v>0.59090909090909094</v>
+        <v>0</v>
       </c>
       <c r="G65" s="24">
         <f t="shared" ref="G65" si="45">IFERROR(SUM(L$35,L$9:L$14,L$44,L$23:L$28)/SUM($K$35:$N$35,$K$9:$N$14,$K$44:$N$44,$K$23:$N$28),0)</f>
-        <v>0.25151515151515152</v>
+        <v>0</v>
       </c>
       <c r="H65" s="24">
         <f>IFERROR(SUM(M$35,M$9:M$14,M$44,M$23:M$28)/SUM($K$35:$N$35,$K$9:$N$14,$K$44:$N$44,$K$23:$N$28),0)</f>
-        <v>0.14545454545454545</v>
+        <v>0</v>
       </c>
       <c r="I65" s="24">
         <f>IFERROR(SUM(N$35,N$9:N$14,N$44,N$23:N$28)/SUM($K$35:$N$35,$K$9:$N$14,$K$44:$N$44,$K$23:$N$28),0)</f>
-        <v>1.2121212121212121E-2</v>
+        <v>0</v>
       </c>
       <c r="J65" s="21"/>
       <c r="K65" s="25">
         <f t="shared" si="44"/>
-        <v>19500</v>
+        <v>0</v>
       </c>
       <c r="L65" s="25">
         <f t="shared" si="44"/>
-        <v>8300</v>
+        <v>0</v>
       </c>
       <c r="M65" s="25">
         <f t="shared" si="44"/>
-        <v>4800</v>
+        <v>0</v>
       </c>
       <c r="N65" s="25">
         <f t="shared" si="44"/>
-        <v>400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.25">
@@ -4469,16 +4469,16 @@
       </c>
       <c r="D67" s="23">
         <f>SUM(Calcs!D65:H65)+SUM(Calcs!D74:H74)</f>
-        <v>72380</v>
+        <v>28000</v>
       </c>
       <c r="E67" s="21"/>
       <c r="F67" s="24">
         <f>IFERROR(SUM(K37,K46)/SUM($K37:$N37,$K46:$N46),0)</f>
-        <v>7.7369439071566737E-2</v>
+        <v>0.1</v>
       </c>
       <c r="G67" s="24">
         <f t="shared" ref="G67:I67" si="47">IFERROR(SUM(L37,L46)/SUM($K37:$N37,$K46:$N46),0)</f>
-        <v>0.92263056092843332</v>
+        <v>0.9</v>
       </c>
       <c r="H67" s="24">
         <f t="shared" si="47"/>
@@ -4491,11 +4491,11 @@
       <c r="J67" s="21"/>
       <c r="K67" s="25">
         <f t="shared" ref="K67:K70" si="48">F67*$D67</f>
-        <v>5600</v>
+        <v>2800</v>
       </c>
       <c r="L67" s="25">
         <f t="shared" ref="L67:L70" si="49">G67*$D67</f>
-        <v>66780</v>
+        <v>25200</v>
       </c>
       <c r="M67" s="25">
         <f t="shared" ref="M67:M70" si="50">H67*$D67</f>
@@ -4513,16 +4513,16 @@
       </c>
       <c r="D68" s="23">
         <f>SUM(Calcs!D66:H66)+SUM(Calcs!D75:H75)</f>
-        <v>72380</v>
+        <v>23520</v>
       </c>
       <c r="E68" s="21"/>
       <c r="F68" s="24">
         <f t="shared" ref="F68:F69" si="52">IFERROR(SUM(K38,K47)/SUM($K38:$N38,$K47:$N47),0)</f>
-        <v>7.7369439071566737E-2</v>
+        <v>0.1</v>
       </c>
       <c r="G68" s="24">
         <f t="shared" ref="G68:G69" si="53">IFERROR(SUM(L38,L47)/SUM($K38:$N38,$K47:$N47),0)</f>
-        <v>0.92263056092843332</v>
+        <v>0.9</v>
       </c>
       <c r="H68" s="24">
         <f t="shared" ref="H68:H69" si="54">IFERROR(SUM(M38,M47)/SUM($K38:$N38,$K47:$N47),0)</f>
@@ -4535,11 +4535,11 @@
       <c r="J68" s="21"/>
       <c r="K68" s="25">
         <f t="shared" ref="K68:K69" si="56">F68*$D68</f>
-        <v>5600</v>
+        <v>2352</v>
       </c>
       <c r="L68" s="25">
         <f t="shared" ref="L68:L69" si="57">G68*$D68</f>
-        <v>66780</v>
+        <v>21168</v>
       </c>
       <c r="M68" s="25">
         <f t="shared" ref="M68:M69" si="58">H68*$D68</f>
@@ -4557,16 +4557,16 @@
       </c>
       <c r="D69" s="23">
         <f>SUM(Calcs!D67:H67)+SUM(Calcs!D76:H76)</f>
-        <v>52740</v>
+        <v>0</v>
       </c>
       <c r="E69" s="21"/>
       <c r="F69" s="24">
         <f t="shared" si="52"/>
-        <v>7.584376185058779E-2</v>
+        <v>0</v>
       </c>
       <c r="G69" s="24">
         <f t="shared" si="53"/>
-        <v>0.92415623814941217</v>
+        <v>0</v>
       </c>
       <c r="H69" s="24">
         <f t="shared" si="54"/>
@@ -4579,11 +4579,11 @@
       <c r="J69" s="21"/>
       <c r="K69" s="25">
         <f t="shared" si="56"/>
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="L69" s="25">
         <f t="shared" si="57"/>
-        <v>48740</v>
+        <v>0</v>
       </c>
       <c r="M69" s="25">
         <f t="shared" si="58"/>
@@ -4601,16 +4601,16 @@
       </c>
       <c r="D70" s="23">
         <f>SUM(Calcs!D68:H68)+SUM(Calcs!D77:H77)</f>
-        <v>6750</v>
+        <v>0</v>
       </c>
       <c r="E70" s="21"/>
       <c r="F70" s="24">
         <f t="shared" ref="F70" si="60">IFERROR(SUM(K40,K49)/SUM($K40:$N40,$K49:$N49),0)</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G70" s="24">
         <f t="shared" ref="G70" si="61">IFERROR(SUM(L40,L49)/SUM($K40:$N40,$K49:$N49),0)</f>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="H70" s="24">
         <f t="shared" ref="H70" si="62">IFERROR(SUM(M40,M49)/SUM($K40:$N40,$K49:$N49),0)</f>
@@ -4623,11 +4623,11 @@
       <c r="J70" s="21"/>
       <c r="K70" s="25">
         <f t="shared" si="48"/>
-        <v>1350</v>
+        <v>0</v>
       </c>
       <c r="L70" s="25">
         <f t="shared" si="49"/>
-        <v>5400</v>
+        <v>0</v>
       </c>
       <c r="M70" s="25">
         <f t="shared" si="50"/>
@@ -5199,23 +5199,23 @@
       </c>
       <c r="M9" s="63">
         <f>$F9*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N9" s="63">
         <f>$F9*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O9" s="63">
         <f>$F9*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P9" s="63">
         <f>$F9*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="63">
         <f>$F9*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S9" s="63">
         <f t="shared" si="1"/>
@@ -5273,23 +5273,23 @@
       </c>
       <c r="M10" s="63">
         <f>$F10*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N10" s="63">
         <f>$F10*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O10" s="63">
         <f>$F10*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P10" s="63">
         <f>$F10*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="63">
         <f>$F10*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S10" s="63">
         <f t="shared" si="1"/>
@@ -5347,43 +5347,43 @@
       </c>
       <c r="M11" s="63">
         <f>$F11*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N11" s="63">
         <f>$F11*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O11" s="63">
         <f>$F11*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P11" s="63">
         <f>$F11*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="63">
         <f>$F11*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S11" s="63">
         <f t="shared" si="1"/>
-        <v>93191.218749999985</v>
+        <v>65119.375000000007</v>
       </c>
       <c r="T11" s="63">
         <f t="shared" si="2"/>
-        <v>18977.430434879232</v>
+        <v>14124.102917770138</v>
       </c>
       <c r="U11" s="63">
         <f>IF(MOD(MONTH($B11),3)=0,SUM(J9:J11,O9:O11),0)</f>
-        <v>73421.221921149117</v>
+        <v>50995.272082229858</v>
       </c>
       <c r="V11" s="63">
         <f t="shared" si="4"/>
-        <v>731.59974828152883</v>
+        <v>0</v>
       </c>
       <c r="W11" s="63">
         <f t="shared" si="5"/>
-        <v>60.966645690125929</v>
+        <v>6.8157979260519141E-13</v>
       </c>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
@@ -5421,23 +5421,23 @@
       </c>
       <c r="M12" s="63">
         <f>$F12*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N12" s="63">
         <f>$F12*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O12" s="63">
         <f>$F12*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P12" s="63">
         <f>$F12*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="63">
         <f>$F12*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S12" s="63">
         <f t="shared" si="1"/>
@@ -5495,23 +5495,23 @@
       </c>
       <c r="M13" s="63">
         <f>$F13*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N13" s="63">
         <f>$F13*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O13" s="63">
         <f>$F13*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P13" s="63">
         <f>$F13*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="63">
         <f>$F13*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S13" s="63">
         <f t="shared" si="1"/>
@@ -5569,43 +5569,43 @@
       </c>
       <c r="M14" s="63">
         <f>$F14*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N14" s="63">
         <f>$F14*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O14" s="63">
         <f>$F14*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P14" s="63">
         <f>$F14*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="63">
         <f>$F14*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S14" s="63">
         <f t="shared" si="1"/>
-        <v>50441.21875</v>
+        <v>22369.375</v>
       </c>
       <c r="T14" s="63">
         <f t="shared" si="2"/>
-        <v>10702.430434879232</v>
+        <v>5849.1029177701384</v>
       </c>
       <c r="U14" s="63">
         <f t="shared" si="3"/>
-        <v>38946.221921149117</v>
+        <v>16520.272082229862</v>
       </c>
       <c r="V14" s="63">
         <f t="shared" si="4"/>
-        <v>731.59974828152883</v>
+        <v>0</v>
       </c>
       <c r="W14" s="63">
         <f t="shared" si="5"/>
-        <v>60.966645690125929</v>
+        <v>6.8157979260519141E-13</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
@@ -5643,23 +5643,23 @@
       </c>
       <c r="M15" s="63">
         <f>$F15*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N15" s="63">
         <f>$F15*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O15" s="63">
         <f>$F15*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P15" s="63">
         <f>$F15*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="63">
         <f>$F15*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S15" s="63">
         <f t="shared" si="1"/>
@@ -5717,23 +5717,23 @@
       </c>
       <c r="M16" s="63">
         <f>$F16*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N16" s="63">
         <f>$F16*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O16" s="63">
         <f>$F16*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P16" s="63">
         <f>$F16*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="63">
         <f>$F16*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S16" s="63">
         <f t="shared" si="1"/>
@@ -5791,43 +5791,43 @@
       </c>
       <c r="M17" s="63">
         <f>$F17*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N17" s="63">
         <f>$F17*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O17" s="63">
         <f>$F17*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P17" s="63">
         <f>$F17*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="63">
         <f>$F17*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S17" s="63">
         <f t="shared" si="1"/>
-        <v>50441.21875</v>
+        <v>22369.375</v>
       </c>
       <c r="T17" s="63">
         <f t="shared" si="2"/>
-        <v>10702.430434879232</v>
+        <v>5849.1029177701384</v>
       </c>
       <c r="U17" s="63">
         <f t="shared" si="3"/>
-        <v>38946.221921149117</v>
+        <v>16520.272082229862</v>
       </c>
       <c r="V17" s="63">
         <f t="shared" si="4"/>
-        <v>731.59974828152883</v>
+        <v>0</v>
       </c>
       <c r="W17" s="63">
         <f t="shared" si="5"/>
-        <v>60.966645690125929</v>
+        <v>6.8157979260519141E-13</v>
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
@@ -5865,23 +5865,23 @@
       </c>
       <c r="M18" s="63">
         <f>$F18*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N18" s="63">
         <f>$F18*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O18" s="63">
         <f>$F18*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P18" s="63">
         <f>$F18*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="63">
         <f>$F18*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S18" s="63">
         <f t="shared" si="1"/>
@@ -5939,23 +5939,23 @@
       </c>
       <c r="M19" s="63">
         <f>$F19*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N19" s="63">
         <f>$F19*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O19" s="63">
         <f>$F19*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P19" s="63">
         <f>$F19*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="63">
         <f>$F19*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S19" s="63">
         <f t="shared" si="1"/>
@@ -6013,43 +6013,43 @@
       </c>
       <c r="M20" s="63">
         <f>$F20*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N20" s="63">
         <f>$F20*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O20" s="63">
         <f>$F20*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P20" s="63">
         <f>$F20*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="63">
         <f>$F20*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S20" s="63">
         <f t="shared" si="1"/>
-        <v>50441.21875</v>
+        <v>22369.375</v>
       </c>
       <c r="T20" s="63">
         <f t="shared" si="2"/>
-        <v>10702.430434879232</v>
+        <v>5849.1029177701384</v>
       </c>
       <c r="U20" s="63">
         <f t="shared" si="3"/>
-        <v>38946.221921149117</v>
+        <v>16520.272082229862</v>
       </c>
       <c r="V20" s="63">
         <f t="shared" si="4"/>
-        <v>731.59974828152883</v>
+        <v>0</v>
       </c>
       <c r="W20" s="63">
         <f t="shared" si="5"/>
-        <v>60.966645690125929</v>
+        <v>6.8157979260519141E-13</v>
       </c>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.25">
@@ -6087,23 +6087,23 @@
       </c>
       <c r="M21" s="63">
         <f>$F21*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N21" s="63">
         <f>$F21*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O21" s="63">
         <f>$F21*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P21" s="63">
         <f>$F21*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="63">
         <f>$F21*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S21" s="63">
         <f t="shared" si="1"/>
@@ -6161,23 +6161,23 @@
       </c>
       <c r="M22" s="63">
         <f>$F22*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N22" s="63">
         <f>$F22*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O22" s="63">
         <f>$F22*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P22" s="63">
         <f>$F22*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="63">
         <f>$F22*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S22" s="63">
         <f t="shared" si="1"/>
@@ -6235,43 +6235,43 @@
       </c>
       <c r="M23" s="63">
         <f>$F23*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N23" s="63">
         <f>$F23*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O23" s="63">
         <f>$F23*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P23" s="63">
         <f>$F23*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="63">
         <f>$F23*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S23" s="63">
         <f t="shared" si="1"/>
-        <v>50441.21875</v>
+        <v>22369.375</v>
       </c>
       <c r="T23" s="63">
         <f t="shared" si="2"/>
-        <v>10702.430434879232</v>
+        <v>5849.1029177701384</v>
       </c>
       <c r="U23" s="63">
         <f t="shared" si="3"/>
-        <v>38946.221921149117</v>
+        <v>16520.272082229862</v>
       </c>
       <c r="V23" s="63">
         <f t="shared" si="4"/>
-        <v>731.59974828152883</v>
+        <v>0</v>
       </c>
       <c r="W23" s="63">
         <f t="shared" si="5"/>
-        <v>60.966645690125929</v>
+        <v>6.8157979260519141E-13</v>
       </c>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.25">
@@ -6309,23 +6309,23 @@
       </c>
       <c r="M24" s="63">
         <f>$F24*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N24" s="63">
         <f>$F24*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O24" s="63">
         <f>$F24*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P24" s="63">
         <f>$F24*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="63">
         <f>$F24*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S24" s="63">
         <f t="shared" si="1"/>
@@ -6383,23 +6383,23 @@
       </c>
       <c r="M25" s="63">
         <f>$F25*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N25" s="63">
         <f>$F25*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O25" s="63">
         <f>$F25*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P25" s="63">
         <f>$F25*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="63">
         <f>$F25*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S25" s="63">
         <f t="shared" si="1"/>
@@ -6457,43 +6457,43 @@
       </c>
       <c r="M26" s="63">
         <f>$F26*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N26" s="63">
         <f>$F26*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O26" s="63">
         <f>$F26*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P26" s="63">
         <f>$F26*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="63">
         <f>$F26*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S26" s="63">
         <f t="shared" si="1"/>
-        <v>50441.21875</v>
+        <v>22369.375</v>
       </c>
       <c r="T26" s="63">
         <f t="shared" si="2"/>
-        <v>10702.430434879232</v>
+        <v>5849.1029177701384</v>
       </c>
       <c r="U26" s="63">
         <f t="shared" si="3"/>
-        <v>38946.221921149117</v>
+        <v>16520.272082229862</v>
       </c>
       <c r="V26" s="63">
         <f t="shared" si="4"/>
-        <v>731.59974828152883</v>
+        <v>0</v>
       </c>
       <c r="W26" s="63">
         <f t="shared" si="5"/>
-        <v>60.966645690125929</v>
+        <v>6.8157979260519141E-13</v>
       </c>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.25">
@@ -6531,23 +6531,23 @@
       </c>
       <c r="M27" s="63">
         <f>$F27*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N27" s="63">
         <f>$F27*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O27" s="63">
         <f>$F27*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P27" s="63">
         <f>$F27*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="63">
         <f>$F27*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S27" s="63">
         <f t="shared" si="1"/>
@@ -6605,23 +6605,23 @@
       </c>
       <c r="M28" s="63">
         <f>$F28*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N28" s="63">
         <f>$F28*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O28" s="63">
         <f>$F28*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P28" s="63">
         <f>$F28*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q28" s="63">
         <f>$F28*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S28" s="63">
         <f t="shared" si="1"/>
@@ -6679,43 +6679,43 @@
       </c>
       <c r="M29" s="63">
         <f>$F29*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N29" s="63">
         <f>$F29*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O29" s="63">
         <f>$F29*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P29" s="63">
         <f>$F29*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q29" s="63">
         <f>$F29*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S29" s="63">
         <f t="shared" si="1"/>
-        <v>50441.21875</v>
+        <v>22369.375</v>
       </c>
       <c r="T29" s="63">
         <f t="shared" si="2"/>
-        <v>10702.430434879232</v>
+        <v>5849.1029177701384</v>
       </c>
       <c r="U29" s="63">
         <f t="shared" si="3"/>
-        <v>38946.221921149117</v>
+        <v>16520.272082229862</v>
       </c>
       <c r="V29" s="63">
         <f t="shared" si="4"/>
-        <v>731.59974828152883</v>
+        <v>0</v>
       </c>
       <c r="W29" s="63">
         <f t="shared" si="5"/>
-        <v>60.966645690125929</v>
+        <v>6.8157979260519141E-13</v>
       </c>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.25">
@@ -6753,23 +6753,23 @@
       </c>
       <c r="M30" s="63">
         <f>$F30*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N30" s="63">
         <f>$F30*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O30" s="63">
         <f>$F30*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P30" s="63">
         <f>$F30*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="63">
         <f>$F30*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S30" s="63">
         <f t="shared" si="1"/>
@@ -6827,23 +6827,23 @@
       </c>
       <c r="M31" s="63">
         <f>$F31*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N31" s="63">
         <f>$F31*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O31" s="63">
         <f>$F31*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P31" s="63">
         <f>$F31*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="63">
         <f>$F31*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S31" s="63">
         <f t="shared" si="1"/>
@@ -6901,43 +6901,43 @@
       </c>
       <c r="M32" s="63">
         <f>$F32*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N32" s="63">
         <f>$F32*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O32" s="63">
         <f>$F32*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P32" s="63">
         <f>$F32*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q32" s="63">
         <f>$F32*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S32" s="63">
         <f t="shared" si="1"/>
-        <v>50441.21875</v>
+        <v>22369.375</v>
       </c>
       <c r="T32" s="63">
         <f t="shared" si="2"/>
-        <v>10702.430434879232</v>
+        <v>5849.1029177701384</v>
       </c>
       <c r="U32" s="63">
         <f t="shared" si="3"/>
-        <v>38946.221921149117</v>
+        <v>16520.272082229862</v>
       </c>
       <c r="V32" s="63">
         <f t="shared" si="4"/>
-        <v>731.59974828152883</v>
+        <v>0</v>
       </c>
       <c r="W32" s="63">
         <f t="shared" si="5"/>
-        <v>60.966645690125929</v>
+        <v>6.8157979260519141E-13</v>
       </c>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.25">
@@ -6975,23 +6975,23 @@
       </c>
       <c r="M33" s="63">
         <f>$F33*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N33" s="63">
         <f>$F33*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O33" s="63">
         <f>$F33*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P33" s="63">
         <f>$F33*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="63">
         <f>$F33*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S33" s="63">
         <f t="shared" si="1"/>
@@ -7049,23 +7049,23 @@
       </c>
       <c r="M34" s="63">
         <f>$F34*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N34" s="63">
         <f>$F34*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O34" s="63">
         <f>$F34*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P34" s="63">
         <f>$F34*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="63">
         <f>$F34*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S34" s="63">
         <f t="shared" si="1"/>
@@ -7123,43 +7123,43 @@
       </c>
       <c r="M35" s="63">
         <f>$F35*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N35" s="63">
         <f>$F35*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O35" s="63">
         <f>$F35*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P35" s="63">
         <f>$F35*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="63">
         <f>$F35*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S35" s="63">
         <f t="shared" si="1"/>
-        <v>50441.21875</v>
+        <v>22369.375</v>
       </c>
       <c r="T35" s="63">
         <f t="shared" si="2"/>
-        <v>10702.430434879232</v>
+        <v>5849.1029177701384</v>
       </c>
       <c r="U35" s="63">
         <f t="shared" si="3"/>
-        <v>38946.221921149117</v>
+        <v>16520.272082229862</v>
       </c>
       <c r="V35" s="63">
         <f t="shared" si="4"/>
-        <v>731.59974828152883</v>
+        <v>0</v>
       </c>
       <c r="W35" s="63">
         <f t="shared" si="5"/>
-        <v>60.966645690125929</v>
+        <v>6.8157979260519141E-13</v>
       </c>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.25">
@@ -7197,23 +7197,23 @@
       </c>
       <c r="M36" s="63">
         <f>$F36*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N36" s="63">
         <f>$F36*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O36" s="63">
         <f>$F36*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P36" s="63">
         <f>$F36*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="63">
         <f>$F36*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S36" s="63">
         <f t="shared" si="1"/>
@@ -7271,23 +7271,23 @@
       </c>
       <c r="M37" s="63">
         <f>$F37*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N37" s="63">
         <f>$F37*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O37" s="63">
         <f>$F37*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P37" s="63">
         <f>$F37*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="63">
         <f>$F37*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S37" s="63">
         <f t="shared" si="1"/>
@@ -7345,43 +7345,43 @@
       </c>
       <c r="M38" s="63">
         <f>$F38*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N38" s="63">
         <f>$F38*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O38" s="63">
         <f>$F38*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P38" s="63">
         <f>$F38*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q38" s="63">
         <f>$F38*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S38" s="63">
         <f t="shared" si="1"/>
-        <v>50441.21875</v>
+        <v>22369.375</v>
       </c>
       <c r="T38" s="63">
         <f t="shared" si="2"/>
-        <v>10702.430434879232</v>
+        <v>5849.1029177701384</v>
       </c>
       <c r="U38" s="63">
         <f t="shared" si="3"/>
-        <v>38946.221921149117</v>
+        <v>16520.272082229862</v>
       </c>
       <c r="V38" s="63">
         <f t="shared" si="4"/>
-        <v>731.59974828152883</v>
+        <v>0</v>
       </c>
       <c r="W38" s="63">
         <f t="shared" si="5"/>
-        <v>60.966645690125929</v>
+        <v>6.8157979260519141E-13</v>
       </c>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.25">
@@ -7419,23 +7419,23 @@
       </c>
       <c r="M39" s="63">
         <f>$F39*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N39" s="63">
         <f>$F39*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O39" s="63">
         <f>$F39*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P39" s="63">
         <f>$F39*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q39" s="63">
         <f>$F39*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S39" s="63">
         <f t="shared" si="1"/>
@@ -7493,23 +7493,23 @@
       </c>
       <c r="M40" s="63">
         <f>$F40*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N40" s="63">
         <f>$F40*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O40" s="63">
         <f>$F40*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P40" s="63">
         <f>$F40*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q40" s="63">
         <f>$F40*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S40" s="63">
         <f t="shared" si="1"/>
@@ -7567,43 +7567,43 @@
       </c>
       <c r="M41" s="63">
         <f>$F41*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N41" s="63">
         <f>$F41*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O41" s="63">
         <f>$F41*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P41" s="63">
         <f>$F41*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q41" s="63">
         <f>$F41*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S41" s="63">
         <f t="shared" si="1"/>
-        <v>50441.21875</v>
+        <v>22369.375</v>
       </c>
       <c r="T41" s="63">
         <f t="shared" si="2"/>
-        <v>10702.430434879232</v>
+        <v>5849.1029177701384</v>
       </c>
       <c r="U41" s="63">
         <f t="shared" si="3"/>
-        <v>38946.221921149117</v>
+        <v>16520.272082229862</v>
       </c>
       <c r="V41" s="63">
         <f t="shared" si="4"/>
-        <v>731.59974828152883</v>
+        <v>0</v>
       </c>
       <c r="W41" s="63">
         <f t="shared" si="5"/>
-        <v>60.966645690125929</v>
+        <v>6.8157979260519141E-13</v>
       </c>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.25">
@@ -7641,23 +7641,23 @@
       </c>
       <c r="M42" s="63">
         <f>$F42*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N42" s="63">
         <f>$F42*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O42" s="63">
         <f>$F42*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P42" s="63">
         <f>$F42*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q42" s="63">
         <f>$F42*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S42" s="63">
         <f t="shared" si="1"/>
@@ -7715,23 +7715,23 @@
       </c>
       <c r="M43" s="63">
         <f>$F43*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N43" s="63">
         <f>$F43*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O43" s="63">
         <f>$F43*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P43" s="63">
         <f>$F43*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q43" s="63">
         <f>$F43*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S43" s="63">
         <f t="shared" si="1"/>
@@ -7789,43 +7789,43 @@
       </c>
       <c r="M44" s="63">
         <f>$F44*Outputs_Internal!$D$56/12</f>
-        <v>16813.739583333332</v>
+        <v>7456.458333333333</v>
       </c>
       <c r="N44" s="63">
         <f>$F44*Outputs_Internal!K$56/12</f>
-        <v>3567.4768116264108</v>
+        <v>1949.7009725900461</v>
       </c>
       <c r="O44" s="63">
         <f>$F44*Outputs_Internal!L$56/12</f>
-        <v>12982.073973716373</v>
+        <v>5506.7573607432869</v>
       </c>
       <c r="P44" s="63">
         <f>$F44*Outputs_Internal!M$56/12</f>
-        <v>243.8665827605096</v>
+        <v>0</v>
       </c>
       <c r="Q44" s="63">
         <f>$F44*Outputs_Internal!N$56/12</f>
-        <v>20.322215230041976</v>
+        <v>2.2719326420173047E-13</v>
       </c>
       <c r="S44" s="63">
         <f>IF(MOD(MONTH($B44),3)=0,SUM(H42:H44,M42:M44),0)</f>
-        <v>50441.21875</v>
+        <v>22369.375</v>
       </c>
       <c r="T44" s="63">
         <f t="shared" si="2"/>
-        <v>10702.430434879232</v>
+        <v>5849.1029177701384</v>
       </c>
       <c r="U44" s="63">
         <f t="shared" si="3"/>
-        <v>38946.221921149117</v>
+        <v>16520.272082229862</v>
       </c>
       <c r="V44" s="63">
         <f t="shared" si="4"/>
-        <v>731.59974828152883</v>
+        <v>0</v>
       </c>
       <c r="W44" s="63">
         <f t="shared" si="5"/>
-        <v>60.966645690125929</v>
+        <v>6.8157979260519141E-13</v>
       </c>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.25">
@@ -11546,7 +11546,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M91" sqref="M91"/>
+      <selection pane="bottomRight" activeCell="K96" sqref="K96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11868,7 +11868,7 @@
       </c>
       <c r="D15" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D9="Y",Inputs!D$19="Y"), Prices!$C10, 0)</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E15" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!E9="Y",Inputs!E$19="Y"), Prices!$C10, 0)</f>
@@ -11893,7 +11893,7 @@
       </c>
       <c r="D16" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D10="Y",Inputs!D$19="Y"), Prices!$C11, 0)</f>
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="E16" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!E10="Y",Inputs!E$19="Y"), Prices!$C11, 0)</f>
@@ -11918,7 +11918,7 @@
       </c>
       <c r="D17" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D11="Y",Inputs!D$19="Y"), Prices!$C12, 0)</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="E17" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!E11="Y",Inputs!E$19="Y"), Prices!$C12, 0)</f>
@@ -11943,7 +11943,7 @@
       </c>
       <c r="D18" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D12="Y",Inputs!D$19="Y"), Prices!$C13, 0)</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="E18" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!E12="Y",Inputs!E$19="Y"), Prices!$C13, 0)</f>
@@ -11968,7 +11968,7 @@
       </c>
       <c r="D19" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D13="Y",Inputs!D$19="Y"), Prices!$C14, 0)</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="E19" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!E13="Y",Inputs!E$19="Y"), Prices!$C14, 0)</f>
@@ -11993,7 +11993,7 @@
       </c>
       <c r="D20" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D14="Y",Inputs!D$19="Y"), Prices!$C15, 0)</f>
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="E20" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!E14="Y",Inputs!E$19="Y"), Prices!$C15, 0)</f>
@@ -12885,7 +12885,7 @@
       </c>
       <c r="D63" s="18">
         <f>IF(Inputs!D19="Y", Prices!$C21, 0)</f>
-        <v>33000</v>
+        <v>0</v>
       </c>
       <c r="E63" s="18">
         <f>IF(Inputs!E19="Y", Prices!$C21, 0)</f>
@@ -12939,7 +12939,7 @@
       </c>
       <c r="E65" s="20">
         <f>IF(Inputs!E21="Y", Prices!$C23, 0)</f>
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="F65" s="20">
         <f>IF(Inputs!F21="Y", Prices!$C23, 0)</f>
@@ -12960,11 +12960,11 @@
       </c>
       <c r="D66" s="20">
         <f>IF(Inputs!D22="Y", Prices!$C24 * IF(Inputs!D21="Y",1-Prices!$L$20,1), 0)</f>
-        <v>28000</v>
+        <v>23520</v>
       </c>
       <c r="E66" s="20">
         <f>IF(Inputs!E22="Y", Prices!$C24 * IF(Inputs!E21="Y",1-Prices!$L$20,1), 0)</f>
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="F66" s="20">
         <f>IF(Inputs!F22="Y", Prices!$C24 * IF(Inputs!F21="Y",1-Prices!$L$20,1), 0)</f>
@@ -12985,11 +12985,11 @@
       </c>
       <c r="D67" s="20">
         <f>IF(Inputs!D23="Y", Prices!$C25, 0)</f>
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="E67" s="20">
         <f>IF(Inputs!E23="Y", Prices!$C25, 0)</f>
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="F67" s="20">
         <f>IF(Inputs!F23="Y", Prices!$C25, 0)</f>
@@ -13010,7 +13010,7 @@
       </c>
       <c r="D68" s="84">
         <f>IF(Inputs!D8="Y", Prices!$C26, 0)</f>
-        <v>6750</v>
+        <v>0</v>
       </c>
       <c r="E68" s="84">
         <f>IF(Inputs!E8="Y", Prices!$C26, 0)</f>
@@ -13110,7 +13110,7 @@
       </c>
       <c r="K72" s="23">
         <f t="shared" ref="K72:O72" si="3">D63+D72+$J72</f>
-        <v>33000.001100000001</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="L72" s="23">
         <f t="shared" si="3"/>
@@ -13188,7 +13188,7 @@
       </c>
       <c r="E74" s="20">
         <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E21 = "Y", E$11*Prices!$E23, 0)))*E$10</f>
-        <v>16380</v>
+        <v>0</v>
       </c>
       <c r="F74" s="20">
         <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F21 = "Y", F$11*Prices!$E23, 0)))*F$10</f>
@@ -13212,7 +13212,7 @@
       </c>
       <c r="L74" s="23">
         <f t="shared" si="6"/>
-        <v>44380.001300000004</v>
+        <v>1.3000000000000002E-3</v>
       </c>
       <c r="M74" s="23">
         <f t="shared" si="6"/>
@@ -13237,7 +13237,7 @@
       </c>
       <c r="E75" s="20">
         <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E22 = "Y", E$11*Prices!$E24 * IF(Inputs!E21="Y",1-Prices!$L$20,1), 0)))*E$10</f>
-        <v>16380</v>
+        <v>0</v>
       </c>
       <c r="F75" s="20">
         <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F22 = "Y", F$11*Prices!$E24 * IF(Inputs!F21="Y",1-Prices!$L$20,1), 0)))*F$10</f>
@@ -13257,11 +13257,11 @@
       </c>
       <c r="K75" s="23">
         <f t="shared" ref="K75:O75" si="7">D66+D75+$J75</f>
-        <v>28000.001400000001</v>
+        <v>23520.001400000001</v>
       </c>
       <c r="L75" s="23">
         <f t="shared" si="7"/>
-        <v>44380.001400000001</v>
+        <v>1.4000000000000002E-3</v>
       </c>
       <c r="M75" s="23">
         <f t="shared" si="7"/>
@@ -13286,7 +13286,7 @@
       </c>
       <c r="E76" s="20">
         <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E23 = "Y", E$11*Prices!$E25, 0)))*E$10</f>
-        <v>12740.000000000002</v>
+        <v>0</v>
       </c>
       <c r="F76" s="20">
         <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F23 = "Y", F$11*Prices!$E25, 0)))*F$10</f>
@@ -13306,11 +13306,11 @@
       </c>
       <c r="K76" s="23">
         <f t="shared" ref="K76:O76" si="8">D67+D76+$J76</f>
-        <v>20000.001499999998</v>
+        <v>1.5000000000000002E-3</v>
       </c>
       <c r="L76" s="23">
         <f t="shared" si="8"/>
-        <v>32740.001499999998</v>
+        <v>1.5000000000000002E-3</v>
       </c>
       <c r="M76" s="23">
         <f t="shared" si="8"/>
@@ -13355,7 +13355,7 @@
       </c>
       <c r="K77" s="23">
         <f t="shared" ref="K77:O77" si="9">D68+D77+$J77</f>
-        <v>6750.0015999999996</v>
+        <v>1.6000000000000003E-3</v>
       </c>
       <c r="L77" s="23">
         <f t="shared" si="9"/>
@@ -13437,7 +13437,7 @@
       </c>
       <c r="D81" s="18">
         <f>IF(D63=0,0,D63-SUM(D15:D20))</f>
-        <v>14000</v>
+        <v>0</v>
       </c>
       <c r="E81" s="18">
         <f>IF(E63=0,0,E63-SUM(E15:E20))</f>
@@ -13457,7 +13457,7 @@
       </c>
       <c r="K81" s="21">
         <f t="shared" ref="K81:O81" si="12">IF(COUNTIF(K$71:K$77,"")&gt;2,"",IFERROR(RANK(K72,K$71:K$77),5))</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L81" s="21">
         <f t="shared" si="12"/>
@@ -13502,7 +13502,7 @@
       </c>
       <c r="K82" s="21">
         <f t="shared" ref="K82:O82" si="13">IF(COUNTIF(K$71:K$77,"")&gt;2,"",IFERROR(RANK(K73,K$71:K$77),5))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L82" s="21">
         <f t="shared" si="13"/>
@@ -13531,7 +13531,7 @@
       </c>
       <c r="E83" s="20">
         <f>E65</f>
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="F83" s="20">
         <f>F65</f>
@@ -13547,11 +13547,11 @@
       </c>
       <c r="K83" s="21">
         <f t="shared" ref="K83:O83" si="14">IF(COUNTIF(K$71:K$77,"")&gt;2,"",IFERROR(RANK(K74,K$71:K$77),5))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L83" s="21">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M83" s="21">
         <f t="shared" si="14"/>
@@ -13572,11 +13572,11 @@
       </c>
       <c r="D84" s="20">
         <f t="shared" ref="D84:H84" si="15">D66</f>
-        <v>28000</v>
+        <v>23520</v>
       </c>
       <c r="E84" s="20">
         <f t="shared" si="15"/>
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="F84" s="20">
         <f t="shared" si="15"/>
@@ -13596,7 +13596,7 @@
       </c>
       <c r="L84" s="21">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M84" s="21">
         <f t="shared" si="16"/>
@@ -13617,11 +13617,11 @@
       </c>
       <c r="D85" s="20">
         <f t="shared" ref="D85:H85" si="17">D67</f>
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="E85" s="20">
         <f t="shared" si="17"/>
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="F85" s="20">
         <f t="shared" si="17"/>
@@ -13641,7 +13641,7 @@
       </c>
       <c r="L85" s="21">
         <f t="shared" si="18"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M85" s="21">
         <f t="shared" si="18"/>
@@ -13662,7 +13662,7 @@
       </c>
       <c r="D86" s="84">
         <f t="shared" ref="D86:H86" si="19">D68</f>
-        <v>6750</v>
+        <v>0</v>
       </c>
       <c r="E86" s="84">
         <f t="shared" si="19"/>
@@ -13682,11 +13682,11 @@
       </c>
       <c r="K86" s="21">
         <f t="shared" ref="K86:O86" si="20">IF(COUNTIF(K$71:K$77,"")&gt;2,"",IFERROR(RANK(K77,K$71:K$77),5))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L86" s="21">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M86" s="21">
         <f t="shared" si="20"/>
@@ -13786,7 +13786,7 @@
       </c>
       <c r="E92" s="20">
         <f>E74</f>
-        <v>16380</v>
+        <v>0</v>
       </c>
       <c r="F92" s="20">
         <f>F74</f>
@@ -13811,7 +13811,7 @@
       </c>
       <c r="E93" s="20">
         <f t="shared" si="21"/>
-        <v>16380</v>
+        <v>0</v>
       </c>
       <c r="F93" s="20">
         <f t="shared" si="21"/>
@@ -13836,7 +13836,7 @@
       </c>
       <c r="E94" s="20">
         <f t="shared" si="22"/>
-        <v>12740.000000000002</v>
+        <v>0</v>
       </c>
       <c r="F94" s="20">
         <f t="shared" si="22"/>
@@ -13890,11 +13890,11 @@
       </c>
       <c r="D98" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$62:D$68, MATCH($A98, K$80:K$86, 0)), INDEX(D$71:D$77, MATCH($A98, K$80:K$86, 0)))*Prices!$L$5*-1, 0)</f>
-        <v>-8400</v>
+        <v>-7056</v>
       </c>
       <c r="E98" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(E$62:E$68, MATCH($A98, L$80:L$86, 0)), INDEX(E$71:E$77, MATCH($A98, L$80:L$86, 0)))*Prices!$L$5*-1, 0)</f>
-        <v>-13314</v>
+        <v>0</v>
       </c>
       <c r="F98" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(F$62:F$68, MATCH($A98, M$80:M$86, 0)), INDEX(F$71:F$77, MATCH($A98, M$80:M$86, 0)))*Prices!$L$5*-1, 0)</f>
@@ -13918,11 +13918,11 @@
       </c>
       <c r="D99" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$62:D$68, MATCH($A99, K$80:K$86, 0)), INDEX(D$71:D$77, MATCH($A99, K$80:K$86, 0)))*Prices!$L$6*-1, 0)</f>
-        <v>-12600</v>
+        <v>0</v>
       </c>
       <c r="E99" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(E$62:E$68, MATCH($A99, L$80:L$86, 0)), INDEX(E$71:E$77, MATCH($A99, L$80:L$86, 0)))*Prices!$L$6*-1, 0)</f>
-        <v>-14733</v>
+        <v>0</v>
       </c>
       <c r="F99" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(F$62:F$68, MATCH($A99, M$80:M$86, 0)), INDEX(F$71:F$77, MATCH($A99, M$80:M$86, 0)))*Prices!$L$6*-1, 0)</f>
@@ -13946,7 +13946,7 @@
       </c>
       <c r="D100" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$62:D$68, MATCH($A100, K$80:K$86, 0)), INDEX(D$71:D$77, MATCH($A100, K$80:K$86, 0)))*Prices!$L$6*-1, 0)</f>
-        <v>-9000</v>
+        <v>0</v>
       </c>
       <c r="E100" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(E$62:E$68, MATCH($A100, L$80:L$86, 0)), INDEX(E$71:E$77, MATCH($A100, L$80:L$86, 0)))*Prices!$L$6*-1, 0)</f>
@@ -13974,7 +13974,7 @@
       </c>
       <c r="D101" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$62:D$68, MATCH($A101, K$80:K$86, 0)), INDEX(D$71:D$77, MATCH($A101, K$80:K$86, 0)))*Prices!$L$6*-1, 0)</f>
-        <v>-3037.5</v>
+        <v>0</v>
       </c>
       <c r="E101" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(E$62:E$68, MATCH($A101, L$80:L$86, 0)), INDEX(E$71:E$77, MATCH($A101, L$80:L$86, 0)))*Prices!$L$6*-1, 0)</f>
@@ -14027,11 +14027,11 @@
       </c>
       <c r="D104" s="7">
         <f>SUM(D38:D47, D50:D59, D62:D68, D71:D77, D98:D102)</f>
-        <v>97712.5</v>
+        <v>59464</v>
       </c>
       <c r="E104" s="7">
         <f t="shared" ref="E104:H104" si="24">SUM(E38:E47, E50:E59, E62:E68, E71:E77, E98:E102)</f>
-        <v>148023</v>
+        <v>54570</v>
       </c>
       <c r="F104" s="7">
         <f t="shared" si="24"/>
@@ -14055,11 +14055,11 @@
       </c>
       <c r="D106" s="1">
         <f>IF(D116=1, 0, IF(D116=2, $E$119, IF(D116=3, $E$120, IF(D116=4, $E$121, IF(D116=5, $E$122, "")))))</f>
-        <v>-43970.625</v>
+        <v>0</v>
       </c>
       <c r="E106" s="1">
         <f t="shared" ref="E106:H106" si="25">IF(E116=1, 0, IF(E116=2, $E$119, IF(E116=3, $E$120, IF(E116=4, $E$121, IF(E116=5, $E$122, "")))))</f>
-        <v>0</v>
+        <v>-24556.5</v>
       </c>
       <c r="F106" s="1">
         <f t="shared" si="25"/>
@@ -14108,11 +14108,11 @@
       </c>
       <c r="D110" s="7">
         <f>SUM(D104, D106)</f>
-        <v>53741.875</v>
+        <v>59464</v>
       </c>
       <c r="E110" s="7">
         <f>SUM(E104, E106)</f>
-        <v>148023</v>
+        <v>30013.5</v>
       </c>
       <c r="F110" s="7">
         <f>SUM(F104, F106)</f>
@@ -14134,11 +14134,11 @@
       </c>
       <c r="D113" s="21">
         <f>IFERROR(_xlfn.RANK.EQ(D104,$D$104:$H$104),5)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E113" s="21">
         <f t="shared" ref="E113:H113" si="26">IFERROR(_xlfn.RANK.EQ(E104,$D$104:$H$104),5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F113" s="21">
         <f t="shared" si="26"/>
@@ -14175,11 +14175,11 @@
       <c r="B115" s="27"/>
       <c r="D115" s="21">
         <f>SUM(D113:D114)</f>
-        <v>2.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E115" s="21">
         <f t="shared" ref="E115:H115" si="27">SUM(E113:E114)</f>
-        <v>1.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F115" s="21">
         <f t="shared" si="27"/>
@@ -14198,11 +14198,11 @@
       <c r="B116" s="27"/>
       <c r="D116" s="21">
         <f>_xlfn.RANK.EQ(D115, $D$115:$H$115, 5)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E116" s="21">
         <f t="shared" ref="E116:H116" si="28">_xlfn.RANK.EQ(E115, $D$115:$H$115, 5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F116" s="21">
         <f t="shared" si="28"/>
@@ -14233,7 +14233,7 @@
       </c>
       <c r="E119" s="23">
         <f>INDEX($D$104:$H$104, 1, MATCH(2, $D$116:$H$116, 0))*Prices!$L$10*-1</f>
-        <v>-43970.625</v>
+        <v>-24556.5</v>
       </c>
     </row>
     <row r="120" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -14279,9 +14279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14698,7 +14696,7 @@
         <v>122</v>
       </c>
       <c r="L20" s="3">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
@@ -14775,22 +14773,22 @@
         <v>118</v>
       </c>
       <c r="C24" s="45">
-        <v>28000</v>
+        <v>33600</v>
       </c>
       <c r="E24" s="41">
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="F24" s="41">
         <f t="shared" ref="F24:H26" si="3">$E24*F$4</f>
-        <v>0.108</v>
+        <v>0.15</v>
       </c>
       <c r="G24" s="41">
         <f t="shared" si="3"/>
-        <v>4.3199999999999995E-2</v>
+        <v>0.06</v>
       </c>
       <c r="H24" s="41">
         <f t="shared" si="3"/>
-        <v>3.5999999999999997E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Change implementation to be charged per datafeed.
Do this because we switched things around to be per datafeed instead of
per population.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Quarterly_Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Quarterly_Premier_Pricing_Model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason.Altieri\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shea.parkes\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Prices" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="ACOInsight1">Inputs!$D$18:$D$19</definedName>
+    <definedName name="ACOInsight1">Inputs!$D$19:$D$20</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Outputs_Internal!$B$1:$M$60</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="125">
   <si>
     <t>One-Time Fees:</t>
   </si>
@@ -123,24 +123,6 @@
     <t>PRM Physician Risk and Credibility Adjusted Report</t>
   </si>
   <si>
-    <t>Data Feed #1</t>
-  </si>
-  <si>
-    <t>Data Feed #2</t>
-  </si>
-  <si>
-    <t>Data Feed #3</t>
-  </si>
-  <si>
-    <t>Data Feed #4</t>
-  </si>
-  <si>
-    <t>Data Feed #5</t>
-  </si>
-  <si>
-    <t>Implementation Fees</t>
-  </si>
-  <si>
     <t>Non-CCLF</t>
   </si>
   <si>
@@ -171,18 +153,6 @@
     <t>3rd Most Expensive Product</t>
   </si>
   <si>
-    <t>Most Expensive Datafeed</t>
-  </si>
-  <si>
-    <t>Multi-Datafeed Discounts</t>
-  </si>
-  <si>
-    <t>2nd Most Expensive Datafeed</t>
-  </si>
-  <si>
-    <t>3rd Most Expensive Datafeed</t>
-  </si>
-  <si>
     <t>Base</t>
   </si>
   <si>
@@ -190,9 +160,6 @@
   </si>
   <si>
     <t>Multi-Product Discount</t>
-  </si>
-  <si>
-    <t>Datafeed Total</t>
   </si>
   <si>
     <t>Product Ranking #1</t>
@@ -208,18 +175,6 @@
   </si>
   <si>
     <t>Product Ranking #5</t>
-  </si>
-  <si>
-    <t>Datafeed Discounts</t>
-  </si>
-  <si>
-    <t>4th Most Expensive Datafeed</t>
-  </si>
-  <si>
-    <t>5th Most Expensive Datafeed</t>
-  </si>
-  <si>
-    <t>Discounted Datafeed Total</t>
   </si>
   <si>
     <t>Annual Data Fees:</t>
@@ -244,9 +199,6 @@
   </si>
   <si>
     <t>Datamart Discounts</t>
-  </si>
-  <si>
-    <t>Datafeed Rank</t>
   </si>
   <si>
     <t>Totals</t>
@@ -439,6 +391,57 @@
   </si>
   <si>
     <t>Noise</t>
+  </si>
+  <si>
+    <t>Population #1</t>
+  </si>
+  <si>
+    <t>Population #2</t>
+  </si>
+  <si>
+    <t>Population #3</t>
+  </si>
+  <si>
+    <t>Population #4</t>
+  </si>
+  <si>
+    <t>Population #5</t>
+  </si>
+  <si>
+    <t>Number of Datafeeds</t>
+  </si>
+  <si>
+    <t>Implementation Fees (Per Datafeed)</t>
+  </si>
+  <si>
+    <t>Population Totoal</t>
+  </si>
+  <si>
+    <t>Discounted Population Total</t>
+  </si>
+  <si>
+    <t>Population Rank</t>
+  </si>
+  <si>
+    <t>Population Discounts</t>
+  </si>
+  <si>
+    <t>2nd Most Expensive Population</t>
+  </si>
+  <si>
+    <t>3rd Most Expensive Population</t>
+  </si>
+  <si>
+    <t>4th Most Expensive Population</t>
+  </si>
+  <si>
+    <t>5th Most Expensive Population</t>
+  </si>
+  <si>
+    <t>Most Expensive Population</t>
+  </si>
+  <si>
+    <t>Multi-Population Discounts</t>
   </si>
 </sst>
 </file>
@@ -1170,13 +1173,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L23"/>
+  <dimension ref="B1:L24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1194,7 @@
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" s="91" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C1" s="70">
         <v>43101</v>
@@ -1199,7 +1202,7 @@
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="67" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C2" s="71">
         <v>36</v>
@@ -1209,19 +1212,19 @@
       <c r="B3" s="68"/>
       <c r="C3" s="72"/>
       <c r="D3" s="13" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>19</v>
+        <v>109</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1232,7 +1235,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F4" s="55"/>
       <c r="G4" s="55"/>
@@ -1243,19 +1246,19 @@
     </row>
     <row r="5" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="69" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="D5" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E5" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="56"/>
       <c r="L5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1266,7 +1269,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
@@ -1288,13 +1291,13 @@
     </row>
     <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="69" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="55" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="55" t="s">
-        <v>39</v>
+        <v>113</v>
+      </c>
+      <c r="D8" s="55">
+        <v>1</v>
+      </c>
+      <c r="E8" s="55">
+        <v>3</v>
       </c>
       <c r="F8" s="55"/>
       <c r="G8" s="55"/>
@@ -1302,13 +1305,13 @@
     </row>
     <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="69" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="D9" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E9" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F9" s="55"/>
       <c r="G9" s="55"/>
@@ -1316,13 +1319,13 @@
     </row>
     <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="69" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E10" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F10" s="55"/>
       <c r="G10" s="55"/>
@@ -1330,13 +1333,13 @@
     </row>
     <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="69" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D11" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F11" s="55"/>
       <c r="G11" s="55"/>
@@ -1344,13 +1347,13 @@
     </row>
     <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="69" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D12" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F12" s="55"/>
       <c r="G12" s="55"/>
@@ -1358,13 +1361,13 @@
     </row>
     <row r="13" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E13" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F13" s="55"/>
       <c r="G13" s="55"/>
@@ -1372,13 +1375,13 @@
     </row>
     <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="69" t="s">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="D14" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E14" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F14" s="55"/>
       <c r="G14" s="55"/>
@@ -1386,13 +1389,13 @@
     </row>
     <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="69" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="D15" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E15" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F15" s="55"/>
       <c r="G15" s="55"/>
@@ -1400,13 +1403,13 @@
     </row>
     <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="69" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F16" s="55"/>
       <c r="G16" s="55"/>
@@ -1414,13 +1417,13 @@
     </row>
     <row r="17" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="69" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F17" s="55"/>
       <c r="G17" s="55"/>
@@ -1428,13 +1431,13 @@
     </row>
     <row r="18" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F18" s="55"/>
       <c r="G18" s="55"/>
@@ -1442,13 +1445,13 @@
     </row>
     <row r="19" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="69" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F19" s="55"/>
       <c r="G19" s="55"/>
@@ -1456,13 +1459,13 @@
     </row>
     <row r="20" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="69" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E20" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F20" s="55"/>
       <c r="G20" s="55"/>
@@ -1470,13 +1473,13 @@
     </row>
     <row r="21" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="55" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E21" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F21" s="55"/>
       <c r="G21" s="55"/>
@@ -1484,43 +1487,54 @@
     </row>
     <row r="22" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="69" t="s">
-        <v>118</v>
+        <v>17</v>
       </c>
       <c r="D22" s="55" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F22" s="55"/>
       <c r="G22" s="55"/>
       <c r="H22" s="56"/>
     </row>
     <row r="23" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="92" t="s">
-        <v>117</v>
-      </c>
-      <c r="C23" s="93"/>
-      <c r="D23" s="94" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="94" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="94"/>
-      <c r="G23" s="94"/>
-      <c r="H23" s="95"/>
+      <c r="B23" s="69" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="56"/>
+    </row>
+    <row r="24" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="92" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="93"/>
+      <c r="D24" s="94" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="94" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="94"/>
+      <c r="G24" s="94"/>
+      <c r="H24" s="95"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:G6 D8:H21 D22:D23">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:H22 D23:D24 D4:H6">
       <formula1>$L$4:$L$5</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:H7">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:H8">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H6">
-      <formula1>$L$4:$L$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1533,10 +1547,10 @@
   <dimension ref="B2:U45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,19 +1568,19 @@
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>109</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.25">
@@ -1584,7 +1598,7 @@
       </c>
       <c r="E4" s="1">
         <f>MAX(Calcs!E4, 0)</f>
-        <v>32750</v>
+        <v>60000</v>
       </c>
       <c r="F4" s="1">
         <f>MAX(Calcs!F4, 0)</f>
@@ -1622,7 +1636,7 @@
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
@@ -1663,7 +1677,7 @@
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C8" s="17" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D8" s="18">
         <f>SUM(Calcs!D39, Calcs!D51)</f>
@@ -1735,7 +1749,7 @@
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C10" s="17" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D10" s="18">
         <f>SUM(Calcs!D41, Calcs!D53)</f>
@@ -1840,7 +1854,7 @@
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C13" s="17" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D13" s="18">
         <f>SUM(Calcs!D44, Calcs!D56)</f>
@@ -1945,7 +1959,7 @@
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C16" s="19" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D16" s="20">
         <f>SUM(Calcs!D47, Calcs!D59)</f>
@@ -1980,7 +1994,7 @@
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
@@ -2125,7 +2139,7 @@
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="D23" s="1">
         <f>SUM(Calcs!D66, Calcs!D75)</f>
@@ -2160,7 +2174,7 @@
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D24" s="1">
         <f>SUM(Calcs!D67, Calcs!D76)</f>
@@ -2195,7 +2209,7 @@
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D25" s="1">
         <f>SUM(Calcs!D68, Calcs!D77)</f>
@@ -2230,12 +2244,12 @@
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D28" s="1">
         <f>SUM(Calcs!D98:D102)</f>
@@ -2270,7 +2284,7 @@
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="D29" s="1">
         <f>Calcs!D106</f>
@@ -2305,7 +2319,7 @@
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D30" s="1">
         <f>Calcs!D108</f>
@@ -2336,7 +2350,7 @@
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="D32" s="7">
         <f>SUM(D7:D16, D19:D25, D28:D30)</f>
@@ -2382,7 +2396,7 @@
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -2408,7 +2422,7 @@
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D37" s="7">
         <f>(D32/12*Inputs!$C$2+D4)*$C$35</f>
@@ -2416,7 +2430,7 @@
       </c>
       <c r="E37" s="7">
         <f>(E32/12*Inputs!$C$2+E4)*$C$35</f>
-        <v>122790.5</v>
+        <v>150040.5</v>
       </c>
       <c r="F37" s="7">
         <f>(F32/12*Inputs!$C$2+F4)*$C$35</f>
@@ -2455,19 +2469,19 @@
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C41" s="7">
         <f>SUM(Outputs_Timeline!S:S)</f>
-        <v>311182.5</v>
+        <v>338432.5</v>
       </c>
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C42" s="52">
         <f>SUM(D37:H37)</f>
-        <v>311182.5</v>
+        <v>338432.5</v>
       </c>
       <c r="D42" s="1"/>
       <c r="G42" s="1"/>
@@ -2500,10 +2514,10 @@
   <dimension ref="B1:N70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2525,7 +2539,7 @@
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F1" s="50" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="G1" s="50"/>
       <c r="H1" s="50"/>
@@ -2533,32 +2547,32 @@
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D2" s="9" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="9" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
@@ -2568,7 +2582,7 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D4" s="1">
         <f>SUMIF(Inputs!$D$4:$H$4, "Y", Outputs_External!D4:'Outputs_External'!H4)</f>
@@ -2607,11 +2621,11 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="D5" s="1">
         <f>SUMIF(Inputs!$D$4:$H$4, "N", Outputs_External!D4:'Outputs_External'!H4)</f>
-        <v>32750</v>
+        <v>60000</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="10">
@@ -2629,11 +2643,11 @@
       </c>
       <c r="K5" s="12">
         <f t="shared" si="0"/>
-        <v>3275</v>
+        <v>6000</v>
       </c>
       <c r="L5" s="12">
         <f t="shared" si="0"/>
-        <v>29475</v>
+        <v>54000</v>
       </c>
       <c r="M5" s="12">
         <f t="shared" si="0"/>
@@ -2655,7 +2669,7 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
@@ -2706,7 +2720,7 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C9" s="17" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D9" s="18">
         <f>SUM(Calcs!D15:H15)</f>
@@ -2783,7 +2797,7 @@
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C11" s="17" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D11" s="18">
         <f>SUM(Calcs!D17:H17)</f>
@@ -2896,7 +2910,7 @@
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C14" s="17" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D14" s="18">
         <f>SUM(Calcs!D20:H20)</f>
@@ -3010,7 +3024,7 @@
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C17" s="19" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D17" s="20">
         <f>SUM(Calcs!D23:H23)</f>
@@ -3057,7 +3071,7 @@
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G19" s="48" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="H19" s="10">
         <v>0.1</v>
@@ -3078,7 +3092,7 @@
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
@@ -3132,7 +3146,7 @@
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C23" s="17" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D23" s="18">
         <f>SUM(Calcs!D27:H27)</f>
@@ -3216,7 +3230,7 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C25" s="17" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D25" s="18">
         <f>SUM(Calcs!D29:H29)</f>
@@ -3339,7 +3353,7 @@
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C28" s="17" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D28" s="18">
         <f>SUM(Calcs!D32:H32)</f>
@@ -3462,7 +3476,7 @@
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C31" s="28" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D31" s="29">
         <f>SUM(Calcs!D35:H35)</f>
@@ -3512,7 +3526,7 @@
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -3676,7 +3690,7 @@
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C38" s="19" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="D38" s="20">
         <f>SUM(Calcs!D84:H84)</f>
@@ -3714,7 +3728,7 @@
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C39" s="19" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D39" s="20">
         <f>SUM(Calcs!D85:H85)</f>
@@ -3752,7 +3766,7 @@
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C40" s="81" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D40" s="84">
         <f>SUM(Calcs!D86:H86)</f>
@@ -3795,7 +3809,7 @@
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
@@ -3967,7 +3981,7 @@
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C47" s="19" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="D47" s="20">
         <f>SUM(Calcs!D93:H93)</f>
@@ -4007,7 +4021,7 @@
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C48" s="19" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D48" s="20">
         <f>SUM(Calcs!D94:H94)</f>
@@ -4047,7 +4061,7 @@
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C49" s="81" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D49" s="84">
         <f>SUM(Calcs!D95:H95)</f>
@@ -4092,7 +4106,7 @@
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
@@ -4100,7 +4114,7 @@
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D52" s="1">
         <f>SUM(Outputs_External!D28:'Outputs_External'!H28)</f>
@@ -4141,7 +4155,7 @@
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="D53" s="1">
         <f>SUM(Outputs_External!D29:'Outputs_External'!H29)</f>
@@ -4182,7 +4196,7 @@
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D54" s="1">
         <f>Outputs_External!D30</f>
@@ -4225,7 +4239,7 @@
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="D56" s="1">
         <f>SUM(Outputs_External!D32:'Outputs_External'!H32)</f>
@@ -4250,7 +4264,7 @@
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C57" s="21" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="D57" s="23">
         <f>SUM(K56:N56)</f>
@@ -4267,19 +4281,19 @@
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B59" s="6" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D59" s="1">
         <f>SUM(Outputs_Timeline!S:S)</f>
-        <v>311182.5</v>
+        <v>338432.5</v>
       </c>
       <c r="K59" s="12">
         <f>SUM(Outputs_Timeline!T:T)</f>
-        <v>78464.23501324169</v>
+        <v>81189.23501324169</v>
       </c>
       <c r="L59" s="12">
         <f>SUM(Outputs_Timeline!U:U)</f>
-        <v>232718.26498675838</v>
+        <v>257243.26498675841</v>
       </c>
       <c r="M59" s="12">
         <f>SUM(Outputs_Timeline!V:V)</f>
@@ -4294,11 +4308,11 @@
       <c r="D60" s="1"/>
       <c r="K60" s="53">
         <f>IFERROR(K59/$D$59, 0)</f>
-        <v>0.25214861058459809</v>
+        <v>0.23989786741297509</v>
       </c>
       <c r="L60" s="53">
         <f>IFERROR(L59/$D$59, 0)</f>
-        <v>0.74785138941540219</v>
+        <v>0.76010213258702519</v>
       </c>
       <c r="M60" s="53">
         <f>IFERROR(M59/$D$59, 0)</f>
@@ -4306,7 +4320,7 @@
       </c>
       <c r="N60" s="53">
         <f>IFERROR(N59/$D$59, 0)</f>
-        <v>2.6283475167344877E-17</v>
+        <v>2.4167175171599351E-17</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
@@ -4316,7 +4330,7 @@
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B63" s="27" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C63" s="21"/>
       <c r="D63" s="21"/>
@@ -4509,7 +4523,7 @@
     <row r="68" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B68" s="27"/>
       <c r="C68" s="21" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="D68" s="23">
         <f>SUM(Calcs!D66:H66)+SUM(Calcs!D75:H75)</f>
@@ -4553,7 +4567,7 @@
     <row r="69" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B69" s="27"/>
       <c r="C69" s="21" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D69" s="23">
         <f>SUM(Calcs!D67:H67)+SUM(Calcs!D76:H76)</f>
@@ -4597,7 +4611,7 @@
     <row r="70" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B70" s="27"/>
       <c r="C70" s="21" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D70" s="23">
         <f>SUM(Calcs!D68:H68)+SUM(Calcs!D77:H77)</f>
@@ -4649,7 +4663,7 @@
   <dimension ref="B1:W94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="P15" sqref="P15"/>
@@ -4680,20 +4694,20 @@
         <v>36</v>
       </c>
       <c r="H1" s="61" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="I1" s="61"/>
       <c r="J1" s="61"/>
       <c r="K1" s="61"/>
       <c r="M1" s="61" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="N1" s="61"/>
       <c r="O1" s="61"/>
       <c r="P1" s="61"/>
       <c r="Q1" s="61"/>
       <c r="S1" s="61" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="T1" s="61"/>
       <c r="U1" s="61"/>
@@ -4701,60 +4715,60 @@
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" s="59" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C2" s="59"/>
       <c r="D2" s="59" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="F2" s="59" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="G2" s="59"/>
       <c r="H2" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="62" t="s">
-        <v>82</v>
-      </c>
-      <c r="J2" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" s="62" t="s">
-        <v>83</v>
-      </c>
-      <c r="M2" s="62" t="s">
+      <c r="Q2" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="S2" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="T2" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="U2" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="N2" s="62" t="s">
-        <v>82</v>
-      </c>
-      <c r="O2" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="P2" s="62" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q2" s="62" t="s">
-        <v>96</v>
-      </c>
-      <c r="S2" s="62" t="s">
-        <v>81</v>
-      </c>
-      <c r="T2" s="62" t="s">
-        <v>82</v>
-      </c>
-      <c r="U2" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="V2" s="62" t="s">
-        <v>97</v>
-      </c>
       <c r="W2" s="62" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
@@ -5183,15 +5197,15 @@
       </c>
       <c r="H9" s="63">
         <f>IF($B9=Inputs!$C$1,SUM(Outputs_Internal!$D$4, Outputs_Internal!$D$5),0)*$D9</f>
-        <v>42750</v>
+        <v>70000</v>
       </c>
       <c r="I9" s="63">
         <f>IF($B9=Inputs!$C$1,SUM(Outputs_Internal!K$4, Outputs_Internal!K$5),0)*$D9</f>
-        <v>8275</v>
+        <v>11000</v>
       </c>
       <c r="J9" s="63">
         <f>IF($B9=Inputs!$C$1,SUM(Outputs_Internal!L$4, Outputs_Internal!L$5),0)*$D9</f>
-        <v>34475</v>
+        <v>59000</v>
       </c>
       <c r="K9" s="63">
         <f>IF($B9=Inputs!$C$1,SUM(Outputs_Internal!M$4, Outputs_Internal!$M$5),0)*$D9</f>
@@ -5367,15 +5381,15 @@
       </c>
       <c r="S11" s="63">
         <f t="shared" si="1"/>
-        <v>65119.375000000007</v>
+        <v>92369.374999999985</v>
       </c>
       <c r="T11" s="63">
         <f t="shared" si="2"/>
-        <v>14124.102917770138</v>
+        <v>16849.102917770138</v>
       </c>
       <c r="U11" s="63">
         <f>IF(MOD(MONTH($B11),3)=0,SUM(J9:J11,O9:O11),0)</f>
-        <v>50995.272082229858</v>
+        <v>75520.272082229858</v>
       </c>
       <c r="V11" s="63">
         <f t="shared" si="4"/>
@@ -11543,10 +11557,10 @@
   <dimension ref="A2:O126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K96" sqref="K96"/>
+      <selection pane="bottomRight" activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11560,34 +11574,34 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>109</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
@@ -11600,23 +11614,23 @@
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <f>IF(AND(Inputs!D5="Y",Inputs!D4="Y"), 0, IF(Inputs!D4="Y", SUM(Prices!$C$3, IF(Inputs!D$6 ="Y", Prices!$C$4, 0)), IF(Inputs!D4="N", Prices!$D$3, 0)))</f>
+        <f>IF(AND(Inputs!D5="Y",Inputs!D4="Y"), 0, IF(Inputs!D4="Y", SUM(Prices!$C$3, IF(Inputs!D$6 ="Y", Prices!$C$4, 0)), IF(Inputs!D4="N", Prices!$D$3, 0)))*Inputs!D8</f>
         <v>10000</v>
       </c>
       <c r="E4" s="1">
-        <f>IF(AND(Inputs!E5="Y",Inputs!E4="Y"), 0, IF(Inputs!E4="Y", SUM(Prices!$C$3, IF(Inputs!E$6 ="Y", Prices!$C$4, 0)), IF(Inputs!E4="N", Prices!$D$3, 0)))</f>
-        <v>32750</v>
+        <f>IF(AND(Inputs!E5="Y",Inputs!E4="Y"), 0, IF(Inputs!E4="Y", SUM(Prices!$C$3, IF(Inputs!E$6 ="Y", Prices!$C$4, 0)), IF(Inputs!E4="N", Prices!$D$3, 0)))*Inputs!E8</f>
+        <v>60000</v>
       </c>
       <c r="F4" s="1">
-        <f>IF(AND(Inputs!F5="Y",Inputs!F4="Y"), 0, IF(Inputs!F4="Y", SUM(Prices!$C$3, IF(Inputs!F$6 ="Y", Prices!$C$4, 0)), IF(Inputs!F4="N", Prices!$D$3, 0)))</f>
+        <f>IF(AND(Inputs!F5="Y",Inputs!F4="Y"), 0, IF(Inputs!F4="Y", SUM(Prices!$C$3, IF(Inputs!F$6 ="Y", Prices!$C$4, 0)), IF(Inputs!F4="N", Prices!$D$3, 0)))*Inputs!F8</f>
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <f>IF(AND(Inputs!G5="Y",Inputs!G4="Y"), 0, IF(Inputs!G4="Y", SUM(Prices!$C$3, IF(Inputs!G$6 ="Y", Prices!$C$4, 0)), IF(Inputs!G4="N", Prices!$D$3, 0)))</f>
+        <f>IF(AND(Inputs!G5="Y",Inputs!G4="Y"), 0, IF(Inputs!G4="Y", SUM(Prices!$C$3, IF(Inputs!G$6 ="Y", Prices!$C$4, 0)), IF(Inputs!G4="N", Prices!$D$3, 0)))*Inputs!G8</f>
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <f>IF(AND(Inputs!H5="Y",Inputs!H4="Y"), 0, IF(Inputs!H4="Y", SUM(Prices!$C$3, IF(Inputs!H$6 ="Y", Prices!$C$4, 0)), IF(Inputs!H4="N", Prices!$D$3, 0)))</f>
+        <f>IF(AND(Inputs!H5="Y",Inputs!H4="Y"), 0, IF(Inputs!H4="Y", SUM(Prices!$C$3, IF(Inputs!H$6 ="Y", Prices!$C$4, 0)), IF(Inputs!H4="N", Prices!$D$3, 0)))*Inputs!H8</f>
         <v>0</v>
       </c>
     </row>
@@ -11627,18 +11641,18 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="K5" s="22" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="L5" s="22" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="M5" s="22" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="D6" s="5">
         <f>IF(Inputs!D$4="N",MIN(MAX(Inputs!D$7-$K6,0),$L6-$K6),0)</f>
@@ -11672,7 +11686,7 @@
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="D7" s="5">
         <f>IF(Inputs!D$4="N",MIN(MAX(Inputs!D$7-$K7,0),$L7-$K7),0)</f>
@@ -11707,7 +11721,7 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="D8" s="5">
         <f>IF(Inputs!D$4="N",MIN(MAX(Inputs!D$7-$K8,0),$L8-$K8),0)</f>
@@ -11742,7 +11756,7 @@
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="D9" s="5">
         <f>IF(Inputs!D$4="N",MIN(MAX(Inputs!D$7-$K9,0),$L9-$K9),0)</f>
@@ -11777,7 +11791,7 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C10" s="78" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="D10" s="79">
         <f>IFERROR(SUMPRODUCT(D6:D9,$M$6:$M$9)/SUM(D6:D9),0)</f>
@@ -11802,7 +11816,7 @@
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" s="78" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D11" s="80">
         <f>SUM(D6:D9)</f>
@@ -11834,7 +11848,7 @@
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
@@ -11864,26 +11878,26 @@
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C15" s="17" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D15" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!D9="Y",Inputs!D$19="Y"), Prices!$C10, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D10="Y",Inputs!D$20="Y"), Prices!$C10, 0)</f>
         <v>0</v>
       </c>
       <c r="E15" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!E9="Y",Inputs!E$19="Y"), Prices!$C10, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E10="Y",Inputs!E$20="Y"), Prices!$C10, 0)</f>
         <v>0</v>
       </c>
       <c r="F15" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!F9="Y",Inputs!F$19="Y"), Prices!$C10, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F10="Y",Inputs!F$20="Y"), Prices!$C10, 0)</f>
         <v>0</v>
       </c>
       <c r="G15" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!G9="Y",Inputs!G$19="Y"), Prices!$C10, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G10="Y",Inputs!G$20="Y"), Prices!$C10, 0)</f>
         <v>0</v>
       </c>
       <c r="H15" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!H9="Y",Inputs!H$19="Y"), Prices!$C10, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H10="Y",Inputs!H$20="Y"), Prices!$C10, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11892,48 +11906,48 @@
         <v>8</v>
       </c>
       <c r="D16" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!D10="Y",Inputs!D$19="Y"), Prices!$C11, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D11="Y",Inputs!D$20="Y"), Prices!$C11, 0)</f>
         <v>0</v>
       </c>
       <c r="E16" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!E10="Y",Inputs!E$19="Y"), Prices!$C11, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E11="Y",Inputs!E$20="Y"), Prices!$C11, 0)</f>
         <v>0</v>
       </c>
       <c r="F16" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!F10="Y",Inputs!F$19="Y"), Prices!$C11, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F11="Y",Inputs!F$20="Y"), Prices!$C11, 0)</f>
         <v>0</v>
       </c>
       <c r="G16" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!G10="Y",Inputs!G$19="Y"), Prices!$C11, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G11="Y",Inputs!G$20="Y"), Prices!$C11, 0)</f>
         <v>0</v>
       </c>
       <c r="H16" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!H10="Y",Inputs!H$19="Y"), Prices!$C11, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H11="Y",Inputs!H$20="Y"), Prices!$C11, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C17" s="17" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D17" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!D11="Y",Inputs!D$19="Y"), Prices!$C12, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D12="Y",Inputs!D$20="Y"), Prices!$C12, 0)</f>
         <v>0</v>
       </c>
       <c r="E17" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!E11="Y",Inputs!E$19="Y"), Prices!$C12, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E12="Y",Inputs!E$20="Y"), Prices!$C12, 0)</f>
         <v>0</v>
       </c>
       <c r="F17" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!F11="Y",Inputs!F$19="Y"), Prices!$C12, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F12="Y",Inputs!F$20="Y"), Prices!$C12, 0)</f>
         <v>0</v>
       </c>
       <c r="G17" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!G11="Y",Inputs!G$19="Y"), Prices!$C12, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G12="Y",Inputs!G$20="Y"), Prices!$C12, 0)</f>
         <v>0</v>
       </c>
       <c r="H17" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!H11="Y",Inputs!H$19="Y"), Prices!$C12, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H12="Y",Inputs!H$20="Y"), Prices!$C12, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11942,23 +11956,23 @@
         <v>9</v>
       </c>
       <c r="D18" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!D12="Y",Inputs!D$19="Y"), Prices!$C13, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D13="Y",Inputs!D$20="Y"), Prices!$C13, 0)</f>
         <v>0</v>
       </c>
       <c r="E18" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!E12="Y",Inputs!E$19="Y"), Prices!$C13, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E13="Y",Inputs!E$20="Y"), Prices!$C13, 0)</f>
         <v>0</v>
       </c>
       <c r="F18" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!F12="Y",Inputs!F$19="Y"), Prices!$C13, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F13="Y",Inputs!F$20="Y"), Prices!$C13, 0)</f>
         <v>0</v>
       </c>
       <c r="G18" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!G12="Y",Inputs!G$19="Y"), Prices!$C13, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G13="Y",Inputs!G$20="Y"), Prices!$C13, 0)</f>
         <v>0</v>
       </c>
       <c r="H18" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!H12="Y",Inputs!H$19="Y"), Prices!$C13, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H13="Y",Inputs!H$20="Y"), Prices!$C13, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11967,48 +11981,48 @@
         <v>10</v>
       </c>
       <c r="D19" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!D13="Y",Inputs!D$19="Y"), Prices!$C14, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D14="Y",Inputs!D$20="Y"), Prices!$C14, 0)</f>
         <v>0</v>
       </c>
       <c r="E19" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!E13="Y",Inputs!E$19="Y"), Prices!$C14, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E14="Y",Inputs!E$20="Y"), Prices!$C14, 0)</f>
         <v>0</v>
       </c>
       <c r="F19" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!F13="Y",Inputs!F$19="Y"), Prices!$C14, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F14="Y",Inputs!F$20="Y"), Prices!$C14, 0)</f>
         <v>0</v>
       </c>
       <c r="G19" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!G13="Y",Inputs!G$19="Y"), Prices!$C14, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G14="Y",Inputs!G$20="Y"), Prices!$C14, 0)</f>
         <v>0</v>
       </c>
       <c r="H19" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!H13="Y",Inputs!H$19="Y"), Prices!$C14, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H14="Y",Inputs!H$20="Y"), Prices!$C14, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C20" s="17" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D20" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!D14="Y",Inputs!D$19="Y"), Prices!$C15, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D15="Y",Inputs!D$20="Y"), Prices!$C15, 0)</f>
         <v>0</v>
       </c>
       <c r="E20" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!E14="Y",Inputs!E$19="Y"), Prices!$C15, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E15="Y",Inputs!E$20="Y"), Prices!$C15, 0)</f>
         <v>0</v>
       </c>
       <c r="F20" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!F14="Y",Inputs!F$19="Y"), Prices!$C15, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F15="Y",Inputs!F$20="Y"), Prices!$C15, 0)</f>
         <v>0</v>
       </c>
       <c r="G20" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!G14="Y",Inputs!G$19="Y"), Prices!$C15, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G15="Y",Inputs!G$20="Y"), Prices!$C15, 0)</f>
         <v>0</v>
       </c>
       <c r="H20" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!H14="Y",Inputs!H$19="Y"), Prices!$C15, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H15="Y",Inputs!H$20="Y"), Prices!$C15, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12017,23 +12031,23 @@
         <v>11</v>
       </c>
       <c r="D21" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!D15="Y",Inputs!D$20="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D16="Y",Inputs!D$21="Y"), Prices!$C16, 0)</f>
         <v>0</v>
       </c>
       <c r="E21" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!E15="Y",Inputs!E$20="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E16="Y",Inputs!E$21="Y"), Prices!$C16, 0)</f>
         <v>0</v>
       </c>
       <c r="F21" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!F15="Y",Inputs!F$20="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F16="Y",Inputs!F$21="Y"), Prices!$C16, 0)</f>
         <v>0</v>
       </c>
       <c r="G21" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!G15="Y",Inputs!G$20="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G16="Y",Inputs!G$21="Y"), Prices!$C16, 0)</f>
         <v>0</v>
       </c>
       <c r="H21" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!H15="Y",Inputs!H$20="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H16="Y",Inputs!H$21="Y"), Prices!$C16, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12042,54 +12056,54 @@
         <v>12</v>
       </c>
       <c r="D22" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!D16="Y",Inputs!D$20="Y"), Prices!$C17, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D17="Y",Inputs!D$21="Y"), Prices!$C17, 0)</f>
         <v>0</v>
       </c>
       <c r="E22" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!E16="Y",Inputs!E$20="Y"), Prices!$C17, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E17="Y",Inputs!E$21="Y"), Prices!$C17, 0)</f>
         <v>0</v>
       </c>
       <c r="F22" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!F16="Y",Inputs!F$20="Y"), Prices!$C17, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F17="Y",Inputs!F$21="Y"), Prices!$C17, 0)</f>
         <v>0</v>
       </c>
       <c r="G22" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!G16="Y",Inputs!G$20="Y"), Prices!$C17, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G17="Y",Inputs!G$21="Y"), Prices!$C17, 0)</f>
         <v>0</v>
       </c>
       <c r="H22" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!H16="Y",Inputs!H$20="Y"), Prices!$C17, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H17="Y",Inputs!H$21="Y"), Prices!$C17, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C23" s="19" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D23" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!D17="Y",Inputs!D$20="Y"), Prices!$C18, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D18="Y",Inputs!D$21="Y"), Prices!$C18, 0)</f>
         <v>0</v>
       </c>
       <c r="E23" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!E17="Y",Inputs!E$20="Y"), Prices!$C18, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E18="Y",Inputs!E$21="Y"), Prices!$C18, 0)</f>
         <v>0</v>
       </c>
       <c r="F23" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!F17="Y",Inputs!F$20="Y"), Prices!$C18, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F18="Y",Inputs!F$21="Y"), Prices!$C18, 0)</f>
         <v>0</v>
       </c>
       <c r="G23" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!G17="Y",Inputs!G$20="Y"), Prices!$C18, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G18="Y",Inputs!G$21="Y"), Prices!$C18, 0)</f>
         <v>0</v>
       </c>
       <c r="H23" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!H17="Y",Inputs!H$20="Y"), Prices!$C18, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H18="Y",Inputs!H$21="Y"), Prices!$C18, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -12119,26 +12133,26 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C27" s="17" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D27" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D9="Y",Inputs!D$19="Y"),PRODUCT(D$11, Prices!$E10),0))*D$10</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D10="Y",Inputs!D$20="Y"),PRODUCT(D$11, Prices!$E10),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E27" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E9="Y",Inputs!E$19="Y"),PRODUCT(E$11, Prices!$E10),0))*E$10</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E10="Y",Inputs!E$20="Y"),PRODUCT(E$11, Prices!$E10),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F27" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F9="Y",Inputs!F$19="Y"),PRODUCT(F$11, Prices!$E10),0))*F$10</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F10="Y",Inputs!F$20="Y"),PRODUCT(F$11, Prices!$E10),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G27" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G9="Y",Inputs!G$19="Y"),PRODUCT(G$11, Prices!$E10),0))*G$10</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G10="Y",Inputs!G$20="Y"),PRODUCT(G$11, Prices!$E10),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H27" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H9="Y",Inputs!H$19="Y"),PRODUCT(H$11, Prices!$E10),0))*H$10</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H10="Y",Inputs!H$20="Y"),PRODUCT(H$11, Prices!$E10),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12147,48 +12161,48 @@
         <v>8</v>
       </c>
       <c r="D28" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D10="Y",Inputs!D$19="Y"),PRODUCT(D$11, Prices!$E11),0))*D$10</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D11="Y",Inputs!D$20="Y"),PRODUCT(D$11, Prices!$E11),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E28" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E10="Y",Inputs!E$19="Y"),PRODUCT(E$11, Prices!$E11),0))*E$10</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E11="Y",Inputs!E$20="Y"),PRODUCT(E$11, Prices!$E11),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F28" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F10="Y",Inputs!F$19="Y"),PRODUCT(F$11, Prices!$E11),0))*F$10</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F11="Y",Inputs!F$20="Y"),PRODUCT(F$11, Prices!$E11),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G28" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G10="Y",Inputs!G$19="Y"),PRODUCT(G$11, Prices!$E11),0))*G$10</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G11="Y",Inputs!G$20="Y"),PRODUCT(G$11, Prices!$E11),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H28" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H10="Y",Inputs!H$19="Y"),PRODUCT(H$11, Prices!$E11),0))*H$10</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H11="Y",Inputs!H$20="Y"),PRODUCT(H$11, Prices!$E11),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C29" s="17" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D29" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D11="Y",Inputs!D$19="Y"),PRODUCT(D$11, Prices!$E12),0))*D$10</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D12="Y",Inputs!D$20="Y"),PRODUCT(D$11, Prices!$E12),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E29" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E11="Y",Inputs!E$19="Y"),PRODUCT(E$11, Prices!$E12),0))*E$10</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E12="Y",Inputs!E$20="Y"),PRODUCT(E$11, Prices!$E12),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F29" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F11="Y",Inputs!F$19="Y"),PRODUCT(F$11, Prices!$E12),0))*F$10</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F12="Y",Inputs!F$20="Y"),PRODUCT(F$11, Prices!$E12),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G29" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G11="Y",Inputs!G$19="Y"),PRODUCT(G$11, Prices!$E12),0))*G$10</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G12="Y",Inputs!G$20="Y"),PRODUCT(G$11, Prices!$E12),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H29" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H11="Y",Inputs!H$19="Y"),PRODUCT(H$11, Prices!$E12),0))*H$10</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H12="Y",Inputs!H$20="Y"),PRODUCT(H$11, Prices!$E12),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12197,23 +12211,23 @@
         <v>9</v>
       </c>
       <c r="D30" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D12="Y",Inputs!D$19="Y"),PRODUCT(D$11, Prices!$E13),0))*D$10</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D13="Y",Inputs!D$20="Y"),PRODUCT(D$11, Prices!$E13),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E30" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E12="Y",Inputs!E$19="Y"),PRODUCT(E$11, Prices!$E13),0))*E$10</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E13="Y",Inputs!E$20="Y"),PRODUCT(E$11, Prices!$E13),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F30" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F12="Y",Inputs!F$19="Y"),PRODUCT(F$11, Prices!$E13),0))*F$10</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F13="Y",Inputs!F$20="Y"),PRODUCT(F$11, Prices!$E13),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G30" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G12="Y",Inputs!G$19="Y"),PRODUCT(G$11, Prices!$E13),0))*G$10</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G13="Y",Inputs!G$20="Y"),PRODUCT(G$11, Prices!$E13),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H30" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H12="Y",Inputs!H$19="Y"),PRODUCT(H$11, Prices!$E13),0))*H$10</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H13="Y",Inputs!H$20="Y"),PRODUCT(H$11, Prices!$E13),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12222,48 +12236,48 @@
         <v>10</v>
       </c>
       <c r="D31" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D13="Y",Inputs!D$19="Y"),PRODUCT(D$11, Prices!$E14),0))*D$10</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D14="Y",Inputs!D$20="Y"),PRODUCT(D$11, Prices!$E14),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E31" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E13="Y",Inputs!E$19="Y"),PRODUCT(E$11, Prices!$E14),0))*E$10</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E14="Y",Inputs!E$20="Y"),PRODUCT(E$11, Prices!$E14),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F31" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F13="Y",Inputs!F$19="Y"),PRODUCT(F$11, Prices!$E14),0))*F$10</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F14="Y",Inputs!F$20="Y"),PRODUCT(F$11, Prices!$E14),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G31" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G13="Y",Inputs!G$19="Y"),PRODUCT(G$11, Prices!$E14),0))*G$10</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G14="Y",Inputs!G$20="Y"),PRODUCT(G$11, Prices!$E14),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H31" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H13="Y",Inputs!H$19="Y"),PRODUCT(H$11, Prices!$E14),0))*H$10</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H14="Y",Inputs!H$20="Y"),PRODUCT(H$11, Prices!$E14),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C32" s="17" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D32" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D14="Y",Inputs!D$19="Y"),PRODUCT(D$11, Prices!$E15),0))*D$10</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D15="Y",Inputs!D$20="Y"),PRODUCT(D$11, Prices!$E15),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E32" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E14="Y",Inputs!E$19="Y"),PRODUCT(E$11, Prices!$E15),0))*E$10</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E15="Y",Inputs!E$20="Y"),PRODUCT(E$11, Prices!$E15),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F32" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F14="Y",Inputs!F$19="Y"),PRODUCT(F$11, Prices!$E15),0))*F$10</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F15="Y",Inputs!F$20="Y"),PRODUCT(F$11, Prices!$E15),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G32" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G14="Y",Inputs!G$19="Y"),PRODUCT(G$11, Prices!$E15),0))*G$10</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G15="Y",Inputs!G$20="Y"),PRODUCT(G$11, Prices!$E15),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H32" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H14="Y",Inputs!H$19="Y"),PRODUCT(H$11, Prices!$E15),0))*H$10</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H15="Y",Inputs!H$20="Y"),PRODUCT(H$11, Prices!$E15),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12272,23 +12286,23 @@
         <v>11</v>
       </c>
       <c r="D33" s="20">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D15="Y",Inputs!D$20="Y"),PRODUCT(D$11, Prices!$E16),0))*D$10</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D16="Y",Inputs!D$21="Y"),PRODUCT(D$11, Prices!$E16),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E33" s="20">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E15="Y",Inputs!E$20="Y"),PRODUCT(E$11, Prices!$E16),0))*E$10</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E16="Y",Inputs!E$21="Y"),PRODUCT(E$11, Prices!$E16),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F33" s="20">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F15="Y",Inputs!F$20="Y"),PRODUCT(F$11, Prices!$E16),0))*F$10</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F16="Y",Inputs!F$21="Y"),PRODUCT(F$11, Prices!$E16),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G33" s="20">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G15="Y",Inputs!G$20="Y"),PRODUCT(G$11, Prices!$E16),0))*G$10</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G16="Y",Inputs!G$21="Y"),PRODUCT(G$11, Prices!$E16),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H33" s="20">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H15="Y",Inputs!H$20="Y"),PRODUCT(H$11, Prices!$E16),0))*H$10</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H16="Y",Inputs!H$21="Y"),PRODUCT(H$11, Prices!$E16),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12297,29 +12311,29 @@
         <v>12</v>
       </c>
       <c r="D34" s="20">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D16="Y",Inputs!D$20="Y"),PRODUCT(D$11, Prices!$E17),0))*D$10</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D17="Y",Inputs!D$21="Y"),PRODUCT(D$11, Prices!$E17),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E34" s="20">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E16="Y",Inputs!E$20="Y"),PRODUCT(E$11, Prices!$E17),0))*E$10</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E17="Y",Inputs!E$21="Y"),PRODUCT(E$11, Prices!$E17),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F34" s="20">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F16="Y",Inputs!F$20="Y"),PRODUCT(F$11, Prices!$E17),0))*F$10</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F17="Y",Inputs!F$21="Y"),PRODUCT(F$11, Prices!$E17),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G34" s="20">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G16="Y",Inputs!G$20="Y"),PRODUCT(G$11, Prices!$E17),0))*G$10</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G17="Y",Inputs!G$21="Y"),PRODUCT(G$11, Prices!$E17),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H34" s="20">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H16="Y",Inputs!H$20="Y"),PRODUCT(H$11, Prices!$E17),0))*H$10</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H17="Y",Inputs!H$21="Y"),PRODUCT(H$11, Prices!$E17),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C35" s="28" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D35" s="29">
         <v>0</v>
@@ -12346,7 +12360,7 @@
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -12376,26 +12390,26 @@
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C39" s="17" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D39" s="18">
-        <f>IF(AND(Inputs!D9="Y",Inputs!D$19="N"),Prices!$C10,0)</f>
+        <f>IF(AND(Inputs!D10="Y",Inputs!D$20="N"),Prices!$C10,0)</f>
         <v>0</v>
       </c>
       <c r="E39" s="18">
-        <f>IF(AND(Inputs!E9="Y",Inputs!E$19="N"),Prices!$C10,0)</f>
+        <f>IF(AND(Inputs!E10="Y",Inputs!E$20="N"),Prices!$C10,0)</f>
         <v>0</v>
       </c>
       <c r="F39" s="18">
-        <f>IF(AND(Inputs!F9="Y",Inputs!F$19="N"),Prices!$C10,0)</f>
+        <f>IF(AND(Inputs!F10="Y",Inputs!F$20="N"),Prices!$C10,0)</f>
         <v>0</v>
       </c>
       <c r="G39" s="18">
-        <f>IF(AND(Inputs!G9="Y",Inputs!G$19="N"),Prices!$C10,0)</f>
+        <f>IF(AND(Inputs!G10="Y",Inputs!G$20="N"),Prices!$C10,0)</f>
         <v>0</v>
       </c>
       <c r="H39" s="18">
-        <f>IF(AND(Inputs!H9="Y",Inputs!H$19="N"),Prices!$C10,0)</f>
+        <f>IF(AND(Inputs!H10="Y",Inputs!H$20="N"),Prices!$C10,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12404,48 +12418,48 @@
         <v>8</v>
       </c>
       <c r="D40" s="18">
-        <f>IF(AND(Inputs!D10="Y",Inputs!D$19="N"),Prices!$C11,0)</f>
+        <f>IF(AND(Inputs!D11="Y",Inputs!D$20="N"),Prices!$C11,0)</f>
         <v>0</v>
       </c>
       <c r="E40" s="18">
-        <f>IF(AND(Inputs!E10="Y",Inputs!E$19="N"),Prices!$C11,0)</f>
+        <f>IF(AND(Inputs!E11="Y",Inputs!E$20="N"),Prices!$C11,0)</f>
         <v>0</v>
       </c>
       <c r="F40" s="18">
-        <f>IF(AND(Inputs!F10="Y",Inputs!F$19="N"),Prices!$C11,0)</f>
+        <f>IF(AND(Inputs!F11="Y",Inputs!F$20="N"),Prices!$C11,0)</f>
         <v>0</v>
       </c>
       <c r="G40" s="18">
-        <f>IF(AND(Inputs!G10="Y",Inputs!G$19="N"),Prices!$C11,0)</f>
+        <f>IF(AND(Inputs!G11="Y",Inputs!G$20="N"),Prices!$C11,0)</f>
         <v>0</v>
       </c>
       <c r="H40" s="18">
-        <f>IF(AND(Inputs!H10="Y",Inputs!H$19="N"),Prices!$C11,0)</f>
+        <f>IF(AND(Inputs!H11="Y",Inputs!H$20="N"),Prices!$C11,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C41" s="17" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D41" s="18">
-        <f>IF(AND(Inputs!D11="Y",Inputs!D$19="N"),Prices!$C12,0)</f>
+        <f>IF(AND(Inputs!D12="Y",Inputs!D$20="N"),Prices!$C12,0)</f>
         <v>0</v>
       </c>
       <c r="E41" s="18">
-        <f>IF(AND(Inputs!E11="Y",Inputs!E$19="N"),Prices!$C12,0)</f>
+        <f>IF(AND(Inputs!E12="Y",Inputs!E$20="N"),Prices!$C12,0)</f>
         <v>0</v>
       </c>
       <c r="F41" s="18">
-        <f>IF(AND(Inputs!F11="Y",Inputs!F$19="N"),Prices!$C12,0)</f>
+        <f>IF(AND(Inputs!F12="Y",Inputs!F$20="N"),Prices!$C12,0)</f>
         <v>0</v>
       </c>
       <c r="G41" s="18">
-        <f>IF(AND(Inputs!G11="Y",Inputs!G$19="N"),Prices!$C12,0)</f>
+        <f>IF(AND(Inputs!G12="Y",Inputs!G$20="N"),Prices!$C12,0)</f>
         <v>0</v>
       </c>
       <c r="H41" s="18">
-        <f>IF(AND(Inputs!H11="Y",Inputs!H$19="N"),Prices!$C12,0)</f>
+        <f>IF(AND(Inputs!H12="Y",Inputs!H$20="N"),Prices!$C12,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12454,23 +12468,23 @@
         <v>9</v>
       </c>
       <c r="D42" s="18">
-        <f>IF(AND(Inputs!D12="Y",Inputs!D$19="N"),Prices!$C13,0)</f>
+        <f>IF(AND(Inputs!D13="Y",Inputs!D$20="N"),Prices!$C13,0)</f>
         <v>0</v>
       </c>
       <c r="E42" s="18">
-        <f>IF(AND(Inputs!E12="Y",Inputs!E$19="N"),Prices!$C13,0)</f>
+        <f>IF(AND(Inputs!E13="Y",Inputs!E$20="N"),Prices!$C13,0)</f>
         <v>0</v>
       </c>
       <c r="F42" s="18">
-        <f>IF(AND(Inputs!F12="Y",Inputs!F$19="N"),Prices!$C13,0)</f>
+        <f>IF(AND(Inputs!F13="Y",Inputs!F$20="N"),Prices!$C13,0)</f>
         <v>0</v>
       </c>
       <c r="G42" s="18">
-        <f>IF(AND(Inputs!G12="Y",Inputs!G$19="N"),Prices!$C13,0)</f>
+        <f>IF(AND(Inputs!G13="Y",Inputs!G$20="N"),Prices!$C13,0)</f>
         <v>0</v>
       </c>
       <c r="H42" s="18">
-        <f>IF(AND(Inputs!H12="Y",Inputs!H$19="N"),Prices!$C13,0)</f>
+        <f>IF(AND(Inputs!H13="Y",Inputs!H$20="N"),Prices!$C13,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12479,48 +12493,48 @@
         <v>10</v>
       </c>
       <c r="D43" s="18">
-        <f>IF(AND(Inputs!D13="Y",Inputs!D$19="N"),Prices!$C14,0)</f>
+        <f>IF(AND(Inputs!D14="Y",Inputs!D$20="N"),Prices!$C14,0)</f>
         <v>0</v>
       </c>
       <c r="E43" s="18">
-        <f>IF(AND(Inputs!E13="Y",Inputs!E$19="N"),Prices!$C14,0)</f>
+        <f>IF(AND(Inputs!E14="Y",Inputs!E$20="N"),Prices!$C14,0)</f>
         <v>0</v>
       </c>
       <c r="F43" s="18">
-        <f>IF(AND(Inputs!F13="Y",Inputs!F$19="N"),Prices!$C14,0)</f>
+        <f>IF(AND(Inputs!F14="Y",Inputs!F$20="N"),Prices!$C14,0)</f>
         <v>0</v>
       </c>
       <c r="G43" s="18">
-        <f>IF(AND(Inputs!G13="Y",Inputs!G$19="N"),Prices!$C14,0)</f>
+        <f>IF(AND(Inputs!G14="Y",Inputs!G$20="N"),Prices!$C14,0)</f>
         <v>0</v>
       </c>
       <c r="H43" s="18">
-        <f>IF(AND(Inputs!H13="Y",Inputs!H$19="N"),Prices!$C14,0)</f>
+        <f>IF(AND(Inputs!H14="Y",Inputs!H$20="N"),Prices!$C14,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C44" s="17" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D44" s="18">
-        <f>IF(AND(Inputs!D14="Y",Inputs!D$19="N"),Prices!$C15,0)</f>
+        <f>IF(AND(Inputs!D15="Y",Inputs!D$20="N"),Prices!$C15,0)</f>
         <v>0</v>
       </c>
       <c r="E44" s="18">
-        <f>IF(AND(Inputs!E14="Y",Inputs!E$19="N"),Prices!$C15,0)</f>
+        <f>IF(AND(Inputs!E15="Y",Inputs!E$20="N"),Prices!$C15,0)</f>
         <v>0</v>
       </c>
       <c r="F44" s="18">
-        <f>IF(AND(Inputs!F14="Y",Inputs!F$19="N"),Prices!$C15,0)</f>
+        <f>IF(AND(Inputs!F15="Y",Inputs!F$20="N"),Prices!$C15,0)</f>
         <v>0</v>
       </c>
       <c r="G44" s="18">
-        <f>IF(AND(Inputs!G14="Y",Inputs!G$19="N"),Prices!$C15,0)</f>
+        <f>IF(AND(Inputs!G15="Y",Inputs!G$20="N"),Prices!$C15,0)</f>
         <v>0</v>
       </c>
       <c r="H44" s="18">
-        <f>IF(AND(Inputs!H14="Y",Inputs!H$19="N"),Prices!$C15,0)</f>
+        <f>IF(AND(Inputs!H15="Y",Inputs!H$20="N"),Prices!$C15,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12529,23 +12543,23 @@
         <v>11</v>
       </c>
       <c r="D45" s="20">
-        <f>IF(AND(Inputs!D15="Y",Inputs!D$20="N"),Prices!$C16,0)</f>
+        <f>IF(AND(Inputs!D16="Y",Inputs!D$21="N"),Prices!$C16,0)</f>
         <v>0</v>
       </c>
       <c r="E45" s="20">
-        <f>IF(AND(Inputs!E15="Y",Inputs!E$20="N"),Prices!$C16,0)</f>
+        <f>IF(AND(Inputs!E16="Y",Inputs!E$21="N"),Prices!$C16,0)</f>
         <v>0</v>
       </c>
       <c r="F45" s="20">
-        <f>IF(AND(Inputs!F15="Y",Inputs!F$20="N"),Prices!$C16,0)</f>
+        <f>IF(AND(Inputs!F16="Y",Inputs!F$21="N"),Prices!$C16,0)</f>
         <v>0</v>
       </c>
       <c r="G45" s="20">
-        <f>IF(AND(Inputs!G15="Y",Inputs!G$20="N"),Prices!$C16,0)</f>
+        <f>IF(AND(Inputs!G16="Y",Inputs!G$21="N"),Prices!$C16,0)</f>
         <v>0</v>
       </c>
       <c r="H45" s="20">
-        <f>IF(AND(Inputs!H15="Y",Inputs!H$20="N"),Prices!$C16,0)</f>
+        <f>IF(AND(Inputs!H16="Y",Inputs!H$21="N"),Prices!$C16,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12554,54 +12568,54 @@
         <v>12</v>
       </c>
       <c r="D46" s="20">
-        <f>IF(AND(Inputs!D16="Y",Inputs!D$20="N"),Prices!$C17,0)</f>
+        <f>IF(AND(Inputs!D17="Y",Inputs!D$21="N"),Prices!$C17,0)</f>
         <v>0</v>
       </c>
       <c r="E46" s="20">
-        <f>IF(AND(Inputs!E16="Y",Inputs!E$20="N"),Prices!$C17,0)</f>
+        <f>IF(AND(Inputs!E17="Y",Inputs!E$21="N"),Prices!$C17,0)</f>
         <v>0</v>
       </c>
       <c r="F46" s="20">
-        <f>IF(AND(Inputs!F16="Y",Inputs!F$20="N"),Prices!$C17,0)</f>
+        <f>IF(AND(Inputs!F17="Y",Inputs!F$21="N"),Prices!$C17,0)</f>
         <v>0</v>
       </c>
       <c r="G46" s="20">
-        <f>IF(AND(Inputs!G16="Y",Inputs!G$20="N"),Prices!$C17,0)</f>
+        <f>IF(AND(Inputs!G17="Y",Inputs!G$21="N"),Prices!$C17,0)</f>
         <v>0</v>
       </c>
       <c r="H46" s="20">
-        <f>IF(AND(Inputs!H16="Y",Inputs!H$20="N"),Prices!$C17,0)</f>
+        <f>IF(AND(Inputs!H17="Y",Inputs!H$21="N"),Prices!$C17,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C47" s="19" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D47" s="20">
-        <f>IF(AND(Inputs!D17="Y",Inputs!D$20="N"),Prices!$C18,0)</f>
+        <f>IF(AND(Inputs!D18="Y",Inputs!D$21="N"),Prices!$C18,0)</f>
         <v>0</v>
       </c>
       <c r="E47" s="20">
-        <f>IF(AND(Inputs!E17="Y",Inputs!E$20="N"),Prices!$C18,0)</f>
+        <f>IF(AND(Inputs!E18="Y",Inputs!E$21="N"),Prices!$C18,0)</f>
         <v>0</v>
       </c>
       <c r="F47" s="20">
-        <f>IF(AND(Inputs!F17="Y",Inputs!F$20="N"),Prices!$C18,0)</f>
+        <f>IF(AND(Inputs!F18="Y",Inputs!F$21="N"),Prices!$C18,0)</f>
         <v>0</v>
       </c>
       <c r="G47" s="20">
-        <f>IF(AND(Inputs!G17="Y",Inputs!G$20="N"),Prices!$C18,0)</f>
+        <f>IF(AND(Inputs!G18="Y",Inputs!G$21="N"),Prices!$C18,0)</f>
         <v>0</v>
       </c>
       <c r="H47" s="20">
-        <f>IF(AND(Inputs!H17="Y",Inputs!H$20="N"),Prices!$C18,0)</f>
+        <f>IF(AND(Inputs!H18="Y",Inputs!H$21="N"),Prices!$C18,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="6" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
@@ -12631,26 +12645,26 @@
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C51" s="17" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D51" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D9="Y",Inputs!D$19="N"),PRODUCT(D$11, Prices!$E10)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D10="Y",Inputs!D$20="N"),PRODUCT(D$11, Prices!$E10)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E51" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E9="Y",Inputs!E$19="N"),PRODUCT(E$11, Prices!$E10)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E10="Y",Inputs!E$20="N"),PRODUCT(E$11, Prices!$E10)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F51" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F9="Y",Inputs!F$19="N"),PRODUCT(F$11, Prices!$E10)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F10="Y",Inputs!F$20="N"),PRODUCT(F$11, Prices!$E10)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G51" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G9="Y",Inputs!G$19="N"),PRODUCT(G$11, Prices!$E10)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G10="Y",Inputs!G$20="N"),PRODUCT(G$11, Prices!$E10)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H51" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H9="Y",Inputs!H$19="N"),PRODUCT(H$11, Prices!$E10)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H10="Y",Inputs!H$20="N"),PRODUCT(H$11, Prices!$E10)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12659,48 +12673,48 @@
         <v>8</v>
       </c>
       <c r="D52" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D10="Y",Inputs!D$19="N"),PRODUCT(D$11, Prices!$E11)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D11="Y",Inputs!D$20="N"),PRODUCT(D$11, Prices!$E11)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E52" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E10="Y",Inputs!E$19="N"),PRODUCT(E$11, Prices!$E11)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E11="Y",Inputs!E$20="N"),PRODUCT(E$11, Prices!$E11)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F52" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F10="Y",Inputs!F$19="N"),PRODUCT(F$11, Prices!$E11)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F11="Y",Inputs!F$20="N"),PRODUCT(F$11, Prices!$E11)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G52" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G10="Y",Inputs!G$19="N"),PRODUCT(G$11, Prices!$E11)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G11="Y",Inputs!G$20="N"),PRODUCT(G$11, Prices!$E11)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H52" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H10="Y",Inputs!H$19="N"),PRODUCT(H$11, Prices!$E11)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H11="Y",Inputs!H$20="N"),PRODUCT(H$11, Prices!$E11)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C53" s="17" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D53" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D11="Y",Inputs!D$19="N"),PRODUCT(D$11, Prices!$E12)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D12="Y",Inputs!D$20="N"),PRODUCT(D$11, Prices!$E12)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E53" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E11="Y",Inputs!E$19="N"),PRODUCT(E$11, Prices!$E12)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E12="Y",Inputs!E$20="N"),PRODUCT(E$11, Prices!$E12)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F53" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F11="Y",Inputs!F$19="N"),PRODUCT(F$11, Prices!$E12)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F12="Y",Inputs!F$20="N"),PRODUCT(F$11, Prices!$E12)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G53" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G11="Y",Inputs!G$19="N"),PRODUCT(G$11, Prices!$E12)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G12="Y",Inputs!G$20="N"),PRODUCT(G$11, Prices!$E12)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H53" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H11="Y",Inputs!H$19="N"),PRODUCT(H$11, Prices!$E12)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H12="Y",Inputs!H$20="N"),PRODUCT(H$11, Prices!$E12)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12709,23 +12723,23 @@
         <v>9</v>
       </c>
       <c r="D54" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D12="Y",Inputs!D$19="N"),PRODUCT(D$11, Prices!$E13)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D13="Y",Inputs!D$20="N"),PRODUCT(D$11, Prices!$E13)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E54" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E12="Y",Inputs!E$19="N"),PRODUCT(E$11, Prices!$E13)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E13="Y",Inputs!E$20="N"),PRODUCT(E$11, Prices!$E13)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F54" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F12="Y",Inputs!F$19="N"),PRODUCT(F$11, Prices!$E13)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F13="Y",Inputs!F$20="N"),PRODUCT(F$11, Prices!$E13)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G54" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G12="Y",Inputs!G$19="N"),PRODUCT(G$11, Prices!$E13)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G13="Y",Inputs!G$20="N"),PRODUCT(G$11, Prices!$E13)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H54" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H12="Y",Inputs!H$19="N"),PRODUCT(H$11, Prices!$E13)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H13="Y",Inputs!H$20="N"),PRODUCT(H$11, Prices!$E13)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12734,48 +12748,48 @@
         <v>10</v>
       </c>
       <c r="D55" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D13="Y",Inputs!D$19="N"),PRODUCT(D$11, Prices!$E14)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D14="Y",Inputs!D$20="N"),PRODUCT(D$11, Prices!$E14)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E55" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E13="Y",Inputs!E$19="N"),PRODUCT(E$11, Prices!$E14)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E14="Y",Inputs!E$20="N"),PRODUCT(E$11, Prices!$E14)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F55" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F13="Y",Inputs!F$19="N"),PRODUCT(F$11, Prices!$E14)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F14="Y",Inputs!F$20="N"),PRODUCT(F$11, Prices!$E14)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G55" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G13="Y",Inputs!G$19="N"),PRODUCT(G$11, Prices!$E14)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G14="Y",Inputs!G$20="N"),PRODUCT(G$11, Prices!$E14)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H55" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H13="Y",Inputs!H$19="N"),PRODUCT(H$11, Prices!$E14)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H14="Y",Inputs!H$20="N"),PRODUCT(H$11, Prices!$E14)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C56" s="17" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D56" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D14="Y",Inputs!D$19="N"),PRODUCT(D$11, Prices!$E15)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D15="Y",Inputs!D$20="N"),PRODUCT(D$11, Prices!$E15)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E56" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E14="Y",Inputs!E$19="N"),PRODUCT(E$11, Prices!$E15)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E15="Y",Inputs!E$20="N"),PRODUCT(E$11, Prices!$E15)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F56" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F14="Y",Inputs!F$19="N"),PRODUCT(F$11, Prices!$E15)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F15="Y",Inputs!F$20="N"),PRODUCT(F$11, Prices!$E15)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G56" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G14="Y",Inputs!G$19="N"),PRODUCT(G$11, Prices!$E15)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G15="Y",Inputs!G$20="N"),PRODUCT(G$11, Prices!$E15)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H56" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H14="Y",Inputs!H$19="N"),PRODUCT(H$11, Prices!$E15)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H15="Y",Inputs!H$20="N"),PRODUCT(H$11, Prices!$E15)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12784,23 +12798,23 @@
         <v>11</v>
       </c>
       <c r="D57" s="20">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D15="Y",Inputs!D$20="N"),PRODUCT(D$11, Prices!$E16)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D16="Y",Inputs!D$21="N"),PRODUCT(D$11, Prices!$E16)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E57" s="20">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E15="Y",Inputs!E$20="N"),PRODUCT(E$11, Prices!$E16)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E16="Y",Inputs!E$21="N"),PRODUCT(E$11, Prices!$E16)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F57" s="20">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F15="Y",Inputs!F$20="N"),PRODUCT(F$11, Prices!$E16)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F16="Y",Inputs!F$21="N"),PRODUCT(F$11, Prices!$E16)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G57" s="20">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G15="Y",Inputs!G$20="N"),PRODUCT(G$11, Prices!$E16)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G16="Y",Inputs!G$21="N"),PRODUCT(G$11, Prices!$E16)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H57" s="20">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H15="Y",Inputs!H$20="N"),PRODUCT(H$11, Prices!$E16)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H16="Y",Inputs!H$21="N"),PRODUCT(H$11, Prices!$E16)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12809,29 +12823,29 @@
         <v>12</v>
       </c>
       <c r="D58" s="20">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D16="Y",Inputs!D$20="N"),PRODUCT(D$11, Prices!$E17)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D17="Y",Inputs!D$21="N"),PRODUCT(D$11, Prices!$E17)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E58" s="20">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E16="Y",Inputs!E$20="N"),PRODUCT(E$11, Prices!$E17)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E17="Y",Inputs!E$21="N"),PRODUCT(E$11, Prices!$E17)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F58" s="20">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F16="Y",Inputs!F$20="N"),PRODUCT(F$11, Prices!$E17)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F17="Y",Inputs!F$21="N"),PRODUCT(F$11, Prices!$E17)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G58" s="20">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G16="Y",Inputs!G$20="N"),PRODUCT(G$11, Prices!$E17)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G17="Y",Inputs!G$21="N"),PRODUCT(G$11, Prices!$E17)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H58" s="20">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H16="Y",Inputs!H$20="N"),PRODUCT(H$11, Prices!$E17)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H17="Y",Inputs!H$21="N"),PRODUCT(H$11, Prices!$E17)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C59" s="28" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D59" s="29">
         <v>0</v>
@@ -12851,7 +12865,7 @@
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
@@ -12859,23 +12873,23 @@
         <v>14</v>
       </c>
       <c r="D62" s="18">
-        <f>IF(Inputs!D$19 = "Y", 0, IF(Inputs!D18="Y", Prices!$C20, 0))</f>
+        <f>IF(Inputs!D$20 = "Y", 0, IF(Inputs!D19="Y", Prices!$C20, 0))</f>
         <v>0</v>
       </c>
       <c r="E62" s="18">
-        <f>IF(Inputs!E$19 = "Y", 0, IF(Inputs!E18="Y", Prices!$C20, 0))</f>
+        <f>IF(Inputs!E$20 = "Y", 0, IF(Inputs!E19="Y", Prices!$C20, 0))</f>
         <v>0</v>
       </c>
       <c r="F62" s="18">
-        <f>IF(Inputs!F$19 = "Y", 0, IF(Inputs!F18="Y", Prices!$C20, 0))</f>
+        <f>IF(Inputs!F$20 = "Y", 0, IF(Inputs!F19="Y", Prices!$C20, 0))</f>
         <v>0</v>
       </c>
       <c r="G62" s="18">
-        <f>IF(Inputs!G$19 = "Y", 0, IF(Inputs!G18="Y", Prices!$C20, 0))</f>
+        <f>IF(Inputs!G$20 = "Y", 0, IF(Inputs!G19="Y", Prices!$C20, 0))</f>
         <v>0</v>
       </c>
       <c r="H62" s="18">
-        <f>IF(Inputs!H$19 = "Y", 0, IF(Inputs!H18="Y", Prices!$C20, 0))</f>
+        <f>IF(Inputs!H$20 = "Y", 0, IF(Inputs!H19="Y", Prices!$C20, 0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12884,23 +12898,23 @@
         <v>15</v>
       </c>
       <c r="D63" s="18">
-        <f>IF(Inputs!D19="Y", Prices!$C21, 0)</f>
+        <f>IF(Inputs!D20="Y", Prices!$C21, 0)</f>
         <v>0</v>
       </c>
       <c r="E63" s="18">
-        <f>IF(Inputs!E19="Y", Prices!$C21, 0)</f>
+        <f>IF(Inputs!E20="Y", Prices!$C21, 0)</f>
         <v>0</v>
       </c>
       <c r="F63" s="18">
-        <f>IF(Inputs!F19="Y", Prices!$C21, 0)</f>
+        <f>IF(Inputs!F20="Y", Prices!$C21, 0)</f>
         <v>0</v>
       </c>
       <c r="G63" s="18">
-        <f>IF(Inputs!G19="Y", Prices!$C21, 0)</f>
+        <f>IF(Inputs!G20="Y", Prices!$C21, 0)</f>
         <v>0</v>
       </c>
       <c r="H63" s="18">
-        <f>IF(Inputs!H19="Y", Prices!$C21, 0)</f>
+        <f>IF(Inputs!H20="Y", Prices!$C21, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12909,23 +12923,23 @@
         <v>16</v>
       </c>
       <c r="D64" s="20">
-        <f>IF(Inputs!D20="Y", Prices!$C22, 0)</f>
+        <f>IF(Inputs!D21="Y", Prices!$C22, 0)</f>
         <v>0</v>
       </c>
       <c r="E64" s="20">
-        <f>IF(Inputs!E20="Y", Prices!$C22, 0)</f>
+        <f>IF(Inputs!E21="Y", Prices!$C22, 0)</f>
         <v>0</v>
       </c>
       <c r="F64" s="20">
-        <f>IF(Inputs!F20="Y", Prices!$C22, 0)</f>
+        <f>IF(Inputs!F21="Y", Prices!$C22, 0)</f>
         <v>0</v>
       </c>
       <c r="G64" s="20">
-        <f>IF(Inputs!G20="Y", Prices!$C22, 0)</f>
+        <f>IF(Inputs!G21="Y", Prices!$C22, 0)</f>
         <v>0</v>
       </c>
       <c r="H64" s="20">
-        <f>IF(Inputs!H20="Y", Prices!$C22, 0)</f>
+        <f>IF(Inputs!H21="Y", Prices!$C22, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12934,107 +12948,107 @@
         <v>17</v>
       </c>
       <c r="D65" s="20">
-        <f>IF(Inputs!D21="Y", Prices!$C23, 0)</f>
+        <f>IF(Inputs!D22="Y", Prices!$C23, 0)</f>
         <v>28000</v>
       </c>
       <c r="E65" s="20">
-        <f>IF(Inputs!E21="Y", Prices!$C23, 0)</f>
+        <f>IF(Inputs!E22="Y", Prices!$C23, 0)</f>
         <v>0</v>
       </c>
       <c r="F65" s="20">
-        <f>IF(Inputs!F21="Y", Prices!$C23, 0)</f>
+        <f>IF(Inputs!F22="Y", Prices!$C23, 0)</f>
         <v>0</v>
       </c>
       <c r="G65" s="20">
-        <f>IF(Inputs!G21="Y", Prices!$C23, 0)</f>
+        <f>IF(Inputs!G22="Y", Prices!$C23, 0)</f>
         <v>0</v>
       </c>
       <c r="H65" s="20">
-        <f>IF(Inputs!H21="Y", Prices!$C23, 0)</f>
+        <f>IF(Inputs!H22="Y", Prices!$C23, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C66" s="19" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="D66" s="20">
-        <f>IF(Inputs!D22="Y", Prices!$C24 * IF(Inputs!D21="Y",1-Prices!$L$20,1), 0)</f>
+        <f>IF(Inputs!D23="Y", Prices!$C24 * IF(Inputs!D22="Y",1-Prices!$L$20,1), 0)</f>
         <v>23520</v>
       </c>
       <c r="E66" s="20">
-        <f>IF(Inputs!E22="Y", Prices!$C24 * IF(Inputs!E21="Y",1-Prices!$L$20,1), 0)</f>
+        <f>IF(Inputs!E23="Y", Prices!$C24 * IF(Inputs!E22="Y",1-Prices!$L$20,1), 0)</f>
         <v>0</v>
       </c>
       <c r="F66" s="20">
-        <f>IF(Inputs!F22="Y", Prices!$C24 * IF(Inputs!F21="Y",1-Prices!$L$20,1), 0)</f>
+        <f>IF(Inputs!F23="Y", Prices!$C24 * IF(Inputs!F22="Y",1-Prices!$L$20,1), 0)</f>
         <v>0</v>
       </c>
       <c r="G66" s="20">
-        <f>IF(Inputs!G22="Y", Prices!$C24 * IF(Inputs!G21="Y",1-Prices!$L$20,1), 0)</f>
+        <f>IF(Inputs!G23="Y", Prices!$C24 * IF(Inputs!G22="Y",1-Prices!$L$20,1), 0)</f>
         <v>0</v>
       </c>
       <c r="H66" s="20">
-        <f>IF(Inputs!H22="Y", Prices!$C24 * IF(Inputs!H21="Y",1-Prices!$L$20,1), 0)</f>
+        <f>IF(Inputs!H23="Y", Prices!$C24 * IF(Inputs!H22="Y",1-Prices!$L$20,1), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C67" s="19" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D67" s="20">
-        <f>IF(Inputs!D23="Y", Prices!$C25, 0)</f>
+        <f>IF(Inputs!D24="Y", Prices!$C25, 0)</f>
         <v>0</v>
       </c>
       <c r="E67" s="20">
-        <f>IF(Inputs!E23="Y", Prices!$C25, 0)</f>
+        <f>IF(Inputs!E24="Y", Prices!$C25, 0)</f>
         <v>0</v>
       </c>
       <c r="F67" s="20">
-        <f>IF(Inputs!F23="Y", Prices!$C25, 0)</f>
+        <f>IF(Inputs!F24="Y", Prices!$C25, 0)</f>
         <v>0</v>
       </c>
       <c r="G67" s="20">
-        <f>IF(Inputs!G23="Y", Prices!$C25, 0)</f>
+        <f>IF(Inputs!G24="Y", Prices!$C25, 0)</f>
         <v>0</v>
       </c>
       <c r="H67" s="20">
-        <f>IF(Inputs!H23="Y", Prices!$C25, 0)</f>
+        <f>IF(Inputs!H24="Y", Prices!$C25, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C68" s="81" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D68" s="84">
-        <f>IF(Inputs!D8="Y", Prices!$C26, 0)</f>
+        <f>IF(Inputs!D9="Y", Prices!$C26, 0)</f>
         <v>0</v>
       </c>
       <c r="E68" s="84">
-        <f>IF(Inputs!E8="Y", Prices!$C26, 0)</f>
+        <f>IF(Inputs!E9="Y", Prices!$C26, 0)</f>
         <v>0</v>
       </c>
       <c r="F68" s="84">
-        <f>IF(Inputs!F8="Y", Prices!$C26, 0)</f>
+        <f>IF(Inputs!F9="Y", Prices!$C26, 0)</f>
         <v>0</v>
       </c>
       <c r="G68" s="84">
-        <f>IF(Inputs!G8="Y", Prices!$C26, 0)</f>
+        <f>IF(Inputs!G9="Y", Prices!$C26, 0)</f>
         <v>0</v>
       </c>
       <c r="H68" s="84">
-        <f>IF(Inputs!H8="Y", Prices!$C26, 0)</f>
+        <f>IF(Inputs!H9="Y", Prices!$C26, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B70" s="6" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="J70" s="89" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
@@ -13085,23 +13099,23 @@
         <v>15</v>
       </c>
       <c r="D72" s="18">
-        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D19 = "Y", D$11*Prices!$E21, 0)))*D$10</f>
+        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D20 = "Y", D$11*Prices!$E21, 0)))*D$10</f>
         <v>0</v>
       </c>
       <c r="E72" s="18">
-        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E19 = "Y", E$11*Prices!$E21, 0)))*E$10</f>
+        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E20 = "Y", E$11*Prices!$E21, 0)))*E$10</f>
         <v>0</v>
       </c>
       <c r="F72" s="18">
-        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F19 = "Y", F$11*Prices!$E21, 0)))*F$10</f>
+        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F20 = "Y", F$11*Prices!$E21, 0)))*F$10</f>
         <v>0</v>
       </c>
       <c r="G72" s="18">
-        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G19 = "Y", G$11*Prices!$E21, 0)))*G$10</f>
+        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G20 = "Y", G$11*Prices!$E21, 0)))*G$10</f>
         <v>0</v>
       </c>
       <c r="H72" s="18">
-        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H19 = "Y", H$11*Prices!$E21, 0)))*H$10</f>
+        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H20 = "Y", H$11*Prices!$E21, 0)))*H$10</f>
         <v>0</v>
       </c>
       <c r="J72" s="90">
@@ -13134,23 +13148,23 @@
         <v>16</v>
       </c>
       <c r="D73" s="20">
-        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D20 = "Y", D$11*Prices!$E22, 0)))*D$10</f>
+        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D21 = "Y", D$11*Prices!$E22, 0)))*D$10</f>
         <v>0</v>
       </c>
       <c r="E73" s="20">
-        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E20 = "Y", E$11*Prices!$E22, 0)))*E$10</f>
+        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E21 = "Y", E$11*Prices!$E22, 0)))*E$10</f>
         <v>0</v>
       </c>
       <c r="F73" s="20">
-        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F20 = "Y", F$11*Prices!$E22, 0)))*F$10</f>
+        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F21 = "Y", F$11*Prices!$E22, 0)))*F$10</f>
         <v>0</v>
       </c>
       <c r="G73" s="20">
-        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G20 = "Y", G$11*Prices!$E22, 0)))*G$10</f>
+        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G21 = "Y", G$11*Prices!$E22, 0)))*G$10</f>
         <v>0</v>
       </c>
       <c r="H73" s="20">
-        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H20 = "Y", H$11*Prices!$E22, 0)))*H$10</f>
+        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H21 = "Y", H$11*Prices!$E22, 0)))*H$10</f>
         <v>0</v>
       </c>
       <c r="J73" s="90">
@@ -13183,23 +13197,23 @@
         <v>17</v>
       </c>
       <c r="D74" s="20">
-        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D21 = "Y", D$11*Prices!$E23, 0)))*D$10</f>
+        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D22 = "Y", D$11*Prices!$E23, 0)))*D$10</f>
         <v>0</v>
       </c>
       <c r="E74" s="20">
-        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E21 = "Y", E$11*Prices!$E23, 0)))*E$10</f>
+        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E22 = "Y", E$11*Prices!$E23, 0)))*E$10</f>
         <v>0</v>
       </c>
       <c r="F74" s="20">
-        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F21 = "Y", F$11*Prices!$E23, 0)))*F$10</f>
+        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F22 = "Y", F$11*Prices!$E23, 0)))*F$10</f>
         <v>0</v>
       </c>
       <c r="G74" s="20">
-        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G21 = "Y", G$11*Prices!$E23, 0)))*G$10</f>
+        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G22 = "Y", G$11*Prices!$E23, 0)))*G$10</f>
         <v>0</v>
       </c>
       <c r="H74" s="20">
-        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H21 = "Y", H$11*Prices!$E23, 0)))*H$10</f>
+        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H22 = "Y", H$11*Prices!$E23, 0)))*H$10</f>
         <v>0</v>
       </c>
       <c r="J74" s="90">
@@ -13229,26 +13243,26 @@
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C75" s="19" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="D75" s="20">
-        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D22 = "Y", D$11*Prices!$E24 * IF(Inputs!D21="Y",1-Prices!$L$20,1), 0)))*D$10</f>
+        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D23 = "Y", D$11*Prices!$E24 * IF(Inputs!D22="Y",1-Prices!$L$20,1), 0)))*D$10</f>
         <v>0</v>
       </c>
       <c r="E75" s="20">
-        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E22 = "Y", E$11*Prices!$E24 * IF(Inputs!E21="Y",1-Prices!$L$20,1), 0)))*E$10</f>
+        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E23 = "Y", E$11*Prices!$E24 * IF(Inputs!E22="Y",1-Prices!$L$20,1), 0)))*E$10</f>
         <v>0</v>
       </c>
       <c r="F75" s="20">
-        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F22 = "Y", F$11*Prices!$E24 * IF(Inputs!F21="Y",1-Prices!$L$20,1), 0)))*F$10</f>
+        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F23 = "Y", F$11*Prices!$E24 * IF(Inputs!F22="Y",1-Prices!$L$20,1), 0)))*F$10</f>
         <v>0</v>
       </c>
       <c r="G75" s="20">
-        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G22 = "Y", G$11*Prices!$E24 * IF(Inputs!G21="Y",1-Prices!$L$20,1), 0)))*G$10</f>
+        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G23 = "Y", G$11*Prices!$E24 * IF(Inputs!G22="Y",1-Prices!$L$20,1), 0)))*G$10</f>
         <v>0</v>
       </c>
       <c r="H75" s="20">
-        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H22 = "Y", H$11*Prices!$E24 * IF(Inputs!H21="Y",1-Prices!$L$20,1), 0)))*H$10</f>
+        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H23 = "Y", H$11*Prices!$E24 * IF(Inputs!H22="Y",1-Prices!$L$20,1), 0)))*H$10</f>
         <v>0</v>
       </c>
       <c r="J75" s="90">
@@ -13278,26 +13292,26 @@
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C76" s="19" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D76" s="20">
-        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D23 = "Y", D$11*Prices!$E25, 0)))*D$10</f>
+        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D24 = "Y", D$11*Prices!$E25, 0)))*D$10</f>
         <v>0</v>
       </c>
       <c r="E76" s="20">
-        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E23 = "Y", E$11*Prices!$E25, 0)))*E$10</f>
+        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E24 = "Y", E$11*Prices!$E25, 0)))*E$10</f>
         <v>0</v>
       </c>
       <c r="F76" s="20">
-        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F23 = "Y", F$11*Prices!$E25, 0)))*F$10</f>
+        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F24 = "Y", F$11*Prices!$E25, 0)))*F$10</f>
         <v>0</v>
       </c>
       <c r="G76" s="20">
-        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G23 = "Y", G$11*Prices!$E25, 0)))*G$10</f>
+        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G24 = "Y", G$11*Prices!$E25, 0)))*G$10</f>
         <v>0</v>
       </c>
       <c r="H76" s="20">
-        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H23 = "Y", H$11*Prices!$E25, 0)))*H$10</f>
+        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H24 = "Y", H$11*Prices!$E25, 0)))*H$10</f>
         <v>0</v>
       </c>
       <c r="J76" s="90">
@@ -13327,26 +13341,26 @@
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C77" s="81" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D77" s="84">
-        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D8 = "Y", D$11*Prices!$E26, 0)))*D$10</f>
+        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D9 = "Y", D$11*Prices!$E26, 0)))*D$10</f>
         <v>0</v>
       </c>
       <c r="E77" s="84">
-        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E8 = "Y", E$11*Prices!$E26, 0)))*E$10</f>
+        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E9 = "Y", E$11*Prices!$E26, 0)))*E$10</f>
         <v>0</v>
       </c>
       <c r="F77" s="84">
-        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F8 = "Y", F$11*Prices!$E26, 0)))*F$10</f>
+        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F9 = "Y", F$11*Prices!$E26, 0)))*F$10</f>
         <v>0</v>
       </c>
       <c r="G77" s="84">
-        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G8 = "Y", G$11*Prices!$E26, 0)))*G$10</f>
+        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G9 = "Y", G$11*Prices!$E26, 0)))*G$10</f>
         <v>0</v>
       </c>
       <c r="H77" s="84">
-        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H8 = "Y", H$11*Prices!$E26, 0)))*H$10</f>
+        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H9 = "Y", H$11*Prices!$E26, 0)))*H$10</f>
         <v>0</v>
       </c>
       <c r="J77" s="90">
@@ -13383,7 +13397,7 @@
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B79" s="6" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
@@ -13568,7 +13582,7 @@
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C84" s="19" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="D84" s="20">
         <f t="shared" ref="D84:H84" si="15">D66</f>
@@ -13613,7 +13627,7 @@
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C85" s="19" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D85" s="20">
         <f t="shared" ref="D85:H85" si="17">D67</f>
@@ -13658,7 +13672,7 @@
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C86" s="81" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D86" s="84">
         <f t="shared" ref="D86:H86" si="19">D68</f>
@@ -13703,7 +13717,7 @@
     </row>
     <row r="88" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B88" s="6" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.25">
@@ -13803,7 +13817,7 @@
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C93" s="19" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="D93" s="20">
         <f t="shared" ref="D93:H93" si="21">D75</f>
@@ -13828,7 +13842,7 @@
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C94" s="19" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D94" s="20">
         <f t="shared" ref="D94:H94" si="22">D76</f>
@@ -13853,7 +13867,7 @@
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C95" s="81" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D95" s="84">
         <f t="shared" ref="D95:H95" si="23">D77</f>
@@ -13878,7 +13892,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B97" s="6" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -13886,7 +13900,7 @@
         <v>2</v>
       </c>
       <c r="C98" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D98" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$62:D$68, MATCH($A98, K$80:K$86, 0)), INDEX(D$71:D$77, MATCH($A98, K$80:K$86, 0)))*Prices!$L$5*-1, 0)</f>
@@ -13914,7 +13928,7 @@
         <v>3</v>
       </c>
       <c r="C99" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D99" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$62:D$68, MATCH($A99, K$80:K$86, 0)), INDEX(D$71:D$77, MATCH($A99, K$80:K$86, 0)))*Prices!$L$6*-1, 0)</f>
@@ -13942,7 +13956,7 @@
         <v>4</v>
       </c>
       <c r="C100" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="D100" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$62:D$68, MATCH($A100, K$80:K$86, 0)), INDEX(D$71:D$77, MATCH($A100, K$80:K$86, 0)))*Prices!$L$6*-1, 0)</f>
@@ -13970,7 +13984,7 @@
         <v>5</v>
       </c>
       <c r="C101" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D101" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$62:D$68, MATCH($A101, K$80:K$86, 0)), INDEX(D$71:D$77, MATCH($A101, K$80:K$86, 0)))*Prices!$L$6*-1, 0)</f>
@@ -13998,7 +14012,7 @@
         <v>6</v>
       </c>
       <c r="C102" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="D102" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$62:D$68, MATCH($A102, K$80:K$86, 0)), INDEX(D$71:D$77, MATCH($A102, K$80:K$86, 0)))*Prices!$L$6*-1, 0)</f>
@@ -14023,7 +14037,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B104" s="6" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="D104" s="7">
         <f>SUM(D38:D47, D50:D59, D62:D68, D71:D77, D98:D102)</f>
@@ -14051,7 +14065,7 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B106" s="6" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D106" s="1">
         <f>IF(D116=1, 0, IF(D116=2, $E$119, IF(D116=3, $E$120, IF(D116=4, $E$121, IF(D116=5, $E$122, "")))))</f>
@@ -14083,7 +14097,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B108" s="6" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D108" s="1">
         <f>IF(Inputs!$D$5 = "Y", Prices!$L$18, 0)*-1</f>
@@ -14104,7 +14118,7 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B110" s="6" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="D110" s="7">
         <f>SUM(D104, D106)</f>
@@ -14130,7 +14144,7 @@
     <row r="113" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B113" s="27"/>
       <c r="C113" s="21" t="s">
-        <v>59</v>
+        <v>117</v>
       </c>
       <c r="D113" s="21">
         <f>IFERROR(_xlfn.RANK.EQ(D104,$D$104:$H$104),5)</f>
@@ -14223,13 +14237,13 @@
     <row r="118" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B118" s="27"/>
       <c r="C118" s="21" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
     </row>
     <row r="119" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B119" s="27"/>
       <c r="D119" s="21" t="s">
-        <v>36</v>
+        <v>119</v>
       </c>
       <c r="E119" s="23">
         <f>INDEX($D$104:$H$104, 1, MATCH(2, $D$116:$H$116, 0))*Prices!$L$10*-1</f>
@@ -14239,7 +14253,7 @@
     <row r="120" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B120" s="27"/>
       <c r="D120" s="21" t="s">
-        <v>37</v>
+        <v>120</v>
       </c>
       <c r="E120" s="23">
         <f>INDEX($D$104:$H$104, 1, MATCH(3, $D$116:$H$116, 0))*Prices!$L$11*-1</f>
@@ -14249,7 +14263,7 @@
     <row r="121" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B121" s="27"/>
       <c r="D121" s="21" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="E121" s="23">
         <f>INDEX($D$104:$H$104, 1, MATCH(4, $D$116:$H$116, 0))*Prices!$L$11*-1</f>
@@ -14259,7 +14273,7 @@
     <row r="122" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B122" s="27"/>
       <c r="D122" s="21" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
       <c r="E122" s="23">
         <f>INDEX($D$104:$H$104, 1, MATCH(5, $D$116:$H$116, 0))*Prices!$L$11*-1</f>
@@ -14279,7 +14293,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14299,30 +14315,30 @@
         <v>5</v>
       </c>
       <c r="D2" s="48" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>23</v>
+        <v>114</v>
       </c>
       <c r="C3" s="1">
         <v>5000</v>
       </c>
       <c r="D3" s="1">
-        <v>32750</v>
+        <v>20000</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="K3" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1">
         <v>5000</v>
@@ -14331,7 +14347,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="F4" s="76">
         <v>0.6</v>
@@ -14343,7 +14359,7 @@
         <v>0.2</v>
       </c>
       <c r="K4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="L4" s="3">
         <v>0</v>
@@ -14351,19 +14367,19 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E5" s="48" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="F5" s="48" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="G5" s="48" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="H5" s="48" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L5" s="3">
         <v>0.3</v>
@@ -14371,7 +14387,7 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C6" s="42">
         <v>15000</v>
@@ -14395,7 +14411,7 @@
         <v>5.4000000000000006E-2</v>
       </c>
       <c r="K6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="L6" s="3">
         <v>0.45</v>
@@ -14405,19 +14421,19 @@
       <c r="C8" s="43"/>
       <c r="D8" s="39"/>
       <c r="K8" s="6" t="s">
-        <v>35</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C9" s="46" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E9" s="47"/>
       <c r="F9" s="47"/>
       <c r="G9" s="47"/>
       <c r="H9" s="47"/>
       <c r="K9" t="s">
-        <v>34</v>
+        <v>123</v>
       </c>
       <c r="L9" s="3">
         <v>0</v>
@@ -14425,7 +14441,7 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C10" s="44">
         <v>1000</v>
@@ -14446,7 +14462,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="K10" t="s">
-        <v>36</v>
+        <v>119</v>
       </c>
       <c r="L10" s="3">
         <v>0.45</v>
@@ -14475,7 +14491,7 @@
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="K11" t="s">
-        <v>37</v>
+        <v>120</v>
       </c>
       <c r="L11" s="3">
         <v>0.5</v>
@@ -14483,7 +14499,7 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C12" s="44">
         <v>2000</v>
@@ -14551,7 +14567,7 @@
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="K14" s="58" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="L14" s="57">
         <v>1.2500000000000001E-2</v>
@@ -14559,7 +14575,7 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C15" s="44">
         <v>4000</v>
@@ -14580,7 +14596,7 @@
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="L15" s="54">
         <v>43466</v>
@@ -14636,7 +14652,7 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C18" s="45">
         <v>5000</v>
@@ -14657,7 +14673,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="L18" s="1">
         <v>3525</v>
@@ -14693,7 +14709,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="L20" s="3">
         <v>0.3</v>
@@ -14770,7 +14786,7 @@
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="19" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C24" s="45">
         <v>33600</v>
@@ -14793,7 +14809,7 @@
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="19" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="C25" s="45">
         <v>20000</v>
@@ -14816,7 +14832,7 @@
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="81" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="C26" s="82">
         <v>6750</v>

</xml_diff>

<commit_message>
Start work on abstracting to Monthly and Quarterly.
Do this because it's silly to have two files at this point.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Quarterly_Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Quarterly_Premier_Pricing_Model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890"/>
+    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Prices" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="ACOInsight1">Inputs!$D$19:$D$20</definedName>
+    <definedName name="ACOInsight1">Inputs!$D$20:$D$21</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Outputs_Internal!$B$1:$M$60</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="129">
   <si>
     <t>One-Time Fees:</t>
   </si>
@@ -443,6 +443,18 @@
   <si>
     <t>Multi-Population Discounts</t>
   </si>
+  <si>
+    <t>Monthly or Quarterly?</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Quarterly</t>
+  </si>
+  <si>
+    <t>Monthly Multiplier</t>
+  </si>
 </sst>
 </file>
 
@@ -714,7 +726,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -879,6 +891,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1173,13 +1186,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L24"/>
+  <dimension ref="B1:L25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M11" sqref="M11"/>
+      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,7 +1201,7 @@
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
     <col min="3" max="3" width="18" style="66" customWidth="1"/>
     <col min="4" max="8" width="18.7109375" customWidth="1"/>
-    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
     <col min="12" max="12" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1209,47 +1222,38 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="68"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="13" t="s">
+      <c r="B3" s="67" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="68"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F4" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G4" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H4" s="14" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="69" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="56"/>
-      <c r="L4" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="69" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="D5" s="55" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E5" s="55" t="s">
         <v>29</v>
@@ -1258,15 +1262,15 @@
       <c r="G5" s="55"/>
       <c r="H5" s="56"/>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="69" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="D6" s="55" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E6" s="55" t="s">
         <v>29</v>
@@ -1274,16 +1278,19 @@
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
       <c r="H6" s="56"/>
+      <c r="L6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="69" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="55">
-        <v>250000</v>
-      </c>
-      <c r="E7" s="55">
-        <v>250000</v>
+        <v>6</v>
+      </c>
+      <c r="D7" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>29</v>
       </c>
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
@@ -1291,35 +1298,41 @@
     </row>
     <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="69" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
       <c r="D8" s="55">
-        <v>1</v>
+        <v>250000</v>
       </c>
       <c r="E8" s="55">
-        <v>3</v>
+        <v>250000</v>
       </c>
       <c r="F8" s="55"/>
       <c r="G8" s="55"/>
       <c r="H8" s="56"/>
+      <c r="L8" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="69" t="s">
-        <v>100</v>
-      </c>
-      <c r="D9" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="55" t="s">
-        <v>29</v>
+        <v>113</v>
+      </c>
+      <c r="D9" s="55">
+        <v>1</v>
+      </c>
+      <c r="E9" s="55">
+        <v>3</v>
       </c>
       <c r="F9" s="55"/>
       <c r="G9" s="55"/>
       <c r="H9" s="56"/>
+      <c r="L9" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="69" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="D10" s="55" t="s">
         <v>29</v>
@@ -1333,7 +1346,7 @@
     </row>
     <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="69" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="55" t="s">
         <v>29</v>
@@ -1347,7 +1360,7 @@
     </row>
     <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="69" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D12" s="55" t="s">
         <v>29</v>
@@ -1361,7 +1374,7 @@
     </row>
     <row r="13" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="69" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D13" s="55" t="s">
         <v>29</v>
@@ -1375,7 +1388,7 @@
     </row>
     <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" s="55" t="s">
         <v>29</v>
@@ -1389,7 +1402,7 @@
     </row>
     <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="69" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="D15" s="55" t="s">
         <v>29</v>
@@ -1403,7 +1416,7 @@
     </row>
     <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="69" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="D16" s="55" t="s">
         <v>29</v>
@@ -1417,7 +1430,7 @@
     </row>
     <row r="17" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="69" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" s="55" t="s">
         <v>29</v>
@@ -1431,7 +1444,7 @@
     </row>
     <row r="18" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="69" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" s="55" t="s">
         <v>29</v>
@@ -1445,7 +1458,7 @@
     </row>
     <row r="19" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="55" t="s">
         <v>29</v>
@@ -1459,7 +1472,7 @@
     </row>
     <row r="20" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="69" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" s="55" t="s">
         <v>29</v>
@@ -1473,7 +1486,7 @@
     </row>
     <row r="21" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="69" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" s="55" t="s">
         <v>29</v>
@@ -1487,10 +1500,10 @@
     </row>
     <row r="22" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" s="55" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E22" s="55" t="s">
         <v>29</v>
@@ -1501,7 +1514,7 @@
     </row>
     <row r="23" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="69" t="s">
-        <v>102</v>
+        <v>17</v>
       </c>
       <c r="D23" s="55" t="s">
         <v>3</v>
@@ -1514,27 +1527,44 @@
       <c r="H23" s="56"/>
     </row>
     <row r="24" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="92" t="s">
+      <c r="B24" s="69" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="56"/>
+    </row>
+    <row r="25" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="92" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="93"/>
-      <c r="D24" s="94" t="s">
+      <c r="C25" s="93"/>
+      <c r="D25" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="94" t="s">
+      <c r="E25" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="94"/>
-      <c r="G24" s="94"/>
-      <c r="H24" s="95"/>
+      <c r="F25" s="94"/>
+      <c r="G25" s="94"/>
+      <c r="H25" s="95"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:H22 D23:D24 D4:H6">
-      <formula1>$L$4:$L$5</formula1>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:H23 D5:H7 D24:D25">
+      <formula1>$L$5:$L$6</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:H8">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:H9">
       <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+      <formula1>$L$8:$L$9</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2585,7 +2615,7 @@
         <v>77</v>
       </c>
       <c r="D4" s="1">
-        <f>SUMIF(Inputs!$D$4:$H$4, "Y", Outputs_External!D4:'Outputs_External'!H4)</f>
+        <f>SUMIF(Inputs!$D$5:$H$5, "Y", Outputs_External!D4:'Outputs_External'!H4)</f>
         <v>10000</v>
       </c>
       <c r="E4" s="3"/>
@@ -2624,7 +2654,7 @@
         <v>78</v>
       </c>
       <c r="D5" s="1">
-        <f>SUMIF(Inputs!$D$4:$H$4, "N", Outputs_External!D4:'Outputs_External'!H4)</f>
+        <f>SUMIF(Inputs!$D$5:$H$5, "N", Outputs_External!D4:'Outputs_External'!H4)</f>
         <v>60000</v>
       </c>
       <c r="E5" s="3"/>
@@ -11614,23 +11644,23 @@
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <f>IF(AND(Inputs!D5="Y",Inputs!D4="Y"), 0, IF(Inputs!D4="Y", SUM(Prices!$C$3, IF(Inputs!D$6 ="Y", Prices!$C$4, 0)), IF(Inputs!D4="N", Prices!$D$3, 0)))*Inputs!D8</f>
+        <f>IF(AND(Inputs!D6="Y",Inputs!D5="Y"), 0, IF(Inputs!D5="Y", SUM(Prices!$C$3, IF(Inputs!D$7 ="Y", Prices!$C$4, 0)), IF(Inputs!D5="N", Prices!$D$3, 0)))*Inputs!D9</f>
         <v>10000</v>
       </c>
       <c r="E4" s="1">
-        <f>IF(AND(Inputs!E5="Y",Inputs!E4="Y"), 0, IF(Inputs!E4="Y", SUM(Prices!$C$3, IF(Inputs!E$6 ="Y", Prices!$C$4, 0)), IF(Inputs!E4="N", Prices!$D$3, 0)))*Inputs!E8</f>
+        <f>IF(AND(Inputs!E6="Y",Inputs!E5="Y"), 0, IF(Inputs!E5="Y", SUM(Prices!$C$3, IF(Inputs!E$7 ="Y", Prices!$C$4, 0)), IF(Inputs!E5="N", Prices!$D$3, 0)))*Inputs!E9</f>
         <v>60000</v>
       </c>
       <c r="F4" s="1">
-        <f>IF(AND(Inputs!F5="Y",Inputs!F4="Y"), 0, IF(Inputs!F4="Y", SUM(Prices!$C$3, IF(Inputs!F$6 ="Y", Prices!$C$4, 0)), IF(Inputs!F4="N", Prices!$D$3, 0)))*Inputs!F8</f>
+        <f>IF(AND(Inputs!F6="Y",Inputs!F5="Y"), 0, IF(Inputs!F5="Y", SUM(Prices!$C$3, IF(Inputs!F$7 ="Y", Prices!$C$4, 0)), IF(Inputs!F5="N", Prices!$D$3, 0)))*Inputs!F9</f>
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <f>IF(AND(Inputs!G5="Y",Inputs!G4="Y"), 0, IF(Inputs!G4="Y", SUM(Prices!$C$3, IF(Inputs!G$6 ="Y", Prices!$C$4, 0)), IF(Inputs!G4="N", Prices!$D$3, 0)))*Inputs!G8</f>
+        <f>IF(AND(Inputs!G6="Y",Inputs!G5="Y"), 0, IF(Inputs!G5="Y", SUM(Prices!$C$3, IF(Inputs!G$7 ="Y", Prices!$C$4, 0)), IF(Inputs!G5="N", Prices!$D$3, 0)))*Inputs!G9</f>
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <f>IF(AND(Inputs!H5="Y",Inputs!H4="Y"), 0, IF(Inputs!H4="Y", SUM(Prices!$C$3, IF(Inputs!H$6 ="Y", Prices!$C$4, 0)), IF(Inputs!H4="N", Prices!$D$3, 0)))*Inputs!H8</f>
+        <f>IF(AND(Inputs!H6="Y",Inputs!H5="Y"), 0, IF(Inputs!H5="Y", SUM(Prices!$C$3, IF(Inputs!H$7 ="Y", Prices!$C$4, 0)), IF(Inputs!H5="N", Prices!$D$3, 0)))*Inputs!H9</f>
         <v>0</v>
       </c>
     </row>
@@ -11655,23 +11685,23 @@
         <v>89</v>
       </c>
       <c r="D6" s="5">
-        <f>IF(Inputs!D$4="N",MIN(MAX(Inputs!D$7-$K6,0),$L6-$K6),0)</f>
+        <f>IF(Inputs!D$5="N",MIN(MAX(Inputs!D$8-$K6,0),$L6-$K6),0)</f>
         <v>0</v>
       </c>
       <c r="E6" s="5">
-        <f>IF(Inputs!E$4="N",MIN(MAX(Inputs!E$7-$K6,0),$L6-$K6),0)</f>
+        <f>IF(Inputs!E$5="N",MIN(MAX(Inputs!E$8-$K6,0),$L6-$K6),0)</f>
         <v>25000</v>
       </c>
       <c r="F6" s="5">
-        <f>IF(Inputs!F$4="N",MIN(MAX(Inputs!F$7-$K6,0),$L6-$K6),0)</f>
+        <f>IF(Inputs!F$5="N",MIN(MAX(Inputs!F$8-$K6,0),$L6-$K6),0)</f>
         <v>0</v>
       </c>
       <c r="G6" s="5">
-        <f>IF(Inputs!G$4="N",MIN(MAX(Inputs!G$7-$K6,0),$L6-$K6),0)</f>
+        <f>IF(Inputs!G$5="N",MIN(MAX(Inputs!G$8-$K6,0),$L6-$K6),0)</f>
         <v>0</v>
       </c>
       <c r="H6" s="5">
-        <f>IF(Inputs!H$4="N",MIN(MAX(Inputs!H$7-$K6,0),$L6-$K6),0)</f>
+        <f>IF(Inputs!H$5="N",MIN(MAX(Inputs!H$8-$K6,0),$L6-$K6),0)</f>
         <v>0</v>
       </c>
       <c r="K6" s="65">
@@ -11689,23 +11719,23 @@
         <v>90</v>
       </c>
       <c r="D7" s="5">
-        <f>IF(Inputs!D$4="N",MIN(MAX(Inputs!D$7-$K7,0),$L7-$K7),0)</f>
+        <f>IF(Inputs!D$5="N",MIN(MAX(Inputs!D$8-$K7,0),$L7-$K7),0)</f>
         <v>0</v>
       </c>
       <c r="E7" s="5">
-        <f>IF(Inputs!E$4="N",MIN(MAX(Inputs!E$7-$K7,0),$L7-$K7),0)</f>
+        <f>IF(Inputs!E$5="N",MIN(MAX(Inputs!E$8-$K7,0),$L7-$K7),0)</f>
         <v>50000</v>
       </c>
       <c r="F7" s="5">
-        <f>IF(Inputs!F$4="N",MIN(MAX(Inputs!F$7-$K7,0),$L7-$K7),0)</f>
+        <f>IF(Inputs!F$5="N",MIN(MAX(Inputs!F$8-$K7,0),$L7-$K7),0)</f>
         <v>0</v>
       </c>
       <c r="G7" s="5">
-        <f>IF(Inputs!G$4="N",MIN(MAX(Inputs!G$7-$K7,0),$L7-$K7),0)</f>
+        <f>IF(Inputs!G$5="N",MIN(MAX(Inputs!G$8-$K7,0),$L7-$K7),0)</f>
         <v>0</v>
       </c>
       <c r="H7" s="5">
-        <f>IF(Inputs!H$4="N",MIN(MAX(Inputs!H$7-$K7,0),$L7-$K7),0)</f>
+        <f>IF(Inputs!H$5="N",MIN(MAX(Inputs!H$8-$K7,0),$L7-$K7),0)</f>
         <v>0</v>
       </c>
       <c r="K7" s="65">
@@ -11724,23 +11754,23 @@
         <v>91</v>
       </c>
       <c r="D8" s="5">
-        <f>IF(Inputs!D$4="N",MIN(MAX(Inputs!D$7-$K8,0),$L8-$K8),0)</f>
+        <f>IF(Inputs!D$5="N",MIN(MAX(Inputs!D$8-$K8,0),$L8-$K8),0)</f>
         <v>0</v>
       </c>
       <c r="E8" s="5">
-        <f>IF(Inputs!E$4="N",MIN(MAX(Inputs!E$7-$K8,0),$L8-$K8),0)</f>
+        <f>IF(Inputs!E$5="N",MIN(MAX(Inputs!E$8-$K8,0),$L8-$K8),0)</f>
         <v>150000</v>
       </c>
       <c r="F8" s="5">
-        <f>IF(Inputs!F$4="N",MIN(MAX(Inputs!F$7-$K8,0),$L8-$K8),0)</f>
+        <f>IF(Inputs!F$5="N",MIN(MAX(Inputs!F$8-$K8,0),$L8-$K8),0)</f>
         <v>0</v>
       </c>
       <c r="G8" s="5">
-        <f>IF(Inputs!G$4="N",MIN(MAX(Inputs!G$7-$K8,0),$L8-$K8),0)</f>
+        <f>IF(Inputs!G$5="N",MIN(MAX(Inputs!G$8-$K8,0),$L8-$K8),0)</f>
         <v>0</v>
       </c>
       <c r="H8" s="5">
-        <f>IF(Inputs!H$4="N",MIN(MAX(Inputs!H$7-$K8,0),$L8-$K8),0)</f>
+        <f>IF(Inputs!H$5="N",MIN(MAX(Inputs!H$8-$K8,0),$L8-$K8),0)</f>
         <v>0</v>
       </c>
       <c r="K8" s="65">
@@ -11759,23 +11789,23 @@
         <v>93</v>
       </c>
       <c r="D9" s="5">
-        <f>IF(Inputs!D$4="N",MIN(MAX(Inputs!D$7-$K9,0),$L9-$K9),0)</f>
+        <f>IF(Inputs!D$5="N",MIN(MAX(Inputs!D$8-$K9,0),$L9-$K9),0)</f>
         <v>0</v>
       </c>
       <c r="E9" s="5">
-        <f>IF(Inputs!E$4="N",MIN(MAX(Inputs!E$7-$K9,0),$L9-$K9),0)</f>
+        <f>IF(Inputs!E$5="N",MIN(MAX(Inputs!E$8-$K9,0),$L9-$K9),0)</f>
         <v>0</v>
       </c>
       <c r="F9" s="5">
-        <f>IF(Inputs!F$4="N",MIN(MAX(Inputs!F$7-$K9,0),$L9-$K9),0)</f>
+        <f>IF(Inputs!F$5="N",MIN(MAX(Inputs!F$8-$K9,0),$L9-$K9),0)</f>
         <v>0</v>
       </c>
       <c r="G9" s="5">
-        <f>IF(Inputs!G$4="N",MIN(MAX(Inputs!G$7-$K9,0),$L9-$K9),0)</f>
+        <f>IF(Inputs!G$5="N",MIN(MAX(Inputs!G$8-$K9,0),$L9-$K9),0)</f>
         <v>0</v>
       </c>
       <c r="H9" s="5">
-        <f>IF(Inputs!H$4="N",MIN(MAX(Inputs!H$7-$K9,0),$L9-$K9),0)</f>
+        <f>IF(Inputs!H$5="N",MIN(MAX(Inputs!H$8-$K9,0),$L9-$K9),0)</f>
         <v>0</v>
       </c>
       <c r="K9" s="65">
@@ -11856,23 +11886,23 @@
         <v>2</v>
       </c>
       <c r="D14" s="16">
-        <f>IF(Inputs!D4="Y", Prices!$C$6, IF(Inputs!D4="N", Prices!$D$6, 0))</f>
+        <f>IF(Inputs!D5="Y", Prices!$C$6, IF(Inputs!D5="N", Prices!$D$6, 0))</f>
         <v>15000</v>
       </c>
       <c r="E14" s="16">
-        <f>IF(Inputs!E4="Y", Prices!$C$6, IF(Inputs!E4="N", Prices!$D$6, 0))</f>
+        <f>IF(Inputs!E5="Y", Prices!$C$6, IF(Inputs!E5="N", Prices!$D$6, 0))</f>
         <v>30000</v>
       </c>
       <c r="F14" s="16">
-        <f>IF(Inputs!F4="Y", Prices!$C$6, IF(Inputs!F4="N", Prices!$D$6, 0))</f>
+        <f>IF(Inputs!F5="Y", Prices!$C$6, IF(Inputs!F5="N", Prices!$D$6, 0))</f>
         <v>0</v>
       </c>
       <c r="G14" s="16">
-        <f>IF(Inputs!G4="Y", Prices!$C$6, IF(Inputs!G4="N", Prices!$D$6, 0))</f>
+        <f>IF(Inputs!G5="Y", Prices!$C$6, IF(Inputs!G5="N", Prices!$D$6, 0))</f>
         <v>0</v>
       </c>
       <c r="H14" s="16">
-        <f>IF(Inputs!H4="Y", Prices!$C$6, IF(Inputs!H4="N", Prices!$D$6, 0))</f>
+        <f>IF(Inputs!H5="Y", Prices!$C$6, IF(Inputs!H5="N", Prices!$D$6, 0))</f>
         <v>0</v>
       </c>
     </row>
@@ -11881,23 +11911,23 @@
         <v>21</v>
       </c>
       <c r="D15" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!D10="Y",Inputs!D$20="Y"), Prices!$C10, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D11="Y",Inputs!D$21="Y"), Prices!$C10, 0)</f>
         <v>0</v>
       </c>
       <c r="E15" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!E10="Y",Inputs!E$20="Y"), Prices!$C10, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E11="Y",Inputs!E$21="Y"), Prices!$C10, 0)</f>
         <v>0</v>
       </c>
       <c r="F15" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!F10="Y",Inputs!F$20="Y"), Prices!$C10, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F11="Y",Inputs!F$21="Y"), Prices!$C10, 0)</f>
         <v>0</v>
       </c>
       <c r="G15" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!G10="Y",Inputs!G$20="Y"), Prices!$C10, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G11="Y",Inputs!G$21="Y"), Prices!$C10, 0)</f>
         <v>0</v>
       </c>
       <c r="H15" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!H10="Y",Inputs!H$20="Y"), Prices!$C10, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H11="Y",Inputs!H$21="Y"), Prices!$C10, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11906,23 +11936,23 @@
         <v>8</v>
       </c>
       <c r="D16" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!D11="Y",Inputs!D$20="Y"), Prices!$C11, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D12="Y",Inputs!D$21="Y"), Prices!$C11, 0)</f>
         <v>0</v>
       </c>
       <c r="E16" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!E11="Y",Inputs!E$20="Y"), Prices!$C11, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E12="Y",Inputs!E$21="Y"), Prices!$C11, 0)</f>
         <v>0</v>
       </c>
       <c r="F16" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!F11="Y",Inputs!F$20="Y"), Prices!$C11, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F12="Y",Inputs!F$21="Y"), Prices!$C11, 0)</f>
         <v>0</v>
       </c>
       <c r="G16" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!G11="Y",Inputs!G$20="Y"), Prices!$C11, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G12="Y",Inputs!G$21="Y"), Prices!$C11, 0)</f>
         <v>0</v>
       </c>
       <c r="H16" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!H11="Y",Inputs!H$20="Y"), Prices!$C11, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H12="Y",Inputs!H$21="Y"), Prices!$C11, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11931,23 +11961,23 @@
         <v>22</v>
       </c>
       <c r="D17" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!D12="Y",Inputs!D$20="Y"), Prices!$C12, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D13="Y",Inputs!D$21="Y"), Prices!$C12, 0)</f>
         <v>0</v>
       </c>
       <c r="E17" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!E12="Y",Inputs!E$20="Y"), Prices!$C12, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E13="Y",Inputs!E$21="Y"), Prices!$C12, 0)</f>
         <v>0</v>
       </c>
       <c r="F17" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!F12="Y",Inputs!F$20="Y"), Prices!$C12, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F13="Y",Inputs!F$21="Y"), Prices!$C12, 0)</f>
         <v>0</v>
       </c>
       <c r="G17" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!G12="Y",Inputs!G$20="Y"), Prices!$C12, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G13="Y",Inputs!G$21="Y"), Prices!$C12, 0)</f>
         <v>0</v>
       </c>
       <c r="H17" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!H12="Y",Inputs!H$20="Y"), Prices!$C12, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H13="Y",Inputs!H$21="Y"), Prices!$C12, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11956,23 +11986,23 @@
         <v>9</v>
       </c>
       <c r="D18" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!D13="Y",Inputs!D$20="Y"), Prices!$C13, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D14="Y",Inputs!D$21="Y"), Prices!$C13, 0)</f>
         <v>0</v>
       </c>
       <c r="E18" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!E13="Y",Inputs!E$20="Y"), Prices!$C13, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E14="Y",Inputs!E$21="Y"), Prices!$C13, 0)</f>
         <v>0</v>
       </c>
       <c r="F18" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!F13="Y",Inputs!F$20="Y"), Prices!$C13, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F14="Y",Inputs!F$21="Y"), Prices!$C13, 0)</f>
         <v>0</v>
       </c>
       <c r="G18" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!G13="Y",Inputs!G$20="Y"), Prices!$C13, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G14="Y",Inputs!G$21="Y"), Prices!$C13, 0)</f>
         <v>0</v>
       </c>
       <c r="H18" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!H13="Y",Inputs!H$20="Y"), Prices!$C13, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H14="Y",Inputs!H$21="Y"), Prices!$C13, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -11981,23 +12011,23 @@
         <v>10</v>
       </c>
       <c r="D19" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!D14="Y",Inputs!D$20="Y"), Prices!$C14, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D15="Y",Inputs!D$21="Y"), Prices!$C14, 0)</f>
         <v>0</v>
       </c>
       <c r="E19" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!E14="Y",Inputs!E$20="Y"), Prices!$C14, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E15="Y",Inputs!E$21="Y"), Prices!$C14, 0)</f>
         <v>0</v>
       </c>
       <c r="F19" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!F14="Y",Inputs!F$20="Y"), Prices!$C14, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F15="Y",Inputs!F$21="Y"), Prices!$C14, 0)</f>
         <v>0</v>
       </c>
       <c r="G19" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!G14="Y",Inputs!G$20="Y"), Prices!$C14, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G15="Y",Inputs!G$21="Y"), Prices!$C14, 0)</f>
         <v>0</v>
       </c>
       <c r="H19" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!H14="Y",Inputs!H$20="Y"), Prices!$C14, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H15="Y",Inputs!H$21="Y"), Prices!$C14, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12006,23 +12036,23 @@
         <v>79</v>
       </c>
       <c r="D20" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!D15="Y",Inputs!D$20="Y"), Prices!$C15, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D16="Y",Inputs!D$21="Y"), Prices!$C15, 0)</f>
         <v>0</v>
       </c>
       <c r="E20" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!E15="Y",Inputs!E$20="Y"), Prices!$C15, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E16="Y",Inputs!E$21="Y"), Prices!$C15, 0)</f>
         <v>0</v>
       </c>
       <c r="F20" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!F15="Y",Inputs!F$20="Y"), Prices!$C15, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F16="Y",Inputs!F$21="Y"), Prices!$C15, 0)</f>
         <v>0</v>
       </c>
       <c r="G20" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!G15="Y",Inputs!G$20="Y"), Prices!$C15, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G16="Y",Inputs!G$21="Y"), Prices!$C15, 0)</f>
         <v>0</v>
       </c>
       <c r="H20" s="18">
-        <f xml:space="preserve"> IF(OR(Inputs!H15="Y",Inputs!H$20="Y"), Prices!$C15, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H16="Y",Inputs!H$21="Y"), Prices!$C15, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12031,23 +12061,23 @@
         <v>11</v>
       </c>
       <c r="D21" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!D16="Y",Inputs!D$21="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D17="Y",Inputs!D$22="Y"), Prices!$C16, 0)</f>
         <v>0</v>
       </c>
       <c r="E21" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!E16="Y",Inputs!E$21="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E17="Y",Inputs!E$22="Y"), Prices!$C16, 0)</f>
         <v>0</v>
       </c>
       <c r="F21" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!F16="Y",Inputs!F$21="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F17="Y",Inputs!F$22="Y"), Prices!$C16, 0)</f>
         <v>0</v>
       </c>
       <c r="G21" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!G16="Y",Inputs!G$21="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G17="Y",Inputs!G$22="Y"), Prices!$C16, 0)</f>
         <v>0</v>
       </c>
       <c r="H21" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!H16="Y",Inputs!H$21="Y"), Prices!$C16, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H17="Y",Inputs!H$22="Y"), Prices!$C16, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12056,23 +12086,23 @@
         <v>12</v>
       </c>
       <c r="D22" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!D17="Y",Inputs!D$21="Y"), Prices!$C17, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D18="Y",Inputs!D$22="Y"), Prices!$C17, 0)</f>
         <v>0</v>
       </c>
       <c r="E22" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!E17="Y",Inputs!E$21="Y"), Prices!$C17, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E18="Y",Inputs!E$22="Y"), Prices!$C17, 0)</f>
         <v>0</v>
       </c>
       <c r="F22" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!F17="Y",Inputs!F$21="Y"), Prices!$C17, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F18="Y",Inputs!F$22="Y"), Prices!$C17, 0)</f>
         <v>0</v>
       </c>
       <c r="G22" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!G17="Y",Inputs!G$21="Y"), Prices!$C17, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G18="Y",Inputs!G$22="Y"), Prices!$C17, 0)</f>
         <v>0</v>
       </c>
       <c r="H22" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!H17="Y",Inputs!H$21="Y"), Prices!$C17, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H18="Y",Inputs!H$22="Y"), Prices!$C17, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12081,23 +12111,23 @@
         <v>23</v>
       </c>
       <c r="D23" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!D18="Y",Inputs!D$21="Y"), Prices!$C18, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!D19="Y",Inputs!D$22="Y"), Prices!$C18, 0)</f>
         <v>0</v>
       </c>
       <c r="E23" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!E18="Y",Inputs!E$21="Y"), Prices!$C18, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!E19="Y",Inputs!E$22="Y"), Prices!$C18, 0)</f>
         <v>0</v>
       </c>
       <c r="F23" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!F18="Y",Inputs!F$21="Y"), Prices!$C18, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!F19="Y",Inputs!F$22="Y"), Prices!$C18, 0)</f>
         <v>0</v>
       </c>
       <c r="G23" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!G18="Y",Inputs!G$21="Y"), Prices!$C18, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!G19="Y",Inputs!G$22="Y"), Prices!$C18, 0)</f>
         <v>0</v>
       </c>
       <c r="H23" s="20">
-        <f xml:space="preserve"> IF(OR(Inputs!H18="Y",Inputs!H$21="Y"), Prices!$C18, 0)</f>
+        <f xml:space="preserve"> IF(OR(Inputs!H19="Y",Inputs!H$22="Y"), Prices!$C18, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12111,23 +12141,23 @@
         <v>2</v>
       </c>
       <c r="D26" s="16">
-        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", "", PRODUCT(D$11, Prices!$E$6)))*D$10</f>
+        <f>IF(Inputs!D$5="Y", 0, IF(D$11 = "", "", PRODUCT(D$11, Prices!$E$6)))*D$10</f>
         <v>0</v>
       </c>
       <c r="E26" s="16">
-        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", "", PRODUCT(E$11, Prices!$E$6)))*E$10</f>
+        <f>IF(Inputs!E$5="Y", 0, IF(E$11 = "", "", PRODUCT(E$11, Prices!$E$6)))*E$10</f>
         <v>24570.000000000004</v>
       </c>
       <c r="F26" s="16">
-        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", "", PRODUCT(F$11, Prices!$E$6)))*F$10</f>
+        <f>IF(Inputs!F$5="Y", 0, IF(F$11 = "", "", PRODUCT(F$11, Prices!$E$6)))*F$10</f>
         <v>0</v>
       </c>
       <c r="G26" s="16">
-        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", "", PRODUCT(G$11, Prices!$E$6)))*G$10</f>
+        <f>IF(Inputs!G$5="Y", 0, IF(G$11 = "", "", PRODUCT(G$11, Prices!$E$6)))*G$10</f>
         <v>0</v>
       </c>
       <c r="H26" s="16">
-        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", "", PRODUCT(H$11, Prices!$E$6)))*H$10</f>
+        <f>IF(Inputs!H$5="Y", 0, IF(H$11 = "", "", PRODUCT(H$11, Prices!$E$6)))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12136,23 +12166,23 @@
         <v>21</v>
       </c>
       <c r="D27" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D10="Y",Inputs!D$20="Y"),PRODUCT(D$11, Prices!$E10),0))*D$10</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(OR(Inputs!D11="Y",Inputs!D$21="Y"),PRODUCT(D$11, Prices!$E10),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E27" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E10="Y",Inputs!E$20="Y"),PRODUCT(E$11, Prices!$E10),0))*E$10</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(OR(Inputs!E11="Y",Inputs!E$21="Y"),PRODUCT(E$11, Prices!$E10),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F27" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F10="Y",Inputs!F$20="Y"),PRODUCT(F$11, Prices!$E10),0))*F$10</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(OR(Inputs!F11="Y",Inputs!F$21="Y"),PRODUCT(F$11, Prices!$E10),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G27" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G10="Y",Inputs!G$20="Y"),PRODUCT(G$11, Prices!$E10),0))*G$10</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(OR(Inputs!G11="Y",Inputs!G$21="Y"),PRODUCT(G$11, Prices!$E10),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H27" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H10="Y",Inputs!H$20="Y"),PRODUCT(H$11, Prices!$E10),0))*H$10</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(OR(Inputs!H11="Y",Inputs!H$21="Y"),PRODUCT(H$11, Prices!$E10),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12161,23 +12191,23 @@
         <v>8</v>
       </c>
       <c r="D28" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D11="Y",Inputs!D$20="Y"),PRODUCT(D$11, Prices!$E11),0))*D$10</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(OR(Inputs!D12="Y",Inputs!D$21="Y"),PRODUCT(D$11, Prices!$E11),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E28" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E11="Y",Inputs!E$20="Y"),PRODUCT(E$11, Prices!$E11),0))*E$10</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(OR(Inputs!E12="Y",Inputs!E$21="Y"),PRODUCT(E$11, Prices!$E11),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F28" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F11="Y",Inputs!F$20="Y"),PRODUCT(F$11, Prices!$E11),0))*F$10</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(OR(Inputs!F12="Y",Inputs!F$21="Y"),PRODUCT(F$11, Prices!$E11),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G28" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G11="Y",Inputs!G$20="Y"),PRODUCT(G$11, Prices!$E11),0))*G$10</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(OR(Inputs!G12="Y",Inputs!G$21="Y"),PRODUCT(G$11, Prices!$E11),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H28" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H11="Y",Inputs!H$20="Y"),PRODUCT(H$11, Prices!$E11),0))*H$10</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(OR(Inputs!H12="Y",Inputs!H$21="Y"),PRODUCT(H$11, Prices!$E11),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12186,23 +12216,23 @@
         <v>22</v>
       </c>
       <c r="D29" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D12="Y",Inputs!D$20="Y"),PRODUCT(D$11, Prices!$E12),0))*D$10</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(OR(Inputs!D13="Y",Inputs!D$21="Y"),PRODUCT(D$11, Prices!$E12),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E29" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E12="Y",Inputs!E$20="Y"),PRODUCT(E$11, Prices!$E12),0))*E$10</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(OR(Inputs!E13="Y",Inputs!E$21="Y"),PRODUCT(E$11, Prices!$E12),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F29" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F12="Y",Inputs!F$20="Y"),PRODUCT(F$11, Prices!$E12),0))*F$10</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(OR(Inputs!F13="Y",Inputs!F$21="Y"),PRODUCT(F$11, Prices!$E12),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G29" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G12="Y",Inputs!G$20="Y"),PRODUCT(G$11, Prices!$E12),0))*G$10</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(OR(Inputs!G13="Y",Inputs!G$21="Y"),PRODUCT(G$11, Prices!$E12),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H29" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H12="Y",Inputs!H$20="Y"),PRODUCT(H$11, Prices!$E12),0))*H$10</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(OR(Inputs!H13="Y",Inputs!H$21="Y"),PRODUCT(H$11, Prices!$E12),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12211,23 +12241,23 @@
         <v>9</v>
       </c>
       <c r="D30" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D13="Y",Inputs!D$20="Y"),PRODUCT(D$11, Prices!$E13),0))*D$10</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(OR(Inputs!D14="Y",Inputs!D$21="Y"),PRODUCT(D$11, Prices!$E13),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E30" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E13="Y",Inputs!E$20="Y"),PRODUCT(E$11, Prices!$E13),0))*E$10</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(OR(Inputs!E14="Y",Inputs!E$21="Y"),PRODUCT(E$11, Prices!$E13),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F30" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F13="Y",Inputs!F$20="Y"),PRODUCT(F$11, Prices!$E13),0))*F$10</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(OR(Inputs!F14="Y",Inputs!F$21="Y"),PRODUCT(F$11, Prices!$E13),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G30" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G13="Y",Inputs!G$20="Y"),PRODUCT(G$11, Prices!$E13),0))*G$10</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(OR(Inputs!G14="Y",Inputs!G$21="Y"),PRODUCT(G$11, Prices!$E13),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H30" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H13="Y",Inputs!H$20="Y"),PRODUCT(H$11, Prices!$E13),0))*H$10</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(OR(Inputs!H14="Y",Inputs!H$21="Y"),PRODUCT(H$11, Prices!$E13),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12236,23 +12266,23 @@
         <v>10</v>
       </c>
       <c r="D31" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D14="Y",Inputs!D$20="Y"),PRODUCT(D$11, Prices!$E14),0))*D$10</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(OR(Inputs!D15="Y",Inputs!D$21="Y"),PRODUCT(D$11, Prices!$E14),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E31" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E14="Y",Inputs!E$20="Y"),PRODUCT(E$11, Prices!$E14),0))*E$10</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(OR(Inputs!E15="Y",Inputs!E$21="Y"),PRODUCT(E$11, Prices!$E14),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F31" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F14="Y",Inputs!F$20="Y"),PRODUCT(F$11, Prices!$E14),0))*F$10</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(OR(Inputs!F15="Y",Inputs!F$21="Y"),PRODUCT(F$11, Prices!$E14),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G31" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G14="Y",Inputs!G$20="Y"),PRODUCT(G$11, Prices!$E14),0))*G$10</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(OR(Inputs!G15="Y",Inputs!G$21="Y"),PRODUCT(G$11, Prices!$E14),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H31" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H14="Y",Inputs!H$20="Y"),PRODUCT(H$11, Prices!$E14),0))*H$10</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(OR(Inputs!H15="Y",Inputs!H$21="Y"),PRODUCT(H$11, Prices!$E14),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12261,23 +12291,23 @@
         <v>79</v>
       </c>
       <c r="D32" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D15="Y",Inputs!D$20="Y"),PRODUCT(D$11, Prices!$E15),0))*D$10</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(OR(Inputs!D16="Y",Inputs!D$21="Y"),PRODUCT(D$11, Prices!$E15),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E32" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E15="Y",Inputs!E$20="Y"),PRODUCT(E$11, Prices!$E15),0))*E$10</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(OR(Inputs!E16="Y",Inputs!E$21="Y"),PRODUCT(E$11, Prices!$E15),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F32" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F15="Y",Inputs!F$20="Y"),PRODUCT(F$11, Prices!$E15),0))*F$10</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(OR(Inputs!F16="Y",Inputs!F$21="Y"),PRODUCT(F$11, Prices!$E15),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G32" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G15="Y",Inputs!G$20="Y"),PRODUCT(G$11, Prices!$E15),0))*G$10</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(OR(Inputs!G16="Y",Inputs!G$21="Y"),PRODUCT(G$11, Prices!$E15),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H32" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H15="Y",Inputs!H$20="Y"),PRODUCT(H$11, Prices!$E15),0))*H$10</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(OR(Inputs!H16="Y",Inputs!H$21="Y"),PRODUCT(H$11, Prices!$E15),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12286,23 +12316,23 @@
         <v>11</v>
       </c>
       <c r="D33" s="20">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D16="Y",Inputs!D$21="Y"),PRODUCT(D$11, Prices!$E16),0))*D$10</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(OR(Inputs!D17="Y",Inputs!D$22="Y"),PRODUCT(D$11, Prices!$E16),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E33" s="20">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E16="Y",Inputs!E$21="Y"),PRODUCT(E$11, Prices!$E16),0))*E$10</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(OR(Inputs!E17="Y",Inputs!E$22="Y"),PRODUCT(E$11, Prices!$E16),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F33" s="20">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F16="Y",Inputs!F$21="Y"),PRODUCT(F$11, Prices!$E16),0))*F$10</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(OR(Inputs!F17="Y",Inputs!F$22="Y"),PRODUCT(F$11, Prices!$E16),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G33" s="20">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G16="Y",Inputs!G$21="Y"),PRODUCT(G$11, Prices!$E16),0))*G$10</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(OR(Inputs!G17="Y",Inputs!G$22="Y"),PRODUCT(G$11, Prices!$E16),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H33" s="20">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H16="Y",Inputs!H$21="Y"),PRODUCT(H$11, Prices!$E16),0))*H$10</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(OR(Inputs!H17="Y",Inputs!H$22="Y"),PRODUCT(H$11, Prices!$E16),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12311,23 +12341,23 @@
         <v>12</v>
       </c>
       <c r="D34" s="20">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D17="Y",Inputs!D$21="Y"),PRODUCT(D$11, Prices!$E17),0))*D$10</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(OR(Inputs!D18="Y",Inputs!D$22="Y"),PRODUCT(D$11, Prices!$E17),0))*D$10</f>
         <v>0</v>
       </c>
       <c r="E34" s="20">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E17="Y",Inputs!E$21="Y"),PRODUCT(E$11, Prices!$E17),0))*E$10</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(OR(Inputs!E18="Y",Inputs!E$22="Y"),PRODUCT(E$11, Prices!$E17),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F34" s="20">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F17="Y",Inputs!F$21="Y"),PRODUCT(F$11, Prices!$E17),0))*F$10</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(OR(Inputs!F18="Y",Inputs!F$22="Y"),PRODUCT(F$11, Prices!$E17),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G34" s="20">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G17="Y",Inputs!G$21="Y"),PRODUCT(G$11, Prices!$E17),0))*G$10</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(OR(Inputs!G18="Y",Inputs!G$22="Y"),PRODUCT(G$11, Prices!$E17),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H34" s="20">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H17="Y",Inputs!H$21="Y"),PRODUCT(H$11, Prices!$E17),0))*H$10</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(OR(Inputs!H18="Y",Inputs!H$22="Y"),PRODUCT(H$11, Prices!$E17),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12368,23 +12398,23 @@
         <v>2</v>
       </c>
       <c r="D38" s="16">
-        <f>IF(Inputs!D4="Y", Prices!$C$6, IF(Inputs!D4="N", Prices!$D$6, 0))</f>
+        <f>IF(Inputs!D5="Y", Prices!$C$6, IF(Inputs!D5="N", Prices!$D$6, 0))</f>
         <v>15000</v>
       </c>
       <c r="E38" s="16">
-        <f>IF(Inputs!E4="Y", Prices!$C$6, IF(Inputs!E4="N", Prices!$D$6, 0))</f>
+        <f>IF(Inputs!E5="Y", Prices!$C$6, IF(Inputs!E5="N", Prices!$D$6, 0))</f>
         <v>30000</v>
       </c>
       <c r="F38" s="16">
-        <f>IF(Inputs!F4="Y", Prices!$C$6, IF(Inputs!F4="N", Prices!$D$6, 0))</f>
+        <f>IF(Inputs!F5="Y", Prices!$C$6, IF(Inputs!F5="N", Prices!$D$6, 0))</f>
         <v>0</v>
       </c>
       <c r="G38" s="16">
-        <f>IF(Inputs!G4="Y", Prices!$C$6, IF(Inputs!G4="N", Prices!$D$6, 0))</f>
+        <f>IF(Inputs!G5="Y", Prices!$C$6, IF(Inputs!G5="N", Prices!$D$6, 0))</f>
         <v>0</v>
       </c>
       <c r="H38" s="16">
-        <f>IF(Inputs!H4="Y", Prices!$C$6, IF(Inputs!H4="N", Prices!$D$6, 0))</f>
+        <f>IF(Inputs!H5="Y", Prices!$C$6, IF(Inputs!H5="N", Prices!$D$6, 0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12393,23 +12423,23 @@
         <v>21</v>
       </c>
       <c r="D39" s="18">
-        <f>IF(AND(Inputs!D10="Y",Inputs!D$20="N"),Prices!$C10,0)</f>
+        <f>IF(AND(Inputs!D11="Y",Inputs!D$21="N"),Prices!$C10,0)</f>
         <v>0</v>
       </c>
       <c r="E39" s="18">
-        <f>IF(AND(Inputs!E10="Y",Inputs!E$20="N"),Prices!$C10,0)</f>
+        <f>IF(AND(Inputs!E11="Y",Inputs!E$21="N"),Prices!$C10,0)</f>
         <v>0</v>
       </c>
       <c r="F39" s="18">
-        <f>IF(AND(Inputs!F10="Y",Inputs!F$20="N"),Prices!$C10,0)</f>
+        <f>IF(AND(Inputs!F11="Y",Inputs!F$21="N"),Prices!$C10,0)</f>
         <v>0</v>
       </c>
       <c r="G39" s="18">
-        <f>IF(AND(Inputs!G10="Y",Inputs!G$20="N"),Prices!$C10,0)</f>
+        <f>IF(AND(Inputs!G11="Y",Inputs!G$21="N"),Prices!$C10,0)</f>
         <v>0</v>
       </c>
       <c r="H39" s="18">
-        <f>IF(AND(Inputs!H10="Y",Inputs!H$20="N"),Prices!$C10,0)</f>
+        <f>IF(AND(Inputs!H11="Y",Inputs!H$21="N"),Prices!$C10,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12418,23 +12448,23 @@
         <v>8</v>
       </c>
       <c r="D40" s="18">
-        <f>IF(AND(Inputs!D11="Y",Inputs!D$20="N"),Prices!$C11,0)</f>
+        <f>IF(AND(Inputs!D12="Y",Inputs!D$21="N"),Prices!$C11,0)</f>
         <v>0</v>
       </c>
       <c r="E40" s="18">
-        <f>IF(AND(Inputs!E11="Y",Inputs!E$20="N"),Prices!$C11,0)</f>
+        <f>IF(AND(Inputs!E12="Y",Inputs!E$21="N"),Prices!$C11,0)</f>
         <v>0</v>
       </c>
       <c r="F40" s="18">
-        <f>IF(AND(Inputs!F11="Y",Inputs!F$20="N"),Prices!$C11,0)</f>
+        <f>IF(AND(Inputs!F12="Y",Inputs!F$21="N"),Prices!$C11,0)</f>
         <v>0</v>
       </c>
       <c r="G40" s="18">
-        <f>IF(AND(Inputs!G11="Y",Inputs!G$20="N"),Prices!$C11,0)</f>
+        <f>IF(AND(Inputs!G12="Y",Inputs!G$21="N"),Prices!$C11,0)</f>
         <v>0</v>
       </c>
       <c r="H40" s="18">
-        <f>IF(AND(Inputs!H11="Y",Inputs!H$20="N"),Prices!$C11,0)</f>
+        <f>IF(AND(Inputs!H12="Y",Inputs!H$21="N"),Prices!$C11,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12443,23 +12473,23 @@
         <v>22</v>
       </c>
       <c r="D41" s="18">
-        <f>IF(AND(Inputs!D12="Y",Inputs!D$20="N"),Prices!$C12,0)</f>
+        <f>IF(AND(Inputs!D13="Y",Inputs!D$21="N"),Prices!$C12,0)</f>
         <v>0</v>
       </c>
       <c r="E41" s="18">
-        <f>IF(AND(Inputs!E12="Y",Inputs!E$20="N"),Prices!$C12,0)</f>
+        <f>IF(AND(Inputs!E13="Y",Inputs!E$21="N"),Prices!$C12,0)</f>
         <v>0</v>
       </c>
       <c r="F41" s="18">
-        <f>IF(AND(Inputs!F12="Y",Inputs!F$20="N"),Prices!$C12,0)</f>
+        <f>IF(AND(Inputs!F13="Y",Inputs!F$21="N"),Prices!$C12,0)</f>
         <v>0</v>
       </c>
       <c r="G41" s="18">
-        <f>IF(AND(Inputs!G12="Y",Inputs!G$20="N"),Prices!$C12,0)</f>
+        <f>IF(AND(Inputs!G13="Y",Inputs!G$21="N"),Prices!$C12,0)</f>
         <v>0</v>
       </c>
       <c r="H41" s="18">
-        <f>IF(AND(Inputs!H12="Y",Inputs!H$20="N"),Prices!$C12,0)</f>
+        <f>IF(AND(Inputs!H13="Y",Inputs!H$21="N"),Prices!$C12,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12468,23 +12498,23 @@
         <v>9</v>
       </c>
       <c r="D42" s="18">
-        <f>IF(AND(Inputs!D13="Y",Inputs!D$20="N"),Prices!$C13,0)</f>
+        <f>IF(AND(Inputs!D14="Y",Inputs!D$21="N"),Prices!$C13,0)</f>
         <v>0</v>
       </c>
       <c r="E42" s="18">
-        <f>IF(AND(Inputs!E13="Y",Inputs!E$20="N"),Prices!$C13,0)</f>
+        <f>IF(AND(Inputs!E14="Y",Inputs!E$21="N"),Prices!$C13,0)</f>
         <v>0</v>
       </c>
       <c r="F42" s="18">
-        <f>IF(AND(Inputs!F13="Y",Inputs!F$20="N"),Prices!$C13,0)</f>
+        <f>IF(AND(Inputs!F14="Y",Inputs!F$21="N"),Prices!$C13,0)</f>
         <v>0</v>
       </c>
       <c r="G42" s="18">
-        <f>IF(AND(Inputs!G13="Y",Inputs!G$20="N"),Prices!$C13,0)</f>
+        <f>IF(AND(Inputs!G14="Y",Inputs!G$21="N"),Prices!$C13,0)</f>
         <v>0</v>
       </c>
       <c r="H42" s="18">
-        <f>IF(AND(Inputs!H13="Y",Inputs!H$20="N"),Prices!$C13,0)</f>
+        <f>IF(AND(Inputs!H14="Y",Inputs!H$21="N"),Prices!$C13,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12493,23 +12523,23 @@
         <v>10</v>
       </c>
       <c r="D43" s="18">
-        <f>IF(AND(Inputs!D14="Y",Inputs!D$20="N"),Prices!$C14,0)</f>
+        <f>IF(AND(Inputs!D15="Y",Inputs!D$21="N"),Prices!$C14,0)</f>
         <v>0</v>
       </c>
       <c r="E43" s="18">
-        <f>IF(AND(Inputs!E14="Y",Inputs!E$20="N"),Prices!$C14,0)</f>
+        <f>IF(AND(Inputs!E15="Y",Inputs!E$21="N"),Prices!$C14,0)</f>
         <v>0</v>
       </c>
       <c r="F43" s="18">
-        <f>IF(AND(Inputs!F14="Y",Inputs!F$20="N"),Prices!$C14,0)</f>
+        <f>IF(AND(Inputs!F15="Y",Inputs!F$21="N"),Prices!$C14,0)</f>
         <v>0</v>
       </c>
       <c r="G43" s="18">
-        <f>IF(AND(Inputs!G14="Y",Inputs!G$20="N"),Prices!$C14,0)</f>
+        <f>IF(AND(Inputs!G15="Y",Inputs!G$21="N"),Prices!$C14,0)</f>
         <v>0</v>
       </c>
       <c r="H43" s="18">
-        <f>IF(AND(Inputs!H14="Y",Inputs!H$20="N"),Prices!$C14,0)</f>
+        <f>IF(AND(Inputs!H15="Y",Inputs!H$21="N"),Prices!$C14,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12518,23 +12548,23 @@
         <v>79</v>
       </c>
       <c r="D44" s="18">
-        <f>IF(AND(Inputs!D15="Y",Inputs!D$20="N"),Prices!$C15,0)</f>
+        <f>IF(AND(Inputs!D16="Y",Inputs!D$21="N"),Prices!$C15,0)</f>
         <v>0</v>
       </c>
       <c r="E44" s="18">
-        <f>IF(AND(Inputs!E15="Y",Inputs!E$20="N"),Prices!$C15,0)</f>
+        <f>IF(AND(Inputs!E16="Y",Inputs!E$21="N"),Prices!$C15,0)</f>
         <v>0</v>
       </c>
       <c r="F44" s="18">
-        <f>IF(AND(Inputs!F15="Y",Inputs!F$20="N"),Prices!$C15,0)</f>
+        <f>IF(AND(Inputs!F16="Y",Inputs!F$21="N"),Prices!$C15,0)</f>
         <v>0</v>
       </c>
       <c r="G44" s="18">
-        <f>IF(AND(Inputs!G15="Y",Inputs!G$20="N"),Prices!$C15,0)</f>
+        <f>IF(AND(Inputs!G16="Y",Inputs!G$21="N"),Prices!$C15,0)</f>
         <v>0</v>
       </c>
       <c r="H44" s="18">
-        <f>IF(AND(Inputs!H15="Y",Inputs!H$20="N"),Prices!$C15,0)</f>
+        <f>IF(AND(Inputs!H16="Y",Inputs!H$21="N"),Prices!$C15,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12543,23 +12573,23 @@
         <v>11</v>
       </c>
       <c r="D45" s="20">
-        <f>IF(AND(Inputs!D16="Y",Inputs!D$21="N"),Prices!$C16,0)</f>
+        <f>IF(AND(Inputs!D17="Y",Inputs!D$22="N"),Prices!$C16,0)</f>
         <v>0</v>
       </c>
       <c r="E45" s="20">
-        <f>IF(AND(Inputs!E16="Y",Inputs!E$21="N"),Prices!$C16,0)</f>
+        <f>IF(AND(Inputs!E17="Y",Inputs!E$22="N"),Prices!$C16,0)</f>
         <v>0</v>
       </c>
       <c r="F45" s="20">
-        <f>IF(AND(Inputs!F16="Y",Inputs!F$21="N"),Prices!$C16,0)</f>
+        <f>IF(AND(Inputs!F17="Y",Inputs!F$22="N"),Prices!$C16,0)</f>
         <v>0</v>
       </c>
       <c r="G45" s="20">
-        <f>IF(AND(Inputs!G16="Y",Inputs!G$21="N"),Prices!$C16,0)</f>
+        <f>IF(AND(Inputs!G17="Y",Inputs!G$22="N"),Prices!$C16,0)</f>
         <v>0</v>
       </c>
       <c r="H45" s="20">
-        <f>IF(AND(Inputs!H16="Y",Inputs!H$21="N"),Prices!$C16,0)</f>
+        <f>IF(AND(Inputs!H17="Y",Inputs!H$22="N"),Prices!$C16,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12568,23 +12598,23 @@
         <v>12</v>
       </c>
       <c r="D46" s="20">
-        <f>IF(AND(Inputs!D17="Y",Inputs!D$21="N"),Prices!$C17,0)</f>
+        <f>IF(AND(Inputs!D18="Y",Inputs!D$22="N"),Prices!$C17,0)</f>
         <v>0</v>
       </c>
       <c r="E46" s="20">
-        <f>IF(AND(Inputs!E17="Y",Inputs!E$21="N"),Prices!$C17,0)</f>
+        <f>IF(AND(Inputs!E18="Y",Inputs!E$22="N"),Prices!$C17,0)</f>
         <v>0</v>
       </c>
       <c r="F46" s="20">
-        <f>IF(AND(Inputs!F17="Y",Inputs!F$21="N"),Prices!$C17,0)</f>
+        <f>IF(AND(Inputs!F18="Y",Inputs!F$22="N"),Prices!$C17,0)</f>
         <v>0</v>
       </c>
       <c r="G46" s="20">
-        <f>IF(AND(Inputs!G17="Y",Inputs!G$21="N"),Prices!$C17,0)</f>
+        <f>IF(AND(Inputs!G18="Y",Inputs!G$22="N"),Prices!$C17,0)</f>
         <v>0</v>
       </c>
       <c r="H46" s="20">
-        <f>IF(AND(Inputs!H17="Y",Inputs!H$21="N"),Prices!$C17,0)</f>
+        <f>IF(AND(Inputs!H18="Y",Inputs!H$22="N"),Prices!$C17,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12593,23 +12623,23 @@
         <v>23</v>
       </c>
       <c r="D47" s="20">
-        <f>IF(AND(Inputs!D18="Y",Inputs!D$21="N"),Prices!$C18,0)</f>
+        <f>IF(AND(Inputs!D19="Y",Inputs!D$22="N"),Prices!$C18,0)</f>
         <v>0</v>
       </c>
       <c r="E47" s="20">
-        <f>IF(AND(Inputs!E18="Y",Inputs!E$21="N"),Prices!$C18,0)</f>
+        <f>IF(AND(Inputs!E19="Y",Inputs!E$22="N"),Prices!$C18,0)</f>
         <v>0</v>
       </c>
       <c r="F47" s="20">
-        <f>IF(AND(Inputs!F18="Y",Inputs!F$21="N"),Prices!$C18,0)</f>
+        <f>IF(AND(Inputs!F19="Y",Inputs!F$22="N"),Prices!$C18,0)</f>
         <v>0</v>
       </c>
       <c r="G47" s="20">
-        <f>IF(AND(Inputs!G18="Y",Inputs!G$21="N"),Prices!$C18,0)</f>
+        <f>IF(AND(Inputs!G19="Y",Inputs!G$22="N"),Prices!$C18,0)</f>
         <v>0</v>
       </c>
       <c r="H47" s="20">
-        <f>IF(AND(Inputs!H18="Y",Inputs!H$21="N"),Prices!$C18,0)</f>
+        <f>IF(AND(Inputs!H19="Y",Inputs!H$22="N"),Prices!$C18,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12623,23 +12653,23 @@
         <v>2</v>
       </c>
       <c r="D50" s="16">
-        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", "", PRODUCT(D$11, Prices!$E$6)*D$10))</f>
+        <f>IF(Inputs!D$5="Y", 0, IF(D$11 = "", "", PRODUCT(D$11, Prices!$E$6)*D$10))</f>
         <v>0</v>
       </c>
       <c r="E50" s="16">
-        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", "", PRODUCT(E$11, Prices!$E$6)*E$10))</f>
+        <f>IF(Inputs!E$5="Y", 0, IF(E$11 = "", "", PRODUCT(E$11, Prices!$E$6)*E$10))</f>
         <v>24570.000000000004</v>
       </c>
       <c r="F50" s="16">
-        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", "", PRODUCT(F$11, Prices!$E$6)*F$10))</f>
+        <f>IF(Inputs!F$5="Y", 0, IF(F$11 = "", "", PRODUCT(F$11, Prices!$E$6)*F$10))</f>
         <v>0</v>
       </c>
       <c r="G50" s="16">
-        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", "", PRODUCT(G$11, Prices!$E$6)*G$10))</f>
+        <f>IF(Inputs!G$5="Y", 0, IF(G$11 = "", "", PRODUCT(G$11, Prices!$E$6)*G$10))</f>
         <v>0</v>
       </c>
       <c r="H50" s="16">
-        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", "", PRODUCT(H$11, Prices!$E$6)*H$10))</f>
+        <f>IF(Inputs!H$5="Y", 0, IF(H$11 = "", "", PRODUCT(H$11, Prices!$E$6)*H$10))</f>
         <v>0</v>
       </c>
     </row>
@@ -12648,23 +12678,23 @@
         <v>21</v>
       </c>
       <c r="D51" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D10="Y",Inputs!D$20="N"),PRODUCT(D$11, Prices!$E10)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(AND(Inputs!D11="Y",Inputs!D$21="N"),PRODUCT(D$11, Prices!$E10)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E51" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E10="Y",Inputs!E$20="N"),PRODUCT(E$11, Prices!$E10)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(AND(Inputs!E11="Y",Inputs!E$21="N"),PRODUCT(E$11, Prices!$E10)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F51" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F10="Y",Inputs!F$20="N"),PRODUCT(F$11, Prices!$E10)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(AND(Inputs!F11="Y",Inputs!F$21="N"),PRODUCT(F$11, Prices!$E10)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G51" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G10="Y",Inputs!G$20="N"),PRODUCT(G$11, Prices!$E10)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(AND(Inputs!G11="Y",Inputs!G$21="N"),PRODUCT(G$11, Prices!$E10)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H51" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H10="Y",Inputs!H$20="N"),PRODUCT(H$11, Prices!$E10)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(AND(Inputs!H11="Y",Inputs!H$21="N"),PRODUCT(H$11, Prices!$E10)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12673,23 +12703,23 @@
         <v>8</v>
       </c>
       <c r="D52" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D11="Y",Inputs!D$20="N"),PRODUCT(D$11, Prices!$E11)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(AND(Inputs!D12="Y",Inputs!D$21="N"),PRODUCT(D$11, Prices!$E11)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E52" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E11="Y",Inputs!E$20="N"),PRODUCT(E$11, Prices!$E11)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(AND(Inputs!E12="Y",Inputs!E$21="N"),PRODUCT(E$11, Prices!$E11)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F52" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F11="Y",Inputs!F$20="N"),PRODUCT(F$11, Prices!$E11)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(AND(Inputs!F12="Y",Inputs!F$21="N"),PRODUCT(F$11, Prices!$E11)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G52" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G11="Y",Inputs!G$20="N"),PRODUCT(G$11, Prices!$E11)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(AND(Inputs!G12="Y",Inputs!G$21="N"),PRODUCT(G$11, Prices!$E11)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H52" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H11="Y",Inputs!H$20="N"),PRODUCT(H$11, Prices!$E11)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(AND(Inputs!H12="Y",Inputs!H$21="N"),PRODUCT(H$11, Prices!$E11)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12698,23 +12728,23 @@
         <v>22</v>
       </c>
       <c r="D53" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D12="Y",Inputs!D$20="N"),PRODUCT(D$11, Prices!$E12)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(AND(Inputs!D13="Y",Inputs!D$21="N"),PRODUCT(D$11, Prices!$E12)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E53" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E12="Y",Inputs!E$20="N"),PRODUCT(E$11, Prices!$E12)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(AND(Inputs!E13="Y",Inputs!E$21="N"),PRODUCT(E$11, Prices!$E12)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F53" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F12="Y",Inputs!F$20="N"),PRODUCT(F$11, Prices!$E12)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(AND(Inputs!F13="Y",Inputs!F$21="N"),PRODUCT(F$11, Prices!$E12)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G53" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G12="Y",Inputs!G$20="N"),PRODUCT(G$11, Prices!$E12)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(AND(Inputs!G13="Y",Inputs!G$21="N"),PRODUCT(G$11, Prices!$E12)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H53" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H12="Y",Inputs!H$20="N"),PRODUCT(H$11, Prices!$E12)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(AND(Inputs!H13="Y",Inputs!H$21="N"),PRODUCT(H$11, Prices!$E12)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12723,23 +12753,23 @@
         <v>9</v>
       </c>
       <c r="D54" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D13="Y",Inputs!D$20="N"),PRODUCT(D$11, Prices!$E13)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(AND(Inputs!D14="Y",Inputs!D$21="N"),PRODUCT(D$11, Prices!$E13)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E54" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E13="Y",Inputs!E$20="N"),PRODUCT(E$11, Prices!$E13)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(AND(Inputs!E14="Y",Inputs!E$21="N"),PRODUCT(E$11, Prices!$E13)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F54" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F13="Y",Inputs!F$20="N"),PRODUCT(F$11, Prices!$E13)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(AND(Inputs!F14="Y",Inputs!F$21="N"),PRODUCT(F$11, Prices!$E13)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G54" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G13="Y",Inputs!G$20="N"),PRODUCT(G$11, Prices!$E13)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(AND(Inputs!G14="Y",Inputs!G$21="N"),PRODUCT(G$11, Prices!$E13)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H54" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H13="Y",Inputs!H$20="N"),PRODUCT(H$11, Prices!$E13)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(AND(Inputs!H14="Y",Inputs!H$21="N"),PRODUCT(H$11, Prices!$E13)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12748,23 +12778,23 @@
         <v>10</v>
       </c>
       <c r="D55" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D14="Y",Inputs!D$20="N"),PRODUCT(D$11, Prices!$E14)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(AND(Inputs!D15="Y",Inputs!D$21="N"),PRODUCT(D$11, Prices!$E14)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E55" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E14="Y",Inputs!E$20="N"),PRODUCT(E$11, Prices!$E14)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(AND(Inputs!E15="Y",Inputs!E$21="N"),PRODUCT(E$11, Prices!$E14)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F55" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F14="Y",Inputs!F$20="N"),PRODUCT(F$11, Prices!$E14)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(AND(Inputs!F15="Y",Inputs!F$21="N"),PRODUCT(F$11, Prices!$E14)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G55" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G14="Y",Inputs!G$20="N"),PRODUCT(G$11, Prices!$E14)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(AND(Inputs!G15="Y",Inputs!G$21="N"),PRODUCT(G$11, Prices!$E14)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H55" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H14="Y",Inputs!H$20="N"),PRODUCT(H$11, Prices!$E14)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(AND(Inputs!H15="Y",Inputs!H$21="N"),PRODUCT(H$11, Prices!$E14)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12773,23 +12803,23 @@
         <v>79</v>
       </c>
       <c r="D56" s="18">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D15="Y",Inputs!D$20="N"),PRODUCT(D$11, Prices!$E15)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(AND(Inputs!D16="Y",Inputs!D$21="N"),PRODUCT(D$11, Prices!$E15)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E56" s="18">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E15="Y",Inputs!E$20="N"),PRODUCT(E$11, Prices!$E15)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(AND(Inputs!E16="Y",Inputs!E$21="N"),PRODUCT(E$11, Prices!$E15)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F56" s="18">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F15="Y",Inputs!F$20="N"),PRODUCT(F$11, Prices!$E15)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(AND(Inputs!F16="Y",Inputs!F$21="N"),PRODUCT(F$11, Prices!$E15)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G56" s="18">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G15="Y",Inputs!G$20="N"),PRODUCT(G$11, Prices!$E15)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(AND(Inputs!G16="Y",Inputs!G$21="N"),PRODUCT(G$11, Prices!$E15)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H56" s="18">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H15="Y",Inputs!H$20="N"),PRODUCT(H$11, Prices!$E15)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(AND(Inputs!H16="Y",Inputs!H$21="N"),PRODUCT(H$11, Prices!$E15)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12798,23 +12828,23 @@
         <v>11</v>
       </c>
       <c r="D57" s="20">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D16="Y",Inputs!D$21="N"),PRODUCT(D$11, Prices!$E16)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(AND(Inputs!D17="Y",Inputs!D$22="N"),PRODUCT(D$11, Prices!$E16)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E57" s="20">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E16="Y",Inputs!E$21="N"),PRODUCT(E$11, Prices!$E16)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(AND(Inputs!E17="Y",Inputs!E$22="N"),PRODUCT(E$11, Prices!$E16)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F57" s="20">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F16="Y",Inputs!F$21="N"),PRODUCT(F$11, Prices!$E16)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(AND(Inputs!F17="Y",Inputs!F$22="N"),PRODUCT(F$11, Prices!$E16)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G57" s="20">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G16="Y",Inputs!G$21="N"),PRODUCT(G$11, Prices!$E16)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(AND(Inputs!G17="Y",Inputs!G$22="N"),PRODUCT(G$11, Prices!$E16)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H57" s="20">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H16="Y",Inputs!H$21="N"),PRODUCT(H$11, Prices!$E16)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(AND(Inputs!H17="Y",Inputs!H$22="N"),PRODUCT(H$11, Prices!$E16)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12823,23 +12853,23 @@
         <v>12</v>
       </c>
       <c r="D58" s="20">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D17="Y",Inputs!D$21="N"),PRODUCT(D$11, Prices!$E17)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$5="Y", D$11 = 0), 0, IF(AND(Inputs!D18="Y",Inputs!D$22="N"),PRODUCT(D$11, Prices!$E17)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E58" s="20">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E17="Y",Inputs!E$21="N"),PRODUCT(E$11, Prices!$E17)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$5="Y", E$11 = 0), 0, IF(AND(Inputs!E18="Y",Inputs!E$22="N"),PRODUCT(E$11, Prices!$E17)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F58" s="20">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F17="Y",Inputs!F$21="N"),PRODUCT(F$11, Prices!$E17)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$5="Y", F$11 = 0), 0, IF(AND(Inputs!F18="Y",Inputs!F$22="N"),PRODUCT(F$11, Prices!$E17)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G58" s="20">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G17="Y",Inputs!G$21="N"),PRODUCT(G$11, Prices!$E17)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$5="Y", G$11 = 0), 0, IF(AND(Inputs!G18="Y",Inputs!G$22="N"),PRODUCT(G$11, Prices!$E17)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H58" s="20">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H17="Y",Inputs!H$21="N"),PRODUCT(H$11, Prices!$E17)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$5="Y", H$11 = 0), 0, IF(AND(Inputs!H18="Y",Inputs!H$22="N"),PRODUCT(H$11, Prices!$E17)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12873,23 +12903,23 @@
         <v>14</v>
       </c>
       <c r="D62" s="18">
-        <f>IF(Inputs!D$20 = "Y", 0, IF(Inputs!D19="Y", Prices!$C20, 0))</f>
+        <f>IF(Inputs!D$21 = "Y", 0, IF(Inputs!D20="Y", Prices!$C20, 0))</f>
         <v>0</v>
       </c>
       <c r="E62" s="18">
-        <f>IF(Inputs!E$20 = "Y", 0, IF(Inputs!E19="Y", Prices!$C20, 0))</f>
+        <f>IF(Inputs!E$21 = "Y", 0, IF(Inputs!E20="Y", Prices!$C20, 0))</f>
         <v>0</v>
       </c>
       <c r="F62" s="18">
-        <f>IF(Inputs!F$20 = "Y", 0, IF(Inputs!F19="Y", Prices!$C20, 0))</f>
+        <f>IF(Inputs!F$21 = "Y", 0, IF(Inputs!F20="Y", Prices!$C20, 0))</f>
         <v>0</v>
       </c>
       <c r="G62" s="18">
-        <f>IF(Inputs!G$20 = "Y", 0, IF(Inputs!G19="Y", Prices!$C20, 0))</f>
+        <f>IF(Inputs!G$21 = "Y", 0, IF(Inputs!G20="Y", Prices!$C20, 0))</f>
         <v>0</v>
       </c>
       <c r="H62" s="18">
-        <f>IF(Inputs!H$20 = "Y", 0, IF(Inputs!H19="Y", Prices!$C20, 0))</f>
+        <f>IF(Inputs!H$21 = "Y", 0, IF(Inputs!H20="Y", Prices!$C20, 0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12898,23 +12928,23 @@
         <v>15</v>
       </c>
       <c r="D63" s="18">
-        <f>IF(Inputs!D20="Y", Prices!$C21, 0)</f>
+        <f>IF(Inputs!D21="Y", Prices!$C21, 0)</f>
         <v>0</v>
       </c>
       <c r="E63" s="18">
-        <f>IF(Inputs!E20="Y", Prices!$C21, 0)</f>
+        <f>IF(Inputs!E21="Y", Prices!$C21, 0)</f>
         <v>0</v>
       </c>
       <c r="F63" s="18">
-        <f>IF(Inputs!F20="Y", Prices!$C21, 0)</f>
+        <f>IF(Inputs!F21="Y", Prices!$C21, 0)</f>
         <v>0</v>
       </c>
       <c r="G63" s="18">
-        <f>IF(Inputs!G20="Y", Prices!$C21, 0)</f>
+        <f>IF(Inputs!G21="Y", Prices!$C21, 0)</f>
         <v>0</v>
       </c>
       <c r="H63" s="18">
-        <f>IF(Inputs!H20="Y", Prices!$C21, 0)</f>
+        <f>IF(Inputs!H21="Y", Prices!$C21, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12923,23 +12953,23 @@
         <v>16</v>
       </c>
       <c r="D64" s="20">
-        <f>IF(Inputs!D21="Y", Prices!$C22, 0)</f>
+        <f>IF(Inputs!D22="Y", Prices!$C22, 0)</f>
         <v>0</v>
       </c>
       <c r="E64" s="20">
-        <f>IF(Inputs!E21="Y", Prices!$C22, 0)</f>
+        <f>IF(Inputs!E22="Y", Prices!$C22, 0)</f>
         <v>0</v>
       </c>
       <c r="F64" s="20">
-        <f>IF(Inputs!F21="Y", Prices!$C22, 0)</f>
+        <f>IF(Inputs!F22="Y", Prices!$C22, 0)</f>
         <v>0</v>
       </c>
       <c r="G64" s="20">
-        <f>IF(Inputs!G21="Y", Prices!$C22, 0)</f>
+        <f>IF(Inputs!G22="Y", Prices!$C22, 0)</f>
         <v>0</v>
       </c>
       <c r="H64" s="20">
-        <f>IF(Inputs!H21="Y", Prices!$C22, 0)</f>
+        <f>IF(Inputs!H22="Y", Prices!$C22, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12948,23 +12978,23 @@
         <v>17</v>
       </c>
       <c r="D65" s="20">
-        <f>IF(Inputs!D22="Y", Prices!$C23, 0)</f>
+        <f>IF(Inputs!D23="Y", Prices!$C23, 0)</f>
         <v>28000</v>
       </c>
       <c r="E65" s="20">
-        <f>IF(Inputs!E22="Y", Prices!$C23, 0)</f>
+        <f>IF(Inputs!E23="Y", Prices!$C23, 0)</f>
         <v>0</v>
       </c>
       <c r="F65" s="20">
-        <f>IF(Inputs!F22="Y", Prices!$C23, 0)</f>
+        <f>IF(Inputs!F23="Y", Prices!$C23, 0)</f>
         <v>0</v>
       </c>
       <c r="G65" s="20">
-        <f>IF(Inputs!G22="Y", Prices!$C23, 0)</f>
+        <f>IF(Inputs!G23="Y", Prices!$C23, 0)</f>
         <v>0</v>
       </c>
       <c r="H65" s="20">
-        <f>IF(Inputs!H22="Y", Prices!$C23, 0)</f>
+        <f>IF(Inputs!H23="Y", Prices!$C23, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12973,23 +13003,23 @@
         <v>102</v>
       </c>
       <c r="D66" s="20">
-        <f>IF(Inputs!D23="Y", Prices!$C24 * IF(Inputs!D22="Y",1-Prices!$L$20,1), 0)</f>
+        <f>IF(Inputs!D24="Y", Prices!$C24 * IF(Inputs!D23="Y",1-Prices!$L$20,1), 0)</f>
         <v>23520</v>
       </c>
       <c r="E66" s="20">
-        <f>IF(Inputs!E23="Y", Prices!$C24 * IF(Inputs!E22="Y",1-Prices!$L$20,1), 0)</f>
+        <f>IF(Inputs!E24="Y", Prices!$C24 * IF(Inputs!E23="Y",1-Prices!$L$20,1), 0)</f>
         <v>0</v>
       </c>
       <c r="F66" s="20">
-        <f>IF(Inputs!F23="Y", Prices!$C24 * IF(Inputs!F22="Y",1-Prices!$L$20,1), 0)</f>
+        <f>IF(Inputs!F24="Y", Prices!$C24 * IF(Inputs!F23="Y",1-Prices!$L$20,1), 0)</f>
         <v>0</v>
       </c>
       <c r="G66" s="20">
-        <f>IF(Inputs!G23="Y", Prices!$C24 * IF(Inputs!G22="Y",1-Prices!$L$20,1), 0)</f>
+        <f>IF(Inputs!G24="Y", Prices!$C24 * IF(Inputs!G23="Y",1-Prices!$L$20,1), 0)</f>
         <v>0</v>
       </c>
       <c r="H66" s="20">
-        <f>IF(Inputs!H23="Y", Prices!$C24 * IF(Inputs!H22="Y",1-Prices!$L$20,1), 0)</f>
+        <f>IF(Inputs!H24="Y", Prices!$C24 * IF(Inputs!H23="Y",1-Prices!$L$20,1), 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -12998,23 +13028,23 @@
         <v>101</v>
       </c>
       <c r="D67" s="20">
-        <f>IF(Inputs!D24="Y", Prices!$C25, 0)</f>
+        <f>IF(Inputs!D25="Y", Prices!$C25, 0)</f>
         <v>0</v>
       </c>
       <c r="E67" s="20">
-        <f>IF(Inputs!E24="Y", Prices!$C25, 0)</f>
+        <f>IF(Inputs!E25="Y", Prices!$C25, 0)</f>
         <v>0</v>
       </c>
       <c r="F67" s="20">
-        <f>IF(Inputs!F24="Y", Prices!$C25, 0)</f>
+        <f>IF(Inputs!F25="Y", Prices!$C25, 0)</f>
         <v>0</v>
       </c>
       <c r="G67" s="20">
-        <f>IF(Inputs!G24="Y", Prices!$C25, 0)</f>
+        <f>IF(Inputs!G25="Y", Prices!$C25, 0)</f>
         <v>0</v>
       </c>
       <c r="H67" s="20">
-        <f>IF(Inputs!H24="Y", Prices!$C25, 0)</f>
+        <f>IF(Inputs!H25="Y", Prices!$C25, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13023,23 +13053,23 @@
         <v>99</v>
       </c>
       <c r="D68" s="84">
-        <f>IF(Inputs!D9="Y", Prices!$C26, 0)</f>
+        <f>IF(Inputs!D10="Y", Prices!$C26, 0)</f>
         <v>0</v>
       </c>
       <c r="E68" s="84">
-        <f>IF(Inputs!E9="Y", Prices!$C26, 0)</f>
+        <f>IF(Inputs!E10="Y", Prices!$C26, 0)</f>
         <v>0</v>
       </c>
       <c r="F68" s="84">
-        <f>IF(Inputs!F9="Y", Prices!$C26, 0)</f>
+        <f>IF(Inputs!F10="Y", Prices!$C26, 0)</f>
         <v>0</v>
       </c>
       <c r="G68" s="84">
-        <f>IF(Inputs!G9="Y", Prices!$C26, 0)</f>
+        <f>IF(Inputs!G10="Y", Prices!$C26, 0)</f>
         <v>0</v>
       </c>
       <c r="H68" s="84">
-        <f>IF(Inputs!H9="Y", Prices!$C26, 0)</f>
+        <f>IF(Inputs!H10="Y", Prices!$C26, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -13099,23 +13129,23 @@
         <v>15</v>
       </c>
       <c r="D72" s="18">
-        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D20 = "Y", D$11*Prices!$E21, 0)))*D$10</f>
+        <f>IF(Inputs!D$5="Y", 0, IF(D$11 = "", 0, IF(Inputs!D21 = "Y", D$11*Prices!$E21, 0)))*D$10</f>
         <v>0</v>
       </c>
       <c r="E72" s="18">
-        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E20 = "Y", E$11*Prices!$E21, 0)))*E$10</f>
+        <f>IF(Inputs!E$5="Y", 0, IF(E$11 = "", 0, IF(Inputs!E21 = "Y", E$11*Prices!$E21, 0)))*E$10</f>
         <v>0</v>
       </c>
       <c r="F72" s="18">
-        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F20 = "Y", F$11*Prices!$E21, 0)))*F$10</f>
+        <f>IF(Inputs!F$5="Y", 0, IF(F$11 = "", 0, IF(Inputs!F21 = "Y", F$11*Prices!$E21, 0)))*F$10</f>
         <v>0</v>
       </c>
       <c r="G72" s="18">
-        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G20 = "Y", G$11*Prices!$E21, 0)))*G$10</f>
+        <f>IF(Inputs!G$5="Y", 0, IF(G$11 = "", 0, IF(Inputs!G21 = "Y", G$11*Prices!$E21, 0)))*G$10</f>
         <v>0</v>
       </c>
       <c r="H72" s="18">
-        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H20 = "Y", H$11*Prices!$E21, 0)))*H$10</f>
+        <f>IF(Inputs!H$5="Y", 0, IF(H$11 = "", 0, IF(Inputs!H21 = "Y", H$11*Prices!$E21, 0)))*H$10</f>
         <v>0</v>
       </c>
       <c r="J72" s="90">
@@ -13148,23 +13178,23 @@
         <v>16</v>
       </c>
       <c r="D73" s="20">
-        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D21 = "Y", D$11*Prices!$E22, 0)))*D$10</f>
+        <f>IF(Inputs!D$5="Y", 0, IF(D$11 = "", 0, IF(Inputs!D22 = "Y", D$11*Prices!$E22, 0)))*D$10</f>
         <v>0</v>
       </c>
       <c r="E73" s="20">
-        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E21 = "Y", E$11*Prices!$E22, 0)))*E$10</f>
+        <f>IF(Inputs!E$5="Y", 0, IF(E$11 = "", 0, IF(Inputs!E22 = "Y", E$11*Prices!$E22, 0)))*E$10</f>
         <v>0</v>
       </c>
       <c r="F73" s="20">
-        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F21 = "Y", F$11*Prices!$E22, 0)))*F$10</f>
+        <f>IF(Inputs!F$5="Y", 0, IF(F$11 = "", 0, IF(Inputs!F22 = "Y", F$11*Prices!$E22, 0)))*F$10</f>
         <v>0</v>
       </c>
       <c r="G73" s="20">
-        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G21 = "Y", G$11*Prices!$E22, 0)))*G$10</f>
+        <f>IF(Inputs!G$5="Y", 0, IF(G$11 = "", 0, IF(Inputs!G22 = "Y", G$11*Prices!$E22, 0)))*G$10</f>
         <v>0</v>
       </c>
       <c r="H73" s="20">
-        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H21 = "Y", H$11*Prices!$E22, 0)))*H$10</f>
+        <f>IF(Inputs!H$5="Y", 0, IF(H$11 = "", 0, IF(Inputs!H22 = "Y", H$11*Prices!$E22, 0)))*H$10</f>
         <v>0</v>
       </c>
       <c r="J73" s="90">
@@ -13197,23 +13227,23 @@
         <v>17</v>
       </c>
       <c r="D74" s="20">
-        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D22 = "Y", D$11*Prices!$E23, 0)))*D$10</f>
+        <f>IF(Inputs!D$5="Y", 0, IF(D$11 = "", 0, IF(Inputs!D23 = "Y", D$11*Prices!$E23, 0)))*D$10</f>
         <v>0</v>
       </c>
       <c r="E74" s="20">
-        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E22 = "Y", E$11*Prices!$E23, 0)))*E$10</f>
+        <f>IF(Inputs!E$5="Y", 0, IF(E$11 = "", 0, IF(Inputs!E23 = "Y", E$11*Prices!$E23, 0)))*E$10</f>
         <v>0</v>
       </c>
       <c r="F74" s="20">
-        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F22 = "Y", F$11*Prices!$E23, 0)))*F$10</f>
+        <f>IF(Inputs!F$5="Y", 0, IF(F$11 = "", 0, IF(Inputs!F23 = "Y", F$11*Prices!$E23, 0)))*F$10</f>
         <v>0</v>
       </c>
       <c r="G74" s="20">
-        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G22 = "Y", G$11*Prices!$E23, 0)))*G$10</f>
+        <f>IF(Inputs!G$5="Y", 0, IF(G$11 = "", 0, IF(Inputs!G23 = "Y", G$11*Prices!$E23, 0)))*G$10</f>
         <v>0</v>
       </c>
       <c r="H74" s="20">
-        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H22 = "Y", H$11*Prices!$E23, 0)))*H$10</f>
+        <f>IF(Inputs!H$5="Y", 0, IF(H$11 = "", 0, IF(Inputs!H23 = "Y", H$11*Prices!$E23, 0)))*H$10</f>
         <v>0</v>
       </c>
       <c r="J74" s="90">
@@ -13246,23 +13276,23 @@
         <v>102</v>
       </c>
       <c r="D75" s="20">
-        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D23 = "Y", D$11*Prices!$E24 * IF(Inputs!D22="Y",1-Prices!$L$20,1), 0)))*D$10</f>
+        <f>IF(Inputs!D$5="Y", 0, IF(D$11 = "", 0, IF(Inputs!D24 = "Y", D$11*Prices!$E24 * IF(Inputs!D23="Y",1-Prices!$L$20,1), 0)))*D$10</f>
         <v>0</v>
       </c>
       <c r="E75" s="20">
-        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E23 = "Y", E$11*Prices!$E24 * IF(Inputs!E22="Y",1-Prices!$L$20,1), 0)))*E$10</f>
+        <f>IF(Inputs!E$5="Y", 0, IF(E$11 = "", 0, IF(Inputs!E24 = "Y", E$11*Prices!$E24 * IF(Inputs!E23="Y",1-Prices!$L$20,1), 0)))*E$10</f>
         <v>0</v>
       </c>
       <c r="F75" s="20">
-        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F23 = "Y", F$11*Prices!$E24 * IF(Inputs!F22="Y",1-Prices!$L$20,1), 0)))*F$10</f>
+        <f>IF(Inputs!F$5="Y", 0, IF(F$11 = "", 0, IF(Inputs!F24 = "Y", F$11*Prices!$E24 * IF(Inputs!F23="Y",1-Prices!$L$20,1), 0)))*F$10</f>
         <v>0</v>
       </c>
       <c r="G75" s="20">
-        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G23 = "Y", G$11*Prices!$E24 * IF(Inputs!G22="Y",1-Prices!$L$20,1), 0)))*G$10</f>
+        <f>IF(Inputs!G$5="Y", 0, IF(G$11 = "", 0, IF(Inputs!G24 = "Y", G$11*Prices!$E24 * IF(Inputs!G23="Y",1-Prices!$L$20,1), 0)))*G$10</f>
         <v>0</v>
       </c>
       <c r="H75" s="20">
-        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H23 = "Y", H$11*Prices!$E24 * IF(Inputs!H22="Y",1-Prices!$L$20,1), 0)))*H$10</f>
+        <f>IF(Inputs!H$5="Y", 0, IF(H$11 = "", 0, IF(Inputs!H24 = "Y", H$11*Prices!$E24 * IF(Inputs!H23="Y",1-Prices!$L$20,1), 0)))*H$10</f>
         <v>0</v>
       </c>
       <c r="J75" s="90">
@@ -13295,23 +13325,23 @@
         <v>101</v>
       </c>
       <c r="D76" s="20">
-        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D24 = "Y", D$11*Prices!$E25, 0)))*D$10</f>
+        <f>IF(Inputs!D$5="Y", 0, IF(D$11 = "", 0, IF(Inputs!D25 = "Y", D$11*Prices!$E25, 0)))*D$10</f>
         <v>0</v>
       </c>
       <c r="E76" s="20">
-        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E24 = "Y", E$11*Prices!$E25, 0)))*E$10</f>
+        <f>IF(Inputs!E$5="Y", 0, IF(E$11 = "", 0, IF(Inputs!E25 = "Y", E$11*Prices!$E25, 0)))*E$10</f>
         <v>0</v>
       </c>
       <c r="F76" s="20">
-        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F24 = "Y", F$11*Prices!$E25, 0)))*F$10</f>
+        <f>IF(Inputs!F$5="Y", 0, IF(F$11 = "", 0, IF(Inputs!F25 = "Y", F$11*Prices!$E25, 0)))*F$10</f>
         <v>0</v>
       </c>
       <c r="G76" s="20">
-        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G24 = "Y", G$11*Prices!$E25, 0)))*G$10</f>
+        <f>IF(Inputs!G$5="Y", 0, IF(G$11 = "", 0, IF(Inputs!G25 = "Y", G$11*Prices!$E25, 0)))*G$10</f>
         <v>0</v>
       </c>
       <c r="H76" s="20">
-        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H24 = "Y", H$11*Prices!$E25, 0)))*H$10</f>
+        <f>IF(Inputs!H$5="Y", 0, IF(H$11 = "", 0, IF(Inputs!H25 = "Y", H$11*Prices!$E25, 0)))*H$10</f>
         <v>0</v>
       </c>
       <c r="J76" s="90">
@@ -13344,23 +13374,23 @@
         <v>99</v>
       </c>
       <c r="D77" s="84">
-        <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D9 = "Y", D$11*Prices!$E26, 0)))*D$10</f>
+        <f>IF(Inputs!D$5="Y", 0, IF(D$11 = "", 0, IF(Inputs!D10 = "Y", D$11*Prices!$E26, 0)))*D$10</f>
         <v>0</v>
       </c>
       <c r="E77" s="84">
-        <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E9 = "Y", E$11*Prices!$E26, 0)))*E$10</f>
+        <f>IF(Inputs!E$5="Y", 0, IF(E$11 = "", 0, IF(Inputs!E10 = "Y", E$11*Prices!$E26, 0)))*E$10</f>
         <v>0</v>
       </c>
       <c r="F77" s="84">
-        <f>IF(Inputs!F$4="Y", 0, IF(F$11 = "", 0, IF(Inputs!F9 = "Y", F$11*Prices!$E26, 0)))*F$10</f>
+        <f>IF(Inputs!F$5="Y", 0, IF(F$11 = "", 0, IF(Inputs!F10 = "Y", F$11*Prices!$E26, 0)))*F$10</f>
         <v>0</v>
       </c>
       <c r="G77" s="84">
-        <f>IF(Inputs!G$4="Y", 0, IF(G$11 = "", 0, IF(Inputs!G9 = "Y", G$11*Prices!$E26, 0)))*G$10</f>
+        <f>IF(Inputs!G$5="Y", 0, IF(G$11 = "", 0, IF(Inputs!G10 = "Y", G$11*Prices!$E26, 0)))*G$10</f>
         <v>0</v>
       </c>
       <c r="H77" s="84">
-        <f>IF(Inputs!H$4="Y", 0, IF(H$11 = "", 0, IF(Inputs!H9 = "Y", H$11*Prices!$E26, 0)))*H$10</f>
+        <f>IF(Inputs!H$5="Y", 0, IF(H$11 = "", 0, IF(Inputs!H10 = "Y", H$11*Prices!$E26, 0)))*H$10</f>
         <v>0</v>
       </c>
       <c r="J77" s="90">
@@ -14100,7 +14130,7 @@
         <v>84</v>
       </c>
       <c r="D108" s="1">
-        <f>IF(Inputs!$D$5 = "Y", Prices!$L$18, 0)*-1</f>
+        <f>IF(Inputs!$D$6 = "Y", Prices!$L$18, 0)*-1</f>
         <v>0</v>
       </c>
       <c r="E108" s="1">
@@ -14293,8 +14323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14783,6 +14813,13 @@
         <f t="shared" si="2"/>
         <v>3.5999999999999997E-2</v>
       </c>
+      <c r="K23" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="L23" s="96">
+        <f>18000/15000</f>
+        <v>1.2</v>
+      </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="19" t="s">

</xml_diff>